<commit_message>
chore(#9915): replace deprecated appearance fields (#9924)
This refactor primarily replaces the `db-object`
appearance field with `select-contact`.
It also replaces two other deprecated appearance
fields namely `horizontal` and `horizontal-compact`.

This now follows the method mentioned by @jkuester mentioned in:
https://github.com/medic/cht-core/pull/9924#pullrequestreview-2800883826
The `.xlsx` files are updated to generate the
`.xml` forms using `cht-conf`'s `convert-contact/app-forms` actions.

Fixes #9915
</commit_message>
<xml_diff>
--- a/config/covid-19/forms/contact/PLACE_TYPE-edit.xlsx
+++ b/config/covid-19/forms/contact/PLACE_TYPE-edit.xlsx
@@ -1,15 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\apoorva\cht-core\config\covid-19\forms\contact\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70D695B6-AB35-47B1-96E1-624F89DB045D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="survey" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="choices" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="settings" sheetId="3" r:id="rId6"/>
+    <sheet name="survey" sheetId="1" r:id="rId1"/>
+    <sheet name="choices" sheetId="2" r:id="rId2"/>
+    <sheet name="settings" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mgrHtCLCFoW/Qhae0+WX+vEV6cAMQ=="/>
     </ext>
@@ -18,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="255">
   <si>
     <t>type</t>
   </si>
@@ -164,9 +182,6 @@
     <t>Seems redundant, but needed to access name from choice label</t>
   </si>
   <si>
-    <t>db:person</t>
-  </si>
-  <si>
     <t>_id</t>
   </si>
   <si>
@@ -188,9 +203,6 @@
     <t>Contact primaire</t>
   </si>
   <si>
-    <t>db-object</t>
-  </si>
-  <si>
     <t>Select the Primary Contact</t>
   </si>
   <si>
@@ -236,9 +248,6 @@
     <t>not(${_id}) or selected( . , 'true') or boolean(${_id})</t>
   </si>
   <si>
-    <t>horizontal-compact</t>
-  </si>
-  <si>
     <t>boolean(${_id})</t>
   </si>
   <si>
@@ -786,41 +795,47 @@
   </si>
   <si>
     <t>en</t>
+  </si>
+  <si>
+    <t>select-contact type-person</t>
+  </si>
+  <si>
+    <t>columns-pack</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
@@ -830,7 +845,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -888,109 +903,107 @@
     </fill>
   </fills>
   <borders count="2">
-    <border/>
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="43">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="8" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="9" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="7" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="10" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="10" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="5" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="6" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="7" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="6" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="7" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="4" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1180,53 +1193,55 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:AR1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2.0" ySplit="1.0" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="C1" sqref="C1" pane="topRight"/>
-      <selection activeCell="A2" sqref="A2" pane="bottomLeft"/>
-      <selection activeCell="C2" sqref="C2" pane="bottomRight"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="19.71"/>
-    <col customWidth="1" min="2" max="2" width="22.71"/>
-    <col customWidth="1" min="3" max="3" width="24.29"/>
-    <col customWidth="1" hidden="1" min="4" max="4" width="38.71"/>
-    <col customWidth="1" hidden="1" min="5" max="5" width="54.57"/>
-    <col customWidth="1" hidden="1" min="6" max="6" width="23.57"/>
-    <col customWidth="1" hidden="1" min="7" max="7" width="55.14"/>
-    <col customWidth="1" hidden="1" min="8" max="8" width="8.14"/>
-    <col customWidth="1" hidden="1" min="9" max="9" width="16.43"/>
-    <col customWidth="1" min="10" max="10" width="8.14"/>
-    <col customWidth="1" min="11" max="11" width="11.43"/>
-    <col customWidth="1" min="12" max="12" width="10.71"/>
-    <col customWidth="1" min="13" max="13" width="15.14"/>
-    <col customWidth="1" min="14" max="14" width="32.0"/>
-    <col customWidth="1" min="15" max="15" width="50.14"/>
-    <col customWidth="1" min="16" max="16" width="48.71"/>
-    <col customWidth="1" min="17" max="17" width="31.14"/>
-    <col customWidth="1" min="18" max="18" width="33.43"/>
-    <col customWidth="1" min="19" max="19" width="36.29"/>
-    <col customWidth="1" min="20" max="21" width="8.14"/>
-    <col customWidth="1" min="22" max="22" width="33.86"/>
-    <col customWidth="1" min="23" max="24" width="8.14"/>
-    <col customWidth="1" min="25" max="25" width="8.71"/>
-    <col customWidth="1" min="26" max="36" width="7.71"/>
-    <col customWidth="1" min="37" max="44" width="15.14"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" customWidth="1"/>
+    <col min="4" max="4" width="38.6640625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="54.5546875" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5546875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="55.109375" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="8.109375" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="8.109375" customWidth="1"/>
+    <col min="11" max="11" width="11.44140625" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" customWidth="1"/>
+    <col min="13" max="13" width="15.109375" customWidth="1"/>
+    <col min="14" max="14" width="32" customWidth="1"/>
+    <col min="15" max="15" width="50.109375" customWidth="1"/>
+    <col min="16" max="16" width="48.6640625" customWidth="1"/>
+    <col min="17" max="17" width="31.109375" customWidth="1"/>
+    <col min="18" max="18" width="33.44140625" customWidth="1"/>
+    <col min="19" max="19" width="36.33203125" customWidth="1"/>
+    <col min="20" max="21" width="8.109375" customWidth="1"/>
+    <col min="22" max="22" width="33.88671875" customWidth="1"/>
+    <col min="23" max="24" width="8.109375" customWidth="1"/>
+    <col min="25" max="25" width="8.6640625" customWidth="1"/>
+    <col min="26" max="36" width="7.6640625" customWidth="1"/>
+    <col min="37" max="44" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
+    <row r="1" spans="1:44" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1324,7 +1339,7 @@
       <c r="AQ1" s="8"/>
       <c r="AR1" s="8"/>
     </row>
-    <row r="2" ht="14.25" customHeight="1">
+    <row r="2" spans="1:44" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
         <v>26</v>
       </c>
@@ -1388,7 +1403,7 @@
       <c r="AQ2" s="10"/>
       <c r="AR2" s="10"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:44" ht="14.4">
       <c r="A3" s="9" t="s">
         <v>26</v>
       </c>
@@ -1450,7 +1465,7 @@
       <c r="AQ3" s="10"/>
       <c r="AR3" s="10"/>
     </row>
-    <row r="4" ht="14.25" customHeight="1">
+    <row r="4" spans="1:44" ht="14.25" customHeight="1">
       <c r="A4" s="9" t="s">
         <v>30</v>
       </c>
@@ -1514,7 +1529,7 @@
       <c r="AQ4" s="10"/>
       <c r="AR4" s="10"/>
     </row>
-    <row r="5" ht="14.25" customHeight="1">
+    <row r="5" spans="1:44" ht="14.25" customHeight="1">
       <c r="A5" s="9" t="s">
         <v>30</v>
       </c>
@@ -1578,7 +1593,7 @@
       <c r="AQ5" s="10"/>
       <c r="AR5" s="10"/>
     </row>
-    <row r="6" ht="14.25" customHeight="1">
+    <row r="6" spans="1:44" ht="14.25" customHeight="1">
       <c r="A6" s="9" t="s">
         <v>30</v>
       </c>
@@ -1642,7 +1657,7 @@
       <c r="AQ6" s="10"/>
       <c r="AR6" s="10"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:44" ht="14.4">
       <c r="A7" s="9" t="s">
         <v>36</v>
       </c>
@@ -1690,7 +1705,7 @@
       <c r="AQ7" s="10"/>
       <c r="AR7" s="10"/>
     </row>
-    <row r="8" ht="14.25" customHeight="1">
+    <row r="8" spans="1:44" ht="14.25" customHeight="1">
       <c r="A8" s="9" t="s">
         <v>36</v>
       </c>
@@ -1738,7 +1753,7 @@
       <c r="AQ8" s="10"/>
       <c r="AR8" s="10"/>
     </row>
-    <row r="9" ht="14.25" customHeight="1">
+    <row r="9" spans="1:44" ht="14.25" customHeight="1">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -1784,7 +1799,7 @@
       <c r="AQ9" s="8"/>
       <c r="AR9" s="8"/>
     </row>
-    <row r="10" ht="14.25" customHeight="1">
+    <row r="10" spans="1:44" ht="14.25" customHeight="1">
       <c r="A10" s="17" t="s">
         <v>26</v>
       </c>
@@ -1848,7 +1863,7 @@
       <c r="AQ10" s="16"/>
       <c r="AR10" s="16"/>
     </row>
-    <row r="11" ht="14.25" customHeight="1">
+    <row r="11" spans="1:44" ht="14.25" customHeight="1">
       <c r="A11" s="17" t="s">
         <v>39</v>
       </c>
@@ -1912,7 +1927,7 @@
       <c r="AQ11" s="16"/>
       <c r="AR11" s="16"/>
     </row>
-    <row r="12" ht="14.25" customHeight="1">
+    <row r="12" spans="1:44" ht="14.25" customHeight="1">
       <c r="A12" s="17" t="s">
         <v>39</v>
       </c>
@@ -1976,7 +1991,7 @@
       <c r="AQ12" s="16"/>
       <c r="AR12" s="16"/>
     </row>
-    <row r="13" ht="14.25" customHeight="1">
+    <row r="13" spans="1:44" ht="14.25" customHeight="1">
       <c r="A13" s="17" t="s">
         <v>26</v>
       </c>
@@ -2040,7 +2055,7 @@
       <c r="AQ13" s="16"/>
       <c r="AR13" s="16"/>
     </row>
-    <row r="14" ht="14.25" customHeight="1">
+    <row r="14" spans="1:44" ht="14.25" customHeight="1">
       <c r="A14" s="17" t="s">
         <v>30</v>
       </c>
@@ -2104,7 +2119,7 @@
       <c r="AQ14" s="16"/>
       <c r="AR14" s="16"/>
     </row>
-    <row r="15" ht="14.25" customHeight="1">
+    <row r="15" spans="1:44" ht="14.25" customHeight="1">
       <c r="A15" s="17" t="s">
         <v>44</v>
       </c>
@@ -2158,36 +2173,36 @@
       <c r="AQ15" s="16"/>
       <c r="AR15" s="16"/>
     </row>
-    <row r="16" ht="14.25" customHeight="1">
+    <row r="16" spans="1:44" ht="14.25" customHeight="1">
       <c r="A16" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="C16" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="D16" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="E16" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="F16" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="16" t="s">
+      <c r="G16" s="16" t="s">
         <v>53</v>
-      </c>
-      <c r="G16" s="16" t="s">
-        <v>54</v>
       </c>
       <c r="H16" s="16"/>
       <c r="I16" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J16" s="16"/>
       <c r="K16" s="16"/>
       <c r="L16" s="16" t="s">
-        <v>56</v>
+        <v>253</v>
       </c>
       <c r="M16" s="16"/>
       <c r="N16" s="16"/>
@@ -2195,23 +2210,23 @@
       <c r="P16" s="16"/>
       <c r="Q16" s="16"/>
       <c r="R16" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="S16" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="T16" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="S16" s="16" t="s">
+      <c r="U16" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="T16" s="16" t="s">
+      <c r="V16" s="16" t="s">
         <v>59</v>
-      </c>
-      <c r="U16" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="V16" s="16" t="s">
-        <v>61</v>
       </c>
       <c r="W16" s="16"/>
       <c r="X16" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="Y16" s="16"/>
       <c r="Z16" s="16"/>
@@ -2234,7 +2249,7 @@
       <c r="AQ16" s="16"/>
       <c r="AR16" s="16"/>
     </row>
-    <row r="17" ht="14.25" customHeight="1">
+    <row r="17" spans="1:44" ht="14.25" customHeight="1">
       <c r="A17" s="17" t="s">
         <v>36</v>
       </c>
@@ -2282,48 +2297,48 @@
       <c r="AQ17" s="16"/>
       <c r="AR17" s="16"/>
     </row>
-    <row r="18" ht="14.25" customHeight="1">
+    <row r="18" spans="1:44" ht="14.25" customHeight="1">
       <c r="A18" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="D18" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="E18" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="F18" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="G18" s="16" t="s">
         <v>67</v>
-      </c>
-      <c r="F18" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="G18" s="16" t="s">
-        <v>69</v>
       </c>
       <c r="H18" s="16"/>
       <c r="I18" s="16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J18" s="16" t="s">
         <v>41</v>
       </c>
       <c r="K18" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L18" s="16" t="s">
-        <v>72</v>
+        <v>254</v>
       </c>
       <c r="M18" s="18" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="N18" s="16"/>
       <c r="O18" s="16"/>
       <c r="P18" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="Q18" s="16"/>
       <c r="R18" s="16"/>
@@ -2335,7 +2350,7 @@
       <c r="X18" s="16"/>
       <c r="Y18" s="16"/>
       <c r="Z18" s="18" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="AA18" s="16"/>
       <c r="AB18" s="16"/>
@@ -2356,12 +2371,12 @@
       <c r="AQ18" s="16"/>
       <c r="AR18" s="16"/>
     </row>
-    <row r="19" ht="14.25" customHeight="1">
+    <row r="19" spans="1:44" ht="14.25" customHeight="1">
       <c r="A19" s="17" t="s">
         <v>44</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
@@ -2377,7 +2392,7 @@
       <c r="N19" s="16"/>
       <c r="O19" s="16"/>
       <c r="P19" s="16" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="Q19" s="16"/>
       <c r="R19" s="16"/>
@@ -2408,7 +2423,7 @@
       <c r="AQ19" s="16"/>
       <c r="AR19" s="16"/>
     </row>
-    <row r="20" ht="14.25" customHeight="1">
+    <row r="20" spans="1:44" ht="14.25" customHeight="1">
       <c r="A20" s="17" t="s">
         <v>30</v>
       </c>
@@ -2416,36 +2431,36 @@
         <v>1</v>
       </c>
       <c r="C20" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="F20" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="G20" s="16" t="s">
         <v>79</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="F20" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="G20" s="16" t="s">
-        <v>82</v>
       </c>
       <c r="H20" s="16"/>
       <c r="I20" s="16" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="J20" s="16" t="s">
         <v>41</v>
       </c>
       <c r="K20" s="16" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="L20" s="16"/>
       <c r="M20" s="16"/>
       <c r="N20" s="16"/>
       <c r="O20" s="16"/>
       <c r="P20" s="18" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="Q20" s="16"/>
       <c r="R20" s="16"/>
@@ -2476,31 +2491,31 @@
       <c r="AQ20" s="16"/>
       <c r="AR20" s="16"/>
     </row>
-    <row r="21" ht="14.25" customHeight="1">
+    <row r="21" spans="1:44" ht="14.25" customHeight="1">
       <c r="A21" s="17" t="s">
         <v>30</v>
       </c>
       <c r="B21" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="E21" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="F21" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="G21" s="16" t="s">
         <v>88</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="F21" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="G21" s="16" t="s">
-        <v>91</v>
       </c>
       <c r="H21" s="16"/>
       <c r="I21" s="16" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="J21" s="16"/>
       <c r="K21" s="16"/>
@@ -2538,15 +2553,15 @@
       <c r="AQ21" s="16"/>
       <c r="AR21" s="16"/>
     </row>
-    <row r="22" ht="14.25" customHeight="1">
+    <row r="22" spans="1:44" ht="14.25" customHeight="1">
       <c r="A22" s="19" t="s">
         <v>30</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D22" s="20"/>
       <c r="E22" s="20"/>
@@ -2590,7 +2605,7 @@
       <c r="AQ22" s="20"/>
       <c r="AR22" s="20"/>
     </row>
-    <row r="23" ht="14.25" customHeight="1">
+    <row r="23" spans="1:44" ht="14.25" customHeight="1">
       <c r="A23" s="17" t="s">
         <v>30</v>
       </c>
@@ -2598,28 +2613,28 @@
         <v>25</v>
       </c>
       <c r="C23" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="F23" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="D23" s="16" t="s">
+      <c r="G23" s="16" t="s">
         <v>96</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="F23" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="G23" s="16" t="s">
-        <v>99</v>
       </c>
       <c r="H23" s="16"/>
       <c r="I23" s="16" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="J23" s="16"/>
       <c r="K23" s="16"/>
       <c r="L23" s="16" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="M23" s="16"/>
       <c r="N23" s="16"/>
@@ -2654,12 +2669,12 @@
       <c r="AQ23" s="16"/>
       <c r="AR23" s="16"/>
     </row>
-    <row r="24" ht="14.25" customHeight="1">
+    <row r="24" spans="1:44" ht="14.25" customHeight="1">
       <c r="A24" s="17" t="s">
         <v>44</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
@@ -2675,7 +2690,7 @@
       <c r="N24" s="16"/>
       <c r="O24" s="16"/>
       <c r="P24" s="16" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="Q24" s="16"/>
       <c r="R24" s="16"/>
@@ -2706,12 +2721,12 @@
       <c r="AQ24" s="16"/>
       <c r="AR24" s="16"/>
     </row>
-    <row r="25" ht="14.25" customHeight="1">
+    <row r="25" spans="1:44" ht="14.25" customHeight="1">
       <c r="A25" s="17" t="s">
         <v>26</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C25" s="16" t="s">
         <v>28</v>
@@ -2770,12 +2785,12 @@
       <c r="AQ25" s="16"/>
       <c r="AR25" s="16"/>
     </row>
-    <row r="26" ht="14.25" customHeight="1">
+    <row r="26" spans="1:44" ht="14.25" customHeight="1">
       <c r="A26" s="17" t="s">
         <v>39</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C26" s="16" t="s">
         <v>28</v>
@@ -2815,7 +2830,7 @@
       <c r="X26" s="16"/>
       <c r="Y26" s="16"/>
       <c r="Z26" s="16" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="AA26" s="16"/>
       <c r="AB26" s="16"/>
@@ -2836,12 +2851,12 @@
       <c r="AQ26" s="16"/>
       <c r="AR26" s="16"/>
     </row>
-    <row r="27" ht="14.25" customHeight="1">
+    <row r="27" spans="1:44" ht="14.25" customHeight="1">
       <c r="A27" s="17" t="s">
         <v>39</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C27" s="16" t="s">
         <v>28</v>
@@ -2900,12 +2915,12 @@
       <c r="AQ27" s="16"/>
       <c r="AR27" s="16"/>
     </row>
-    <row r="28" ht="14.25" customHeight="1">
+    <row r="28" spans="1:44" ht="14.25" customHeight="1">
       <c r="A28" s="17" t="s">
         <v>39</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C28" s="16" t="s">
         <v>28</v>
@@ -2962,12 +2977,12 @@
       <c r="AQ28" s="16"/>
       <c r="AR28" s="16"/>
     </row>
-    <row r="29" ht="14.25" customHeight="1">
+    <row r="29" spans="1:44" ht="14.25" customHeight="1">
       <c r="A29" s="17" t="s">
         <v>44</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C29" s="16"/>
       <c r="D29" s="16"/>
@@ -2983,7 +2998,7 @@
       <c r="N29" s="16"/>
       <c r="O29" s="16"/>
       <c r="P29" s="16" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="Q29" s="16"/>
       <c r="R29" s="16"/>
@@ -2995,7 +3010,7 @@
       <c r="X29" s="16"/>
       <c r="Y29" s="16"/>
       <c r="Z29" s="16" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="AA29" s="16"/>
       <c r="AB29" s="16"/>
@@ -3016,12 +3031,12 @@
       <c r="AQ29" s="16"/>
       <c r="AR29" s="16"/>
     </row>
-    <row r="30" ht="14.25" customHeight="1">
+    <row r="30" spans="1:44" ht="14.25" customHeight="1">
       <c r="A30" s="17" t="s">
         <v>44</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C30" s="16"/>
       <c r="D30" s="16"/>
@@ -3037,7 +3052,7 @@
       <c r="N30" s="16"/>
       <c r="O30" s="16"/>
       <c r="P30" s="16" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="Q30" s="16"/>
       <c r="R30" s="16"/>
@@ -3068,12 +3083,12 @@
       <c r="AQ30" s="16"/>
       <c r="AR30" s="16"/>
     </row>
-    <row r="31" ht="14.25" customHeight="1">
+    <row r="31" spans="1:44" ht="14.25" customHeight="1">
       <c r="A31" s="17" t="s">
         <v>44</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C31" s="16"/>
       <c r="D31" s="16"/>
@@ -3089,7 +3104,7 @@
       <c r="N31" s="16"/>
       <c r="O31" s="16"/>
       <c r="P31" s="16" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="Q31" s="16"/>
       <c r="R31" s="16"/>
@@ -3120,7 +3135,7 @@
       <c r="AQ31" s="16"/>
       <c r="AR31" s="16"/>
     </row>
-    <row r="32" ht="14.25" customHeight="1">
+    <row r="32" spans="1:44" ht="14.25" customHeight="1">
       <c r="A32" s="17" t="s">
         <v>36</v>
       </c>
@@ -3168,7 +3183,7 @@
       <c r="AQ32" s="16"/>
       <c r="AR32" s="16"/>
     </row>
-    <row r="33" ht="14.25" customHeight="1">
+    <row r="33" spans="1:44" ht="14.25" customHeight="1">
       <c r="A33" s="17" t="s">
         <v>36</v>
       </c>
@@ -3216,7 +3231,7 @@
       <c r="AQ33" s="16"/>
       <c r="AR33" s="16"/>
     </row>
-    <row r="34" ht="14.25" customHeight="1">
+    <row r="34" spans="1:44" ht="14.25" customHeight="1">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
@@ -3262,12 +3277,12 @@
       <c r="AQ34" s="8"/>
       <c r="AR34" s="8"/>
     </row>
-    <row r="35" ht="14.25" customHeight="1">
+    <row r="35" spans="1:44" ht="14.25" customHeight="1">
       <c r="A35" s="17" t="s">
         <v>26</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C35" s="16" t="s">
         <v>28</v>
@@ -3291,7 +3306,7 @@
       <c r="J35" s="16"/>
       <c r="K35" s="16"/>
       <c r="L35" s="16" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="M35" s="16"/>
       <c r="N35" s="16"/>
@@ -3326,12 +3341,12 @@
       <c r="AQ35" s="16"/>
       <c r="AR35" s="16"/>
     </row>
-    <row r="36" ht="14.25" customHeight="1">
+    <row r="36" spans="1:44" ht="14.25" customHeight="1">
       <c r="A36" s="17" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C36" s="16" t="s">
         <v>28</v>
@@ -3361,7 +3376,7 @@
       <c r="N36" s="16"/>
       <c r="O36" s="16"/>
       <c r="P36" s="18" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="Q36" s="16"/>
       <c r="R36" s="16"/>
@@ -3392,12 +3407,12 @@
       <c r="AQ36" s="16"/>
       <c r="AR36" s="16"/>
     </row>
-    <row r="37" ht="13.5" customHeight="1">
+    <row r="37" spans="1:44" ht="13.5" customHeight="1">
       <c r="A37" s="17" t="s">
         <v>44</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C37" s="16"/>
       <c r="D37" s="16"/>
@@ -3413,7 +3428,7 @@
       <c r="N37" s="16"/>
       <c r="O37" s="16"/>
       <c r="P37" s="18" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="Q37" s="16"/>
       <c r="R37" s="16"/>
@@ -3444,12 +3459,12 @@
       <c r="AQ37" s="16"/>
       <c r="AR37" s="16"/>
     </row>
-    <row r="38" ht="14.25" customHeight="1">
+    <row r="38" spans="1:44" ht="14.25" customHeight="1">
       <c r="A38" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C38" s="16" t="s">
         <v>28</v>
@@ -3479,7 +3494,7 @@
       <c r="N38" s="16"/>
       <c r="O38" s="16"/>
       <c r="P38" s="18" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="Q38" s="16"/>
       <c r="R38" s="16"/>
@@ -3510,12 +3525,12 @@
       <c r="AQ38" s="16"/>
       <c r="AR38" s="16"/>
     </row>
-    <row r="39" ht="14.25" customHeight="1">
+    <row r="39" spans="1:44" ht="14.25" customHeight="1">
       <c r="A39" s="17" t="s">
         <v>44</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C39" s="16"/>
       <c r="D39" s="16"/>
@@ -3531,7 +3546,7 @@
       <c r="N39" s="16"/>
       <c r="O39" s="16"/>
       <c r="P39" s="18" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="Q39" s="16"/>
       <c r="R39" s="16"/>
@@ -3562,7 +3577,7 @@
       <c r="AQ39" s="16"/>
       <c r="AR39" s="16"/>
     </row>
-    <row r="40" ht="14.25" customHeight="1">
+    <row r="40" spans="1:44" ht="14.25" customHeight="1">
       <c r="A40" s="17" t="s">
         <v>36</v>
       </c>
@@ -3610,14 +3625,14 @@
       <c r="AQ40" s="16"/>
       <c r="AR40" s="16"/>
     </row>
-    <row r="41" ht="15.75" customHeight="1"/>
-    <row r="42" ht="15.75" customHeight="1"/>
-    <row r="43" ht="15.75" customHeight="1"/>
-    <row r="44" ht="15.75" customHeight="1"/>
-    <row r="45" ht="15.75" customHeight="1"/>
-    <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
-    <row r="48" ht="15.75" customHeight="1"/>
+    <row r="41" spans="1:44" ht="15.75" customHeight="1"/>
+    <row r="42" spans="1:44" ht="15.75" customHeight="1"/>
+    <row r="43" spans="1:44" ht="15.75" customHeight="1"/>
+    <row r="44" spans="1:44" ht="15.75" customHeight="1"/>
+    <row r="45" spans="1:44" ht="15.75" customHeight="1"/>
+    <row r="46" spans="1:44" ht="15.75" customHeight="1"/>
+    <row r="47" spans="1:44" ht="15.75" customHeight="1"/>
+    <row r="48" spans="1:44" ht="15.75" customHeight="1"/>
     <row r="49" ht="15.75" customHeight="1"/>
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1"/>
@@ -4572,46 +4587,44 @@
     <row r="1000" ht="15.75" customHeight="1"/>
     <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="21.14"/>
-    <col customWidth="1" min="2" max="2" width="9.71"/>
-    <col customWidth="1" min="3" max="3" width="26.71"/>
-    <col customWidth="1" min="4" max="4" width="46.0"/>
-    <col customWidth="1" min="5" max="5" width="51.57"/>
-    <col customWidth="1" min="6" max="6" width="49.14"/>
-    <col customWidth="1" min="7" max="7" width="35.0"/>
-    <col customWidth="1" min="8" max="8" width="7.71"/>
-    <col customWidth="1" min="9" max="9" width="17.57"/>
-    <col customWidth="1" min="10" max="13" width="7.71"/>
-    <col customWidth="1" min="14" max="26" width="15.14"/>
+    <col min="1" max="1" width="21.109375" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="46" customWidth="1"/>
+    <col min="5" max="5" width="51.5546875" customWidth="1"/>
+    <col min="6" max="6" width="49.109375" customWidth="1"/>
+    <col min="7" max="7" width="35" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" customWidth="1"/>
+    <col min="9" max="9" width="17.5546875" customWidth="1"/>
+    <col min="10" max="13" width="7.6640625" customWidth="1"/>
+    <col min="14" max="26" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
+    <row r="1" spans="1:26" ht="14.25" customHeight="1">
       <c r="A1" s="21" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D1" s="22" t="s">
         <v>3</v>
@@ -4649,31 +4662,31 @@
       <c r="Y1" s="28"/>
       <c r="Z1" s="28"/>
     </row>
-    <row r="2" ht="14.25" customHeight="1">
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" s="30" t="s">
         <v>128</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="E2" s="31" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="F2" s="32" t="s">
         <v>130</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="G2" s="33" t="s">
         <v>131</v>
-      </c>
-      <c r="E2" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="F2" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="G2" s="33" t="s">
-        <v>134</v>
       </c>
       <c r="H2" s="34"/>
       <c r="I2" s="35" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J2" s="28"/>
       <c r="K2" s="28"/>
@@ -4693,31 +4706,31 @@
       <c r="Y2" s="28"/>
       <c r="Z2" s="28"/>
     </row>
-    <row r="3" ht="14.25" customHeight="1">
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="29" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B3" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="E3" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="F3" s="32" t="s">
         <v>137</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="G3" s="33" t="s">
         <v>138</v>
-      </c>
-      <c r="E3" s="31" t="s">
-        <v>139</v>
-      </c>
-      <c r="F3" s="32" t="s">
-        <v>140</v>
-      </c>
-      <c r="G3" s="33" t="s">
-        <v>141</v>
       </c>
       <c r="H3" s="34"/>
       <c r="I3" s="35" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="J3" s="28"/>
       <c r="K3" s="28"/>
@@ -4737,31 +4750,31 @@
       <c r="Y3" s="28"/>
       <c r="Z3" s="28"/>
     </row>
-    <row r="4" ht="14.25" customHeight="1">
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="29" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" s="37" t="s">
+        <v>141</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>142</v>
+      </c>
+      <c r="E4" s="39" t="s">
         <v>143</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="F4" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="G4" s="33" t="s">
         <v>145</v>
-      </c>
-      <c r="E4" s="39" t="s">
-        <v>146</v>
-      </c>
-      <c r="F4" s="32" t="s">
-        <v>147</v>
-      </c>
-      <c r="G4" s="33" t="s">
-        <v>148</v>
       </c>
       <c r="H4" s="34"/>
       <c r="I4" s="35" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J4" s="28"/>
       <c r="K4" s="28"/>
@@ -4781,31 +4794,31 @@
       <c r="Y4" s="28"/>
       <c r="Z4" s="28"/>
     </row>
-    <row r="5" ht="14.25" customHeight="1">
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" s="29" t="s">
         <v>42</v>
       </c>
       <c r="B5" s="36" t="s">
+        <v>147</v>
+      </c>
+      <c r="C5" s="37" t="s">
+        <v>148</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="E5" s="39" t="s">
         <v>150</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="F5" s="32" t="s">
         <v>151</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="G5" s="33" t="s">
         <v>152</v>
-      </c>
-      <c r="E5" s="39" t="s">
-        <v>153</v>
-      </c>
-      <c r="F5" s="32" t="s">
-        <v>154</v>
-      </c>
-      <c r="G5" s="33" t="s">
-        <v>155</v>
       </c>
       <c r="H5" s="34"/>
       <c r="I5" s="35" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="J5" s="28"/>
       <c r="K5" s="28"/>
@@ -4825,31 +4838,31 @@
       <c r="Y5" s="28"/>
       <c r="Z5" s="28"/>
     </row>
-    <row r="6" ht="14.25" customHeight="1">
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="B6" s="36" t="s">
+        <v>155</v>
+      </c>
+      <c r="C6" s="37" t="s">
+        <v>156</v>
+      </c>
+      <c r="D6" s="30" t="s">
         <v>157</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="E6" s="39" t="s">
         <v>158</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="F6" s="32" t="s">
         <v>159</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="G6" s="33" t="s">
         <v>160</v>
-      </c>
-      <c r="E6" s="39" t="s">
-        <v>161</v>
-      </c>
-      <c r="F6" s="32" t="s">
-        <v>162</v>
-      </c>
-      <c r="G6" s="33" t="s">
-        <v>163</v>
       </c>
       <c r="H6" s="34"/>
       <c r="I6" s="35" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J6" s="28"/>
       <c r="K6" s="28"/>
@@ -4869,31 +4882,31 @@
       <c r="Y6" s="28"/>
       <c r="Z6" s="28"/>
     </row>
-    <row r="7" ht="14.25" customHeight="1">
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="28" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B7" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>163</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>164</v>
+      </c>
+      <c r="E7" s="39" t="s">
         <v>165</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="F7" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="G7" s="33" t="s">
         <v>167</v>
-      </c>
-      <c r="E7" s="39" t="s">
-        <v>168</v>
-      </c>
-      <c r="F7" s="32" t="s">
-        <v>169</v>
-      </c>
-      <c r="G7" s="33" t="s">
-        <v>170</v>
       </c>
       <c r="H7" s="34"/>
       <c r="I7" s="35" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="J7" s="28"/>
       <c r="K7" s="28"/>
@@ -4913,31 +4926,31 @@
       <c r="Y7" s="28"/>
       <c r="Z7" s="28"/>
     </row>
-    <row r="8" ht="14.25" customHeight="1">
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="28" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B8" s="28" t="s">
+        <v>169</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>170</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="E8" s="39" t="s">
         <v>172</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="F8" s="32" t="s">
         <v>173</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="G8" s="33" t="s">
         <v>174</v>
-      </c>
-      <c r="E8" s="39" t="s">
-        <v>175</v>
-      </c>
-      <c r="F8" s="32" t="s">
-        <v>176</v>
-      </c>
-      <c r="G8" s="33" t="s">
-        <v>177</v>
       </c>
       <c r="H8" s="34"/>
       <c r="I8" s="35" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J8" s="28"/>
       <c r="K8" s="28"/>
@@ -4957,31 +4970,31 @@
       <c r="Y8" s="28"/>
       <c r="Z8" s="28"/>
     </row>
-    <row r="9" ht="14.25" customHeight="1">
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="28" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B9" s="36" t="s">
+        <v>175</v>
+      </c>
+      <c r="C9" s="37" t="s">
+        <v>176</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>177</v>
+      </c>
+      <c r="E9" s="39" t="s">
         <v>178</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="F9" s="32" t="s">
         <v>179</v>
       </c>
-      <c r="D9" s="30" t="s">
-        <v>180</v>
-      </c>
-      <c r="E9" s="39" t="s">
-        <v>181</v>
-      </c>
-      <c r="F9" s="32" t="s">
-        <v>182</v>
-      </c>
       <c r="G9" s="33" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H9" s="34"/>
       <c r="I9" s="35" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="J9" s="28"/>
       <c r="K9" s="28"/>
@@ -5001,31 +5014,31 @@
       <c r="Y9" s="28"/>
       <c r="Z9" s="28"/>
     </row>
-    <row r="10" ht="14.25" customHeight="1">
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>182</v>
+      </c>
+      <c r="C10" s="37" t="s">
+        <v>183</v>
+      </c>
+      <c r="D10" s="30" t="s">
         <v>184</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="E10" s="39" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="F10" s="40" t="s">
         <v>186</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="G10" s="33" t="s">
         <v>187</v>
-      </c>
-      <c r="E10" s="39" t="s">
-        <v>188</v>
-      </c>
-      <c r="F10" s="40" t="s">
-        <v>189</v>
-      </c>
-      <c r="G10" s="33" t="s">
-        <v>190</v>
       </c>
       <c r="H10" s="34"/>
       <c r="I10" s="35" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="J10" s="28"/>
       <c r="K10" s="28"/>
@@ -5045,31 +5058,31 @@
       <c r="Y10" s="28"/>
       <c r="Z10" s="28"/>
     </row>
-    <row r="11" ht="14.25" customHeight="1">
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="28" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B11" s="36" t="s">
+        <v>189</v>
+      </c>
+      <c r="C11" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="E11" s="39" t="s">
         <v>192</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="F11" s="40" t="s">
         <v>193</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="G11" s="33" t="s">
         <v>194</v>
-      </c>
-      <c r="E11" s="39" t="s">
-        <v>195</v>
-      </c>
-      <c r="F11" s="40" t="s">
-        <v>196</v>
-      </c>
-      <c r="G11" s="33" t="s">
-        <v>197</v>
       </c>
       <c r="H11" s="34"/>
       <c r="I11" s="35" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="J11" s="28"/>
       <c r="K11" s="28"/>
@@ -5089,31 +5102,31 @@
       <c r="Y11" s="28"/>
       <c r="Z11" s="28"/>
     </row>
-    <row r="12" ht="14.25" customHeight="1">
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="29" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B12" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="E12" s="39" t="s">
         <v>129</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="F12" s="32" t="s">
         <v>130</v>
       </c>
-      <c r="D12" s="30" t="s">
-        <v>131</v>
-      </c>
-      <c r="E12" s="39" t="s">
-        <v>132</v>
-      </c>
-      <c r="F12" s="32" t="s">
-        <v>133</v>
-      </c>
       <c r="G12" s="33" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="H12" s="34"/>
       <c r="I12" s="35" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J12" s="28"/>
       <c r="K12" s="28"/>
@@ -5133,31 +5146,31 @@
       <c r="Y12" s="28"/>
       <c r="Z12" s="28"/>
     </row>
-    <row r="13" ht="14.25" customHeight="1">
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="29" t="s">
+        <v>196</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="D13" s="30" t="s">
         <v>199</v>
       </c>
-      <c r="B13" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="C13" s="29" t="s">
+      <c r="E13" s="39" t="s">
+        <v>200</v>
+      </c>
+      <c r="F13" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="D13" s="30" t="s">
+      <c r="G13" s="33" t="s">
         <v>202</v>
-      </c>
-      <c r="E13" s="39" t="s">
-        <v>203</v>
-      </c>
-      <c r="F13" s="32" t="s">
-        <v>204</v>
-      </c>
-      <c r="G13" s="33" t="s">
-        <v>205</v>
       </c>
       <c r="H13" s="34"/>
       <c r="I13" s="35" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="K13" s="28"/>
       <c r="L13" s="28"/>
@@ -5176,31 +5189,31 @@
       <c r="Y13" s="28"/>
       <c r="Z13" s="28"/>
     </row>
-    <row r="14" ht="14.25" customHeight="1">
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="28" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B14" s="36" t="s">
+        <v>204</v>
+      </c>
+      <c r="C14" s="37" t="s">
+        <v>205</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>206</v>
+      </c>
+      <c r="E14" s="39" t="s">
         <v>207</v>
       </c>
-      <c r="C14" s="37" t="s">
+      <c r="F14" s="32" t="s">
         <v>208</v>
       </c>
-      <c r="D14" s="30" t="s">
+      <c r="G14" s="33" t="s">
         <v>209</v>
-      </c>
-      <c r="E14" s="39" t="s">
-        <v>210</v>
-      </c>
-      <c r="F14" s="32" t="s">
-        <v>211</v>
-      </c>
-      <c r="G14" s="33" t="s">
-        <v>212</v>
       </c>
       <c r="H14" s="34"/>
       <c r="I14" s="35" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="J14" s="28"/>
       <c r="K14" s="28"/>
@@ -5220,31 +5233,31 @@
       <c r="Y14" s="28"/>
       <c r="Z14" s="28"/>
     </row>
-    <row r="15" ht="14.25" customHeight="1">
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="28" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B15" s="36" t="s">
+        <v>211</v>
+      </c>
+      <c r="C15" s="37" t="s">
+        <v>212</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>213</v>
+      </c>
+      <c r="E15" s="39" t="s">
         <v>214</v>
       </c>
-      <c r="C15" s="37" t="s">
+      <c r="F15" s="32" t="s">
         <v>215</v>
       </c>
-      <c r="D15" s="30" t="s">
+      <c r="G15" s="33" t="s">
         <v>216</v>
-      </c>
-      <c r="E15" s="39" t="s">
-        <v>217</v>
-      </c>
-      <c r="F15" s="32" t="s">
-        <v>218</v>
-      </c>
-      <c r="G15" s="33" t="s">
-        <v>219</v>
       </c>
       <c r="H15" s="34"/>
       <c r="I15" s="35" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="J15" s="28"/>
       <c r="K15" s="28"/>
@@ -5264,31 +5277,31 @@
       <c r="Y15" s="28"/>
       <c r="Z15" s="28"/>
     </row>
-    <row r="16" ht="14.25" customHeight="1">
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="28" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B16" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="C16" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>220</v>
+      </c>
+      <c r="E16" s="39" t="s">
         <v>221</v>
       </c>
-      <c r="C16" s="37" t="s">
+      <c r="F16" s="32" t="s">
         <v>222</v>
       </c>
-      <c r="D16" s="30" t="s">
-        <v>223</v>
-      </c>
-      <c r="E16" s="39" t="s">
-        <v>224</v>
-      </c>
-      <c r="F16" s="32" t="s">
-        <v>225</v>
-      </c>
       <c r="G16" s="33" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="H16" s="34"/>
       <c r="I16" s="35" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="J16" s="28"/>
       <c r="K16" s="28"/>
@@ -5308,31 +5321,31 @@
       <c r="Y16" s="28"/>
       <c r="Z16" s="28"/>
     </row>
-    <row r="17" ht="14.25" customHeight="1">
+    <row r="17" spans="1:26" ht="14.25" customHeight="1">
       <c r="A17" s="28" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B17" s="36" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C17" s="37" t="s">
+        <v>224</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>225</v>
+      </c>
+      <c r="E17" s="39" t="s">
+        <v>226</v>
+      </c>
+      <c r="F17" s="32" t="s">
         <v>227</v>
       </c>
-      <c r="D17" s="30" t="s">
+      <c r="G17" s="33" t="s">
         <v>228</v>
-      </c>
-      <c r="E17" s="39" t="s">
-        <v>229</v>
-      </c>
-      <c r="F17" s="32" t="s">
-        <v>230</v>
-      </c>
-      <c r="G17" s="33" t="s">
-        <v>231</v>
       </c>
       <c r="H17" s="34"/>
       <c r="I17" s="35" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
@@ -5352,31 +5365,31 @@
       <c r="Y17" s="8"/>
       <c r="Z17" s="8"/>
     </row>
-    <row r="18" ht="14.25" customHeight="1">
+    <row r="18" spans="1:26" ht="14.25" customHeight="1">
       <c r="A18" s="28" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B18" s="36" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C18" s="37" t="s">
+        <v>230</v>
+      </c>
+      <c r="D18" s="30" t="s">
+        <v>231</v>
+      </c>
+      <c r="E18" s="39" t="s">
+        <v>232</v>
+      </c>
+      <c r="F18" s="32" t="s">
         <v>233</v>
       </c>
-      <c r="D18" s="30" t="s">
+      <c r="G18" s="33" t="s">
         <v>234</v>
-      </c>
-      <c r="E18" s="39" t="s">
-        <v>235</v>
-      </c>
-      <c r="F18" s="32" t="s">
-        <v>236</v>
-      </c>
-      <c r="G18" s="33" t="s">
-        <v>237</v>
       </c>
       <c r="H18" s="34"/>
       <c r="I18" s="35" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
@@ -5396,31 +5409,31 @@
       <c r="Y18" s="8"/>
       <c r="Z18" s="8"/>
     </row>
-    <row r="19" ht="14.25" customHeight="1">
+    <row r="19" spans="1:26" ht="14.25" customHeight="1">
       <c r="A19" s="28" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B19" s="36" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C19" s="37" t="s">
+        <v>236</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>237</v>
+      </c>
+      <c r="E19" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="F19" s="32" t="s">
         <v>239</v>
       </c>
-      <c r="D19" s="30" t="s">
+      <c r="G19" s="33" t="s">
         <v>240</v>
-      </c>
-      <c r="E19" s="39" t="s">
-        <v>241</v>
-      </c>
-      <c r="F19" s="32" t="s">
-        <v>242</v>
-      </c>
-      <c r="G19" s="33" t="s">
-        <v>243</v>
       </c>
       <c r="H19" s="34"/>
       <c r="I19" s="35" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
@@ -5440,19 +5453,19 @@
       <c r="Y19" s="8"/>
       <c r="Z19" s="8"/>
     </row>
-    <row r="20" ht="15.75" customHeight="1"/>
-    <row r="21" ht="15.75" customHeight="1"/>
-    <row r="22" ht="15.75" customHeight="1"/>
-    <row r="23" ht="15.75" customHeight="1"/>
-    <row r="24" ht="15.75" customHeight="1"/>
-    <row r="25" ht="15.75" customHeight="1"/>
-    <row r="26" ht="15.75" customHeight="1"/>
-    <row r="27" ht="15.75" customHeight="1"/>
-    <row r="28" ht="15.75" customHeight="1"/>
-    <row r="29" ht="15.75" customHeight="1"/>
-    <row r="30" ht="15.75" customHeight="1"/>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
+    <row r="20" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="21" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="22" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="23" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="24" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="25" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="26" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="27" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="28" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="29" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="30" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="31" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="32" spans="1:26" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -6420,55 +6433,53 @@
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="28.14"/>
-    <col customWidth="1" min="2" max="2" width="12.71"/>
-    <col customWidth="1" min="3" max="3" width="20.14"/>
-    <col customWidth="1" min="4" max="4" width="5.71"/>
-    <col customWidth="1" min="5" max="5" width="14.29"/>
-    <col customWidth="1" min="6" max="6" width="34.0"/>
-    <col customWidth="1" min="7" max="16" width="7.71"/>
-    <col customWidth="1" min="17" max="26" width="15.14"/>
+    <col min="1" max="1" width="28.109375" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" customWidth="1"/>
+    <col min="4" max="4" width="5.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="34" customWidth="1"/>
+    <col min="7" max="16" width="7.6640625" customWidth="1"/>
+    <col min="17" max="26" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
+    <row r="1" spans="1:26" ht="14.25" customHeight="1">
       <c r="A1" s="41" t="s">
+        <v>242</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>243</v>
+      </c>
+      <c r="C1" s="41" t="s">
+        <v>244</v>
+      </c>
+      <c r="D1" s="41" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="E1" s="41" t="s">
         <v>246</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="F1" s="41" t="s">
         <v>247</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="G1" s="41" t="s">
         <v>248</v>
-      </c>
-      <c r="E1" s="41" t="s">
-        <v>249</v>
-      </c>
-      <c r="F1" s="41" t="s">
-        <v>250</v>
-      </c>
-      <c r="G1" s="41" t="s">
-        <v>251</v>
       </c>
       <c r="H1" s="28"/>
       <c r="I1" s="28"/>
@@ -6490,24 +6501,24 @@
       <c r="Y1" s="28"/>
       <c r="Z1" s="28"/>
     </row>
-    <row r="2" ht="14.25" customHeight="1">
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="28" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C2" s="42" t="str">
-        <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2021-08-18_00-07</v>
+        <f ca="1">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
+        <v>2025-05-01 23-04</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F2" s="28"/>
       <c r="G2" s="28" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="H2" s="28"/>
       <c r="I2" s="28"/>
@@ -6529,7 +6540,7 @@
       <c r="Y2" s="28"/>
       <c r="Z2" s="28"/>
     </row>
-    <row r="3" ht="14.25" customHeight="1">
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="28"/>
       <c r="B3" s="28"/>
       <c r="C3" s="28"/>
@@ -6557,7 +6568,7 @@
       <c r="Y3" s="28"/>
       <c r="Z3" s="28"/>
     </row>
-    <row r="4" ht="14.25" customHeight="1">
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="28"/>
       <c r="B4" s="28"/>
       <c r="C4" s="28"/>
@@ -6585,7 +6596,7 @@
       <c r="Y4" s="28"/>
       <c r="Z4" s="28"/>
     </row>
-    <row r="5" ht="14.25" customHeight="1">
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" s="28"/>
       <c r="B5" s="28"/>
       <c r="C5" s="28"/>
@@ -6613,7 +6624,7 @@
       <c r="Y5" s="28"/>
       <c r="Z5" s="28"/>
     </row>
-    <row r="6" ht="14.25" customHeight="1">
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="28"/>
       <c r="B6" s="28"/>
       <c r="C6" s="28"/>
@@ -6641,7 +6652,7 @@
       <c r="Y6" s="28"/>
       <c r="Z6" s="28"/>
     </row>
-    <row r="7" ht="14.25" customHeight="1">
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="28"/>
       <c r="B7" s="28"/>
       <c r="C7" s="28"/>
@@ -6669,7 +6680,7 @@
       <c r="Y7" s="28"/>
       <c r="Z7" s="28"/>
     </row>
-    <row r="8" ht="14.25" customHeight="1">
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="28"/>
       <c r="B8" s="28"/>
       <c r="C8" s="28"/>
@@ -6697,7 +6708,7 @@
       <c r="Y8" s="28"/>
       <c r="Z8" s="28"/>
     </row>
-    <row r="9" ht="14.25" customHeight="1">
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="28"/>
       <c r="B9" s="28"/>
       <c r="C9" s="28"/>
@@ -6725,7 +6736,7 @@
       <c r="Y9" s="28"/>
       <c r="Z9" s="28"/>
     </row>
-    <row r="10" ht="14.25" customHeight="1">
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="28"/>
       <c r="B10" s="28"/>
       <c r="C10" s="28"/>
@@ -6753,7 +6764,7 @@
       <c r="Y10" s="28"/>
       <c r="Z10" s="28"/>
     </row>
-    <row r="11" ht="14.25" customHeight="1">
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="28"/>
       <c r="B11" s="28"/>
       <c r="C11" s="28"/>
@@ -6781,7 +6792,7 @@
       <c r="Y11" s="28"/>
       <c r="Z11" s="28"/>
     </row>
-    <row r="12" ht="14.25" customHeight="1">
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="28"/>
       <c r="B12" s="28"/>
       <c r="C12" s="28"/>
@@ -6809,7 +6820,7 @@
       <c r="Y12" s="28"/>
       <c r="Z12" s="28"/>
     </row>
-    <row r="13" ht="14.25" customHeight="1">
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="28"/>
       <c r="B13" s="28"/>
       <c r="C13" s="28"/>
@@ -6837,7 +6848,7 @@
       <c r="Y13" s="28"/>
       <c r="Z13" s="28"/>
     </row>
-    <row r="14" ht="14.25" customHeight="1">
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="28"/>
       <c r="B14" s="28"/>
       <c r="C14" s="28"/>
@@ -6865,7 +6876,7 @@
       <c r="Y14" s="28"/>
       <c r="Z14" s="28"/>
     </row>
-    <row r="15" ht="14.25" customHeight="1">
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="28"/>
       <c r="B15" s="28"/>
       <c r="C15" s="28"/>
@@ -6893,7 +6904,7 @@
       <c r="Y15" s="28"/>
       <c r="Z15" s="28"/>
     </row>
-    <row r="16" ht="14.25" customHeight="1">
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="28"/>
       <c r="B16" s="28"/>
       <c r="C16" s="28"/>
@@ -6921,7 +6932,7 @@
       <c r="Y16" s="28"/>
       <c r="Z16" s="28"/>
     </row>
-    <row r="17" ht="14.25" customHeight="1">
+    <row r="17" spans="1:26" ht="14.25" customHeight="1">
       <c r="A17" s="28"/>
       <c r="B17" s="28"/>
       <c r="C17" s="28"/>
@@ -6949,7 +6960,7 @@
       <c r="Y17" s="28"/>
       <c r="Z17" s="28"/>
     </row>
-    <row r="18" ht="14.25" customHeight="1">
+    <row r="18" spans="1:26" ht="14.25" customHeight="1">
       <c r="A18" s="28"/>
       <c r="B18" s="28"/>
       <c r="C18" s="28"/>
@@ -6977,7 +6988,7 @@
       <c r="Y18" s="28"/>
       <c r="Z18" s="28"/>
     </row>
-    <row r="19" ht="14.25" customHeight="1">
+    <row r="19" spans="1:26" ht="14.25" customHeight="1">
       <c r="A19" s="28"/>
       <c r="B19" s="28"/>
       <c r="C19" s="28"/>
@@ -7005,7 +7016,7 @@
       <c r="Y19" s="28"/>
       <c r="Z19" s="28"/>
     </row>
-    <row r="20" ht="14.25" customHeight="1">
+    <row r="20" spans="1:26" ht="14.25" customHeight="1">
       <c r="A20" s="28"/>
       <c r="B20" s="28"/>
       <c r="C20" s="28"/>
@@ -7033,7 +7044,7 @@
       <c r="Y20" s="28"/>
       <c r="Z20" s="28"/>
     </row>
-    <row r="21" ht="14.25" customHeight="1">
+    <row r="21" spans="1:26" ht="14.25" customHeight="1">
       <c r="A21" s="28"/>
       <c r="B21" s="28"/>
       <c r="C21" s="28"/>
@@ -7061,7 +7072,7 @@
       <c r="Y21" s="28"/>
       <c r="Z21" s="28"/>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
+    <row r="22" spans="1:26" ht="15.75" customHeight="1">
       <c r="A22" s="28"/>
       <c r="B22" s="28"/>
       <c r="C22" s="28"/>
@@ -7089,7 +7100,7 @@
       <c r="Y22" s="28"/>
       <c r="Z22" s="28"/>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
+    <row r="23" spans="1:26" ht="15.75" customHeight="1">
       <c r="A23" s="28"/>
       <c r="B23" s="28"/>
       <c r="C23" s="28"/>
@@ -7117,7 +7128,7 @@
       <c r="Y23" s="28"/>
       <c r="Z23" s="28"/>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
+    <row r="24" spans="1:26" ht="15.75" customHeight="1">
       <c r="A24" s="28"/>
       <c r="B24" s="28"/>
       <c r="C24" s="28"/>
@@ -7145,7 +7156,7 @@
       <c r="Y24" s="28"/>
       <c r="Z24" s="28"/>
     </row>
-    <row r="25" ht="15.75" customHeight="1">
+    <row r="25" spans="1:26" ht="15.75" customHeight="1">
       <c r="A25" s="28"/>
       <c r="B25" s="28"/>
       <c r="C25" s="28"/>
@@ -7173,7 +7184,7 @@
       <c r="Y25" s="28"/>
       <c r="Z25" s="28"/>
     </row>
-    <row r="26" ht="15.75" customHeight="1">
+    <row r="26" spans="1:26" ht="15.75" customHeight="1">
       <c r="A26" s="28"/>
       <c r="B26" s="28"/>
       <c r="C26" s="28"/>
@@ -7201,7 +7212,7 @@
       <c r="Y26" s="28"/>
       <c r="Z26" s="28"/>
     </row>
-    <row r="27" ht="15.75" customHeight="1">
+    <row r="27" spans="1:26" ht="15.75" customHeight="1">
       <c r="A27" s="28"/>
       <c r="B27" s="28"/>
       <c r="C27" s="28"/>
@@ -7229,7 +7240,7 @@
       <c r="Y27" s="28"/>
       <c r="Z27" s="28"/>
     </row>
-    <row r="28" ht="15.75" customHeight="1">
+    <row r="28" spans="1:26" ht="15.75" customHeight="1">
       <c r="A28" s="28"/>
       <c r="B28" s="28"/>
       <c r="C28" s="28"/>
@@ -7257,7 +7268,7 @@
       <c r="Y28" s="28"/>
       <c r="Z28" s="28"/>
     </row>
-    <row r="29" ht="15.75" customHeight="1">
+    <row r="29" spans="1:26" ht="15.75" customHeight="1">
       <c r="A29" s="28"/>
       <c r="B29" s="28"/>
       <c r="C29" s="28"/>
@@ -7285,7 +7296,7 @@
       <c r="Y29" s="28"/>
       <c r="Z29" s="28"/>
     </row>
-    <row r="30" ht="15.75" customHeight="1">
+    <row r="30" spans="1:26" ht="15.75" customHeight="1">
       <c r="A30" s="28"/>
       <c r="B30" s="28"/>
       <c r="C30" s="28"/>
@@ -7313,7 +7324,7 @@
       <c r="Y30" s="28"/>
       <c r="Z30" s="28"/>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
+    <row r="31" spans="1:26" ht="15.75" customHeight="1">
       <c r="A31" s="28"/>
       <c r="B31" s="28"/>
       <c r="C31" s="28"/>
@@ -7341,7 +7352,7 @@
       <c r="Y31" s="28"/>
       <c r="Z31" s="28"/>
     </row>
-    <row r="32" ht="15.75" customHeight="1">
+    <row r="32" spans="1:26" ht="15.75" customHeight="1">
       <c r="A32" s="28"/>
       <c r="B32" s="28"/>
       <c r="C32" s="28"/>
@@ -7369,7 +7380,7 @@
       <c r="Y32" s="28"/>
       <c r="Z32" s="28"/>
     </row>
-    <row r="33" ht="15.75" customHeight="1">
+    <row r="33" spans="1:26" ht="15.75" customHeight="1">
       <c r="A33" s="28"/>
       <c r="B33" s="28"/>
       <c r="C33" s="28"/>
@@ -7397,7 +7408,7 @@
       <c r="Y33" s="28"/>
       <c r="Z33" s="28"/>
     </row>
-    <row r="34" ht="15.75" customHeight="1">
+    <row r="34" spans="1:26" ht="15.75" customHeight="1">
       <c r="A34" s="28"/>
       <c r="B34" s="28"/>
       <c r="C34" s="28"/>
@@ -7425,7 +7436,7 @@
       <c r="Y34" s="28"/>
       <c r="Z34" s="28"/>
     </row>
-    <row r="35" ht="15.75" customHeight="1">
+    <row r="35" spans="1:26" ht="15.75" customHeight="1">
       <c r="A35" s="28"/>
       <c r="B35" s="28"/>
       <c r="C35" s="28"/>
@@ -7453,7 +7464,7 @@
       <c r="Y35" s="28"/>
       <c r="Z35" s="28"/>
     </row>
-    <row r="36" ht="15.75" customHeight="1">
+    <row r="36" spans="1:26" ht="15.75" customHeight="1">
       <c r="A36" s="28"/>
       <c r="B36" s="28"/>
       <c r="C36" s="28"/>
@@ -7481,7 +7492,7 @@
       <c r="Y36" s="28"/>
       <c r="Z36" s="28"/>
     </row>
-    <row r="37" ht="15.75" customHeight="1">
+    <row r="37" spans="1:26" ht="15.75" customHeight="1">
       <c r="A37" s="28"/>
       <c r="B37" s="28"/>
       <c r="C37" s="28"/>
@@ -7509,7 +7520,7 @@
       <c r="Y37" s="28"/>
       <c r="Z37" s="28"/>
     </row>
-    <row r="38" ht="15.75" customHeight="1">
+    <row r="38" spans="1:26" ht="15.75" customHeight="1">
       <c r="A38" s="28"/>
       <c r="B38" s="28"/>
       <c r="C38" s="28"/>
@@ -7537,7 +7548,7 @@
       <c r="Y38" s="28"/>
       <c r="Z38" s="28"/>
     </row>
-    <row r="39" ht="15.75" customHeight="1">
+    <row r="39" spans="1:26" ht="15.75" customHeight="1">
       <c r="A39" s="28"/>
       <c r="B39" s="28"/>
       <c r="C39" s="28"/>
@@ -7565,7 +7576,7 @@
       <c r="Y39" s="28"/>
       <c r="Z39" s="28"/>
     </row>
-    <row r="40" ht="15.75" customHeight="1">
+    <row r="40" spans="1:26" ht="15.75" customHeight="1">
       <c r="A40" s="28"/>
       <c r="B40" s="28"/>
       <c r="C40" s="28"/>
@@ -7593,7 +7604,7 @@
       <c r="Y40" s="28"/>
       <c r="Z40" s="28"/>
     </row>
-    <row r="41" ht="15.75" customHeight="1">
+    <row r="41" spans="1:26" ht="15.75" customHeight="1">
       <c r="A41" s="28"/>
       <c r="B41" s="28"/>
       <c r="C41" s="28"/>
@@ -7621,7 +7632,7 @@
       <c r="Y41" s="28"/>
       <c r="Z41" s="28"/>
     </row>
-    <row r="42" ht="15.75" customHeight="1">
+    <row r="42" spans="1:26" ht="15.75" customHeight="1">
       <c r="A42" s="28"/>
       <c r="B42" s="28"/>
       <c r="C42" s="28"/>
@@ -7649,7 +7660,7 @@
       <c r="Y42" s="28"/>
       <c r="Z42" s="28"/>
     </row>
-    <row r="43" ht="15.75" customHeight="1">
+    <row r="43" spans="1:26" ht="15.75" customHeight="1">
       <c r="A43" s="28"/>
       <c r="B43" s="28"/>
       <c r="C43" s="28"/>
@@ -7677,7 +7688,7 @@
       <c r="Y43" s="28"/>
       <c r="Z43" s="28"/>
     </row>
-    <row r="44" ht="15.75" customHeight="1">
+    <row r="44" spans="1:26" ht="15.75" customHeight="1">
       <c r="A44" s="28"/>
       <c r="B44" s="28"/>
       <c r="C44" s="28"/>
@@ -7705,7 +7716,7 @@
       <c r="Y44" s="28"/>
       <c r="Z44" s="28"/>
     </row>
-    <row r="45" ht="15.75" customHeight="1">
+    <row r="45" spans="1:26" ht="15.75" customHeight="1">
       <c r="A45" s="28"/>
       <c r="B45" s="28"/>
       <c r="C45" s="28"/>
@@ -7733,7 +7744,7 @@
       <c r="Y45" s="28"/>
       <c r="Z45" s="28"/>
     </row>
-    <row r="46" ht="15.75" customHeight="1">
+    <row r="46" spans="1:26" ht="15.75" customHeight="1">
       <c r="A46" s="28"/>
       <c r="B46" s="28"/>
       <c r="C46" s="28"/>
@@ -7761,7 +7772,7 @@
       <c r="Y46" s="28"/>
       <c r="Z46" s="28"/>
     </row>
-    <row r="47" ht="15.75" customHeight="1">
+    <row r="47" spans="1:26" ht="15.75" customHeight="1">
       <c r="A47" s="28"/>
       <c r="B47" s="28"/>
       <c r="C47" s="28"/>
@@ -7789,7 +7800,7 @@
       <c r="Y47" s="28"/>
       <c r="Z47" s="28"/>
     </row>
-    <row r="48" ht="15.75" customHeight="1">
+    <row r="48" spans="1:26" ht="15.75" customHeight="1">
       <c r="A48" s="28"/>
       <c r="B48" s="28"/>
       <c r="C48" s="28"/>
@@ -7817,7 +7828,7 @@
       <c r="Y48" s="28"/>
       <c r="Z48" s="28"/>
     </row>
-    <row r="49" ht="15.75" customHeight="1">
+    <row r="49" spans="1:26" ht="15.75" customHeight="1">
       <c r="A49" s="28"/>
       <c r="B49" s="28"/>
       <c r="C49" s="28"/>
@@ -7845,7 +7856,7 @@
       <c r="Y49" s="28"/>
       <c r="Z49" s="28"/>
     </row>
-    <row r="50" ht="15.75" customHeight="1">
+    <row r="50" spans="1:26" ht="15.75" customHeight="1">
       <c r="A50" s="28"/>
       <c r="B50" s="28"/>
       <c r="C50" s="28"/>
@@ -7873,7 +7884,7 @@
       <c r="Y50" s="28"/>
       <c r="Z50" s="28"/>
     </row>
-    <row r="51" ht="15.75" customHeight="1">
+    <row r="51" spans="1:26" ht="15.75" customHeight="1">
       <c r="A51" s="28"/>
       <c r="B51" s="28"/>
       <c r="C51" s="28"/>
@@ -7901,7 +7912,7 @@
       <c r="Y51" s="28"/>
       <c r="Z51" s="28"/>
     </row>
-    <row r="52" ht="15.75" customHeight="1">
+    <row r="52" spans="1:26" ht="15.75" customHeight="1">
       <c r="A52" s="28"/>
       <c r="B52" s="28"/>
       <c r="C52" s="28"/>
@@ -7929,7 +7940,7 @@
       <c r="Y52" s="28"/>
       <c r="Z52" s="28"/>
     </row>
-    <row r="53" ht="15.75" customHeight="1">
+    <row r="53" spans="1:26" ht="15.75" customHeight="1">
       <c r="A53" s="28"/>
       <c r="B53" s="28"/>
       <c r="C53" s="28"/>
@@ -7957,7 +7968,7 @@
       <c r="Y53" s="28"/>
       <c r="Z53" s="28"/>
     </row>
-    <row r="54" ht="15.75" customHeight="1">
+    <row r="54" spans="1:26" ht="15.75" customHeight="1">
       <c r="A54" s="28"/>
       <c r="B54" s="28"/>
       <c r="C54" s="28"/>
@@ -7985,7 +7996,7 @@
       <c r="Y54" s="28"/>
       <c r="Z54" s="28"/>
     </row>
-    <row r="55" ht="15.75" customHeight="1">
+    <row r="55" spans="1:26" ht="15.75" customHeight="1">
       <c r="A55" s="28"/>
       <c r="B55" s="28"/>
       <c r="C55" s="28"/>
@@ -8013,7 +8024,7 @@
       <c r="Y55" s="28"/>
       <c r="Z55" s="28"/>
     </row>
-    <row r="56" ht="15.75" customHeight="1">
+    <row r="56" spans="1:26" ht="15.75" customHeight="1">
       <c r="A56" s="28"/>
       <c r="B56" s="28"/>
       <c r="C56" s="28"/>
@@ -8041,7 +8052,7 @@
       <c r="Y56" s="28"/>
       <c r="Z56" s="28"/>
     </row>
-    <row r="57" ht="15.75" customHeight="1">
+    <row r="57" spans="1:26" ht="15.75" customHeight="1">
       <c r="A57" s="28"/>
       <c r="B57" s="28"/>
       <c r="C57" s="28"/>
@@ -8069,7 +8080,7 @@
       <c r="Y57" s="28"/>
       <c r="Z57" s="28"/>
     </row>
-    <row r="58" ht="15.75" customHeight="1">
+    <row r="58" spans="1:26" ht="15.75" customHeight="1">
       <c r="A58" s="28"/>
       <c r="B58" s="28"/>
       <c r="C58" s="28"/>
@@ -8097,7 +8108,7 @@
       <c r="Y58" s="28"/>
       <c r="Z58" s="28"/>
     </row>
-    <row r="59" ht="15.75" customHeight="1">
+    <row r="59" spans="1:26" ht="15.75" customHeight="1">
       <c r="A59" s="28"/>
       <c r="B59" s="28"/>
       <c r="C59" s="28"/>
@@ -8125,7 +8136,7 @@
       <c r="Y59" s="28"/>
       <c r="Z59" s="28"/>
     </row>
-    <row r="60" ht="15.75" customHeight="1">
+    <row r="60" spans="1:26" ht="15.75" customHeight="1">
       <c r="A60" s="28"/>
       <c r="B60" s="28"/>
       <c r="C60" s="28"/>
@@ -8153,7 +8164,7 @@
       <c r="Y60" s="28"/>
       <c r="Z60" s="28"/>
     </row>
-    <row r="61" ht="15.75" customHeight="1">
+    <row r="61" spans="1:26" ht="15.75" customHeight="1">
       <c r="A61" s="28"/>
       <c r="B61" s="28"/>
       <c r="C61" s="28"/>
@@ -8181,7 +8192,7 @@
       <c r="Y61" s="28"/>
       <c r="Z61" s="28"/>
     </row>
-    <row r="62" ht="15.75" customHeight="1">
+    <row r="62" spans="1:26" ht="15.75" customHeight="1">
       <c r="A62" s="28"/>
       <c r="B62" s="28"/>
       <c r="C62" s="28"/>
@@ -8209,7 +8220,7 @@
       <c r="Y62" s="28"/>
       <c r="Z62" s="28"/>
     </row>
-    <row r="63" ht="15.75" customHeight="1">
+    <row r="63" spans="1:26" ht="15.75" customHeight="1">
       <c r="A63" s="28"/>
       <c r="B63" s="28"/>
       <c r="C63" s="28"/>
@@ -8237,7 +8248,7 @@
       <c r="Y63" s="28"/>
       <c r="Z63" s="28"/>
     </row>
-    <row r="64" ht="15.75" customHeight="1">
+    <row r="64" spans="1:26" ht="15.75" customHeight="1">
       <c r="A64" s="28"/>
       <c r="B64" s="28"/>
       <c r="C64" s="28"/>
@@ -8265,7 +8276,7 @@
       <c r="Y64" s="28"/>
       <c r="Z64" s="28"/>
     </row>
-    <row r="65" ht="15.75" customHeight="1">
+    <row r="65" spans="1:26" ht="15.75" customHeight="1">
       <c r="A65" s="28"/>
       <c r="B65" s="28"/>
       <c r="C65" s="28"/>
@@ -8293,7 +8304,7 @@
       <c r="Y65" s="28"/>
       <c r="Z65" s="28"/>
     </row>
-    <row r="66" ht="15.75" customHeight="1">
+    <row r="66" spans="1:26" ht="15.75" customHeight="1">
       <c r="A66" s="28"/>
       <c r="B66" s="28"/>
       <c r="C66" s="28"/>
@@ -8321,7 +8332,7 @@
       <c r="Y66" s="28"/>
       <c r="Z66" s="28"/>
     </row>
-    <row r="67" ht="15.75" customHeight="1">
+    <row r="67" spans="1:26" ht="15.75" customHeight="1">
       <c r="A67" s="28"/>
       <c r="B67" s="28"/>
       <c r="C67" s="28"/>
@@ -8349,7 +8360,7 @@
       <c r="Y67" s="28"/>
       <c r="Z67" s="28"/>
     </row>
-    <row r="68" ht="15.75" customHeight="1">
+    <row r="68" spans="1:26" ht="15.75" customHeight="1">
       <c r="A68" s="28"/>
       <c r="B68" s="28"/>
       <c r="C68" s="28"/>
@@ -8377,7 +8388,7 @@
       <c r="Y68" s="28"/>
       <c r="Z68" s="28"/>
     </row>
-    <row r="69" ht="15.75" customHeight="1">
+    <row r="69" spans="1:26" ht="15.75" customHeight="1">
       <c r="A69" s="28"/>
       <c r="B69" s="28"/>
       <c r="C69" s="28"/>
@@ -8405,7 +8416,7 @@
       <c r="Y69" s="28"/>
       <c r="Z69" s="28"/>
     </row>
-    <row r="70" ht="15.75" customHeight="1">
+    <row r="70" spans="1:26" ht="15.75" customHeight="1">
       <c r="A70" s="28"/>
       <c r="B70" s="28"/>
       <c r="C70" s="28"/>
@@ -8433,7 +8444,7 @@
       <c r="Y70" s="28"/>
       <c r="Z70" s="28"/>
     </row>
-    <row r="71" ht="15.75" customHeight="1">
+    <row r="71" spans="1:26" ht="15.75" customHeight="1">
       <c r="A71" s="28"/>
       <c r="B71" s="28"/>
       <c r="C71" s="28"/>
@@ -8461,7 +8472,7 @@
       <c r="Y71" s="28"/>
       <c r="Z71" s="28"/>
     </row>
-    <row r="72" ht="15.75" customHeight="1">
+    <row r="72" spans="1:26" ht="15.75" customHeight="1">
       <c r="A72" s="28"/>
       <c r="B72" s="28"/>
       <c r="C72" s="28"/>
@@ -8489,7 +8500,7 @@
       <c r="Y72" s="28"/>
       <c r="Z72" s="28"/>
     </row>
-    <row r="73" ht="15.75" customHeight="1">
+    <row r="73" spans="1:26" ht="15.75" customHeight="1">
       <c r="A73" s="28"/>
       <c r="B73" s="28"/>
       <c r="C73" s="28"/>
@@ -8517,7 +8528,7 @@
       <c r="Y73" s="28"/>
       <c r="Z73" s="28"/>
     </row>
-    <row r="74" ht="15.75" customHeight="1">
+    <row r="74" spans="1:26" ht="15.75" customHeight="1">
       <c r="A74" s="28"/>
       <c r="B74" s="28"/>
       <c r="C74" s="28"/>
@@ -8545,7 +8556,7 @@
       <c r="Y74" s="28"/>
       <c r="Z74" s="28"/>
     </row>
-    <row r="75" ht="15.75" customHeight="1">
+    <row r="75" spans="1:26" ht="15.75" customHeight="1">
       <c r="A75" s="28"/>
       <c r="B75" s="28"/>
       <c r="C75" s="28"/>
@@ -8573,7 +8584,7 @@
       <c r="Y75" s="28"/>
       <c r="Z75" s="28"/>
     </row>
-    <row r="76" ht="15.75" customHeight="1">
+    <row r="76" spans="1:26" ht="15.75" customHeight="1">
       <c r="A76" s="28"/>
       <c r="B76" s="28"/>
       <c r="C76" s="28"/>
@@ -8601,7 +8612,7 @@
       <c r="Y76" s="28"/>
       <c r="Z76" s="28"/>
     </row>
-    <row r="77" ht="15.75" customHeight="1">
+    <row r="77" spans="1:26" ht="15.75" customHeight="1">
       <c r="A77" s="28"/>
       <c r="B77" s="28"/>
       <c r="C77" s="28"/>
@@ -8629,7 +8640,7 @@
       <c r="Y77" s="28"/>
       <c r="Z77" s="28"/>
     </row>
-    <row r="78" ht="15.75" customHeight="1">
+    <row r="78" spans="1:26" ht="15.75" customHeight="1">
       <c r="A78" s="28"/>
       <c r="B78" s="28"/>
       <c r="C78" s="28"/>
@@ -8657,7 +8668,7 @@
       <c r="Y78" s="28"/>
       <c r="Z78" s="28"/>
     </row>
-    <row r="79" ht="15.75" customHeight="1">
+    <row r="79" spans="1:26" ht="15.75" customHeight="1">
       <c r="A79" s="28"/>
       <c r="B79" s="28"/>
       <c r="C79" s="28"/>
@@ -8685,7 +8696,7 @@
       <c r="Y79" s="28"/>
       <c r="Z79" s="28"/>
     </row>
-    <row r="80" ht="15.75" customHeight="1">
+    <row r="80" spans="1:26" ht="15.75" customHeight="1">
       <c r="A80" s="28"/>
       <c r="B80" s="28"/>
       <c r="C80" s="28"/>
@@ -8713,7 +8724,7 @@
       <c r="Y80" s="28"/>
       <c r="Z80" s="28"/>
     </row>
-    <row r="81" ht="15.75" customHeight="1">
+    <row r="81" spans="1:26" ht="15.75" customHeight="1">
       <c r="A81" s="28"/>
       <c r="B81" s="28"/>
       <c r="C81" s="28"/>
@@ -8741,7 +8752,7 @@
       <c r="Y81" s="28"/>
       <c r="Z81" s="28"/>
     </row>
-    <row r="82" ht="15.75" customHeight="1">
+    <row r="82" spans="1:26" ht="15.75" customHeight="1">
       <c r="A82" s="28"/>
       <c r="B82" s="28"/>
       <c r="C82" s="28"/>
@@ -8769,7 +8780,7 @@
       <c r="Y82" s="28"/>
       <c r="Z82" s="28"/>
     </row>
-    <row r="83" ht="15.75" customHeight="1">
+    <row r="83" spans="1:26" ht="15.75" customHeight="1">
       <c r="A83" s="28"/>
       <c r="B83" s="28"/>
       <c r="C83" s="28"/>
@@ -8797,7 +8808,7 @@
       <c r="Y83" s="28"/>
       <c r="Z83" s="28"/>
     </row>
-    <row r="84" ht="15.75" customHeight="1">
+    <row r="84" spans="1:26" ht="15.75" customHeight="1">
       <c r="A84" s="28"/>
       <c r="B84" s="28"/>
       <c r="C84" s="28"/>
@@ -8825,7 +8836,7 @@
       <c r="Y84" s="28"/>
       <c r="Z84" s="28"/>
     </row>
-    <row r="85" ht="15.75" customHeight="1">
+    <row r="85" spans="1:26" ht="15.75" customHeight="1">
       <c r="A85" s="28"/>
       <c r="B85" s="28"/>
       <c r="C85" s="28"/>
@@ -8853,7 +8864,7 @@
       <c r="Y85" s="28"/>
       <c r="Z85" s="28"/>
     </row>
-    <row r="86" ht="15.75" customHeight="1">
+    <row r="86" spans="1:26" ht="15.75" customHeight="1">
       <c r="A86" s="28"/>
       <c r="B86" s="28"/>
       <c r="C86" s="28"/>
@@ -8881,7 +8892,7 @@
       <c r="Y86" s="28"/>
       <c r="Z86" s="28"/>
     </row>
-    <row r="87" ht="15.75" customHeight="1">
+    <row r="87" spans="1:26" ht="15.75" customHeight="1">
       <c r="A87" s="28"/>
       <c r="B87" s="28"/>
       <c r="C87" s="28"/>
@@ -8909,7 +8920,7 @@
       <c r="Y87" s="28"/>
       <c r="Z87" s="28"/>
     </row>
-    <row r="88" ht="15.75" customHeight="1">
+    <row r="88" spans="1:26" ht="15.75" customHeight="1">
       <c r="A88" s="28"/>
       <c r="B88" s="28"/>
       <c r="C88" s="28"/>
@@ -8937,7 +8948,7 @@
       <c r="Y88" s="28"/>
       <c r="Z88" s="28"/>
     </row>
-    <row r="89" ht="15.75" customHeight="1">
+    <row r="89" spans="1:26" ht="15.75" customHeight="1">
       <c r="A89" s="28"/>
       <c r="B89" s="28"/>
       <c r="C89" s="28"/>
@@ -8965,7 +8976,7 @@
       <c r="Y89" s="28"/>
       <c r="Z89" s="28"/>
     </row>
-    <row r="90" ht="15.75" customHeight="1">
+    <row r="90" spans="1:26" ht="15.75" customHeight="1">
       <c r="A90" s="28"/>
       <c r="B90" s="28"/>
       <c r="C90" s="28"/>
@@ -8993,7 +9004,7 @@
       <c r="Y90" s="28"/>
       <c r="Z90" s="28"/>
     </row>
-    <row r="91" ht="15.75" customHeight="1">
+    <row r="91" spans="1:26" ht="15.75" customHeight="1">
       <c r="A91" s="28"/>
       <c r="B91" s="28"/>
       <c r="C91" s="28"/>
@@ -9021,7 +9032,7 @@
       <c r="Y91" s="28"/>
       <c r="Z91" s="28"/>
     </row>
-    <row r="92" ht="15.75" customHeight="1">
+    <row r="92" spans="1:26" ht="15.75" customHeight="1">
       <c r="A92" s="28"/>
       <c r="B92" s="28"/>
       <c r="C92" s="28"/>
@@ -9049,7 +9060,7 @@
       <c r="Y92" s="28"/>
       <c r="Z92" s="28"/>
     </row>
-    <row r="93" ht="15.75" customHeight="1">
+    <row r="93" spans="1:26" ht="15.75" customHeight="1">
       <c r="A93" s="28"/>
       <c r="B93" s="28"/>
       <c r="C93" s="28"/>
@@ -9077,7 +9088,7 @@
       <c r="Y93" s="28"/>
       <c r="Z93" s="28"/>
     </row>
-    <row r="94" ht="15.75" customHeight="1">
+    <row r="94" spans="1:26" ht="15.75" customHeight="1">
       <c r="A94" s="28"/>
       <c r="B94" s="28"/>
       <c r="C94" s="28"/>
@@ -9105,7 +9116,7 @@
       <c r="Y94" s="28"/>
       <c r="Z94" s="28"/>
     </row>
-    <row r="95" ht="15.75" customHeight="1">
+    <row r="95" spans="1:26" ht="15.75" customHeight="1">
       <c r="A95" s="28"/>
       <c r="B95" s="28"/>
       <c r="C95" s="28"/>
@@ -9133,7 +9144,7 @@
       <c r="Y95" s="28"/>
       <c r="Z95" s="28"/>
     </row>
-    <row r="96" ht="15.75" customHeight="1">
+    <row r="96" spans="1:26" ht="15.75" customHeight="1">
       <c r="A96" s="28"/>
       <c r="B96" s="28"/>
       <c r="C96" s="28"/>
@@ -9161,7 +9172,7 @@
       <c r="Y96" s="28"/>
       <c r="Z96" s="28"/>
     </row>
-    <row r="97" ht="15.75" customHeight="1">
+    <row r="97" spans="1:26" ht="15.75" customHeight="1">
       <c r="A97" s="28"/>
       <c r="B97" s="28"/>
       <c r="C97" s="28"/>
@@ -9189,7 +9200,7 @@
       <c r="Y97" s="28"/>
       <c r="Z97" s="28"/>
     </row>
-    <row r="98" ht="15.75" customHeight="1">
+    <row r="98" spans="1:26" ht="15.75" customHeight="1">
       <c r="A98" s="28"/>
       <c r="B98" s="28"/>
       <c r="C98" s="28"/>
@@ -9217,7 +9228,7 @@
       <c r="Y98" s="28"/>
       <c r="Z98" s="28"/>
     </row>
-    <row r="99" ht="15.75" customHeight="1">
+    <row r="99" spans="1:26" ht="15.75" customHeight="1">
       <c r="A99" s="28"/>
       <c r="B99" s="28"/>
       <c r="C99" s="28"/>
@@ -9245,7 +9256,7 @@
       <c r="Y99" s="28"/>
       <c r="Z99" s="28"/>
     </row>
-    <row r="100" ht="15.75" customHeight="1">
+    <row r="100" spans="1:26" ht="15.75" customHeight="1">
       <c r="A100" s="28"/>
       <c r="B100" s="28"/>
       <c r="C100" s="28"/>
@@ -9273,7 +9284,7 @@
       <c r="Y100" s="28"/>
       <c r="Z100" s="28"/>
     </row>
-    <row r="101" ht="15.75" customHeight="1">
+    <row r="101" spans="1:26" ht="15.75" customHeight="1">
       <c r="A101" s="28"/>
       <c r="B101" s="28"/>
       <c r="C101" s="28"/>
@@ -9301,7 +9312,7 @@
       <c r="Y101" s="28"/>
       <c r="Z101" s="28"/>
     </row>
-    <row r="102" ht="15.75" customHeight="1">
+    <row r="102" spans="1:26" ht="15.75" customHeight="1">
       <c r="A102" s="28"/>
       <c r="B102" s="28"/>
       <c r="C102" s="28"/>
@@ -9329,7 +9340,7 @@
       <c r="Y102" s="28"/>
       <c r="Z102" s="28"/>
     </row>
-    <row r="103" ht="15.75" customHeight="1">
+    <row r="103" spans="1:26" ht="15.75" customHeight="1">
       <c r="A103" s="28"/>
       <c r="B103" s="28"/>
       <c r="C103" s="28"/>
@@ -9357,7 +9368,7 @@
       <c r="Y103" s="28"/>
       <c r="Z103" s="28"/>
     </row>
-    <row r="104" ht="15.75" customHeight="1">
+    <row r="104" spans="1:26" ht="15.75" customHeight="1">
       <c r="A104" s="28"/>
       <c r="B104" s="28"/>
       <c r="C104" s="28"/>
@@ -9385,7 +9396,7 @@
       <c r="Y104" s="28"/>
       <c r="Z104" s="28"/>
     </row>
-    <row r="105" ht="15.75" customHeight="1">
+    <row r="105" spans="1:26" ht="15.75" customHeight="1">
       <c r="A105" s="28"/>
       <c r="B105" s="28"/>
       <c r="C105" s="28"/>
@@ -9413,7 +9424,7 @@
       <c r="Y105" s="28"/>
       <c r="Z105" s="28"/>
     </row>
-    <row r="106" ht="15.75" customHeight="1">
+    <row r="106" spans="1:26" ht="15.75" customHeight="1">
       <c r="A106" s="28"/>
       <c r="B106" s="28"/>
       <c r="C106" s="28"/>
@@ -9441,7 +9452,7 @@
       <c r="Y106" s="28"/>
       <c r="Z106" s="28"/>
     </row>
-    <row r="107" ht="15.75" customHeight="1">
+    <row r="107" spans="1:26" ht="15.75" customHeight="1">
       <c r="A107" s="28"/>
       <c r="B107" s="28"/>
       <c r="C107" s="28"/>
@@ -9469,7 +9480,7 @@
       <c r="Y107" s="28"/>
       <c r="Z107" s="28"/>
     </row>
-    <row r="108" ht="15.75" customHeight="1">
+    <row r="108" spans="1:26" ht="15.75" customHeight="1">
       <c r="A108" s="28"/>
       <c r="B108" s="28"/>
       <c r="C108" s="28"/>
@@ -9497,7 +9508,7 @@
       <c r="Y108" s="28"/>
       <c r="Z108" s="28"/>
     </row>
-    <row r="109" ht="15.75" customHeight="1">
+    <row r="109" spans="1:26" ht="15.75" customHeight="1">
       <c r="A109" s="28"/>
       <c r="B109" s="28"/>
       <c r="C109" s="28"/>
@@ -9525,7 +9536,7 @@
       <c r="Y109" s="28"/>
       <c r="Z109" s="28"/>
     </row>
-    <row r="110" ht="15.75" customHeight="1">
+    <row r="110" spans="1:26" ht="15.75" customHeight="1">
       <c r="A110" s="28"/>
       <c r="B110" s="28"/>
       <c r="C110" s="28"/>
@@ -9553,7 +9564,7 @@
       <c r="Y110" s="28"/>
       <c r="Z110" s="28"/>
     </row>
-    <row r="111" ht="15.75" customHeight="1">
+    <row r="111" spans="1:26" ht="15.75" customHeight="1">
       <c r="A111" s="28"/>
       <c r="B111" s="28"/>
       <c r="C111" s="28"/>
@@ -9581,7 +9592,7 @@
       <c r="Y111" s="28"/>
       <c r="Z111" s="28"/>
     </row>
-    <row r="112" ht="15.75" customHeight="1">
+    <row r="112" spans="1:26" ht="15.75" customHeight="1">
       <c r="A112" s="28"/>
       <c r="B112" s="28"/>
       <c r="C112" s="28"/>
@@ -9609,7 +9620,7 @@
       <c r="Y112" s="28"/>
       <c r="Z112" s="28"/>
     </row>
-    <row r="113" ht="15.75" customHeight="1">
+    <row r="113" spans="1:26" ht="15.75" customHeight="1">
       <c r="A113" s="28"/>
       <c r="B113" s="28"/>
       <c r="C113" s="28"/>
@@ -9637,7 +9648,7 @@
       <c r="Y113" s="28"/>
       <c r="Z113" s="28"/>
     </row>
-    <row r="114" ht="15.75" customHeight="1">
+    <row r="114" spans="1:26" ht="15.75" customHeight="1">
       <c r="A114" s="28"/>
       <c r="B114" s="28"/>
       <c r="C114" s="28"/>
@@ -9665,7 +9676,7 @@
       <c r="Y114" s="28"/>
       <c r="Z114" s="28"/>
     </row>
-    <row r="115" ht="15.75" customHeight="1">
+    <row r="115" spans="1:26" ht="15.75" customHeight="1">
       <c r="A115" s="28"/>
       <c r="B115" s="28"/>
       <c r="C115" s="28"/>
@@ -9693,7 +9704,7 @@
       <c r="Y115" s="28"/>
       <c r="Z115" s="28"/>
     </row>
-    <row r="116" ht="15.75" customHeight="1">
+    <row r="116" spans="1:26" ht="15.75" customHeight="1">
       <c r="A116" s="28"/>
       <c r="B116" s="28"/>
       <c r="C116" s="28"/>
@@ -9721,7 +9732,7 @@
       <c r="Y116" s="28"/>
       <c r="Z116" s="28"/>
     </row>
-    <row r="117" ht="15.75" customHeight="1">
+    <row r="117" spans="1:26" ht="15.75" customHeight="1">
       <c r="A117" s="28"/>
       <c r="B117" s="28"/>
       <c r="C117" s="28"/>
@@ -9749,7 +9760,7 @@
       <c r="Y117" s="28"/>
       <c r="Z117" s="28"/>
     </row>
-    <row r="118" ht="15.75" customHeight="1">
+    <row r="118" spans="1:26" ht="15.75" customHeight="1">
       <c r="A118" s="28"/>
       <c r="B118" s="28"/>
       <c r="C118" s="28"/>
@@ -9777,7 +9788,7 @@
       <c r="Y118" s="28"/>
       <c r="Z118" s="28"/>
     </row>
-    <row r="119" ht="15.75" customHeight="1">
+    <row r="119" spans="1:26" ht="15.75" customHeight="1">
       <c r="A119" s="28"/>
       <c r="B119" s="28"/>
       <c r="C119" s="28"/>
@@ -9805,7 +9816,7 @@
       <c r="Y119" s="28"/>
       <c r="Z119" s="28"/>
     </row>
-    <row r="120" ht="15.75" customHeight="1">
+    <row r="120" spans="1:26" ht="15.75" customHeight="1">
       <c r="A120" s="28"/>
       <c r="B120" s="28"/>
       <c r="C120" s="28"/>
@@ -9833,7 +9844,7 @@
       <c r="Y120" s="28"/>
       <c r="Z120" s="28"/>
     </row>
-    <row r="121" ht="15.75" customHeight="1">
+    <row r="121" spans="1:26" ht="15.75" customHeight="1">
       <c r="A121" s="28"/>
       <c r="B121" s="28"/>
       <c r="C121" s="28"/>
@@ -9861,7 +9872,7 @@
       <c r="Y121" s="28"/>
       <c r="Z121" s="28"/>
     </row>
-    <row r="122" ht="15.75" customHeight="1">
+    <row r="122" spans="1:26" ht="15.75" customHeight="1">
       <c r="A122" s="28"/>
       <c r="B122" s="28"/>
       <c r="C122" s="28"/>
@@ -9889,7 +9900,7 @@
       <c r="Y122" s="28"/>
       <c r="Z122" s="28"/>
     </row>
-    <row r="123" ht="15.75" customHeight="1">
+    <row r="123" spans="1:26" ht="15.75" customHeight="1">
       <c r="A123" s="28"/>
       <c r="B123" s="28"/>
       <c r="C123" s="28"/>
@@ -9917,7 +9928,7 @@
       <c r="Y123" s="28"/>
       <c r="Z123" s="28"/>
     </row>
-    <row r="124" ht="15.75" customHeight="1">
+    <row r="124" spans="1:26" ht="15.75" customHeight="1">
       <c r="A124" s="28"/>
       <c r="B124" s="28"/>
       <c r="C124" s="28"/>
@@ -9945,7 +9956,7 @@
       <c r="Y124" s="28"/>
       <c r="Z124" s="28"/>
     </row>
-    <row r="125" ht="15.75" customHeight="1">
+    <row r="125" spans="1:26" ht="15.75" customHeight="1">
       <c r="A125" s="28"/>
       <c r="B125" s="28"/>
       <c r="C125" s="28"/>
@@ -9973,7 +9984,7 @@
       <c r="Y125" s="28"/>
       <c r="Z125" s="28"/>
     </row>
-    <row r="126" ht="15.75" customHeight="1">
+    <row r="126" spans="1:26" ht="15.75" customHeight="1">
       <c r="A126" s="28"/>
       <c r="B126" s="28"/>
       <c r="C126" s="28"/>
@@ -10001,7 +10012,7 @@
       <c r="Y126" s="28"/>
       <c r="Z126" s="28"/>
     </row>
-    <row r="127" ht="15.75" customHeight="1">
+    <row r="127" spans="1:26" ht="15.75" customHeight="1">
       <c r="A127" s="28"/>
       <c r="B127" s="28"/>
       <c r="C127" s="28"/>
@@ -10029,7 +10040,7 @@
       <c r="Y127" s="28"/>
       <c r="Z127" s="28"/>
     </row>
-    <row r="128" ht="15.75" customHeight="1">
+    <row r="128" spans="1:26" ht="15.75" customHeight="1">
       <c r="A128" s="28"/>
       <c r="B128" s="28"/>
       <c r="C128" s="28"/>
@@ -10057,7 +10068,7 @@
       <c r="Y128" s="28"/>
       <c r="Z128" s="28"/>
     </row>
-    <row r="129" ht="15.75" customHeight="1">
+    <row r="129" spans="1:26" ht="15.75" customHeight="1">
       <c r="A129" s="28"/>
       <c r="B129" s="28"/>
       <c r="C129" s="28"/>
@@ -10085,7 +10096,7 @@
       <c r="Y129" s="28"/>
       <c r="Z129" s="28"/>
     </row>
-    <row r="130" ht="15.75" customHeight="1">
+    <row r="130" spans="1:26" ht="15.75" customHeight="1">
       <c r="A130" s="28"/>
       <c r="B130" s="28"/>
       <c r="C130" s="28"/>
@@ -10113,7 +10124,7 @@
       <c r="Y130" s="28"/>
       <c r="Z130" s="28"/>
     </row>
-    <row r="131" ht="15.75" customHeight="1">
+    <row r="131" spans="1:26" ht="15.75" customHeight="1">
       <c r="A131" s="28"/>
       <c r="B131" s="28"/>
       <c r="C131" s="28"/>
@@ -10141,7 +10152,7 @@
       <c r="Y131" s="28"/>
       <c r="Z131" s="28"/>
     </row>
-    <row r="132" ht="15.75" customHeight="1">
+    <row r="132" spans="1:26" ht="15.75" customHeight="1">
       <c r="A132" s="28"/>
       <c r="B132" s="28"/>
       <c r="C132" s="28"/>
@@ -10169,7 +10180,7 @@
       <c r="Y132" s="28"/>
       <c r="Z132" s="28"/>
     </row>
-    <row r="133" ht="15.75" customHeight="1">
+    <row r="133" spans="1:26" ht="15.75" customHeight="1">
       <c r="A133" s="28"/>
       <c r="B133" s="28"/>
       <c r="C133" s="28"/>
@@ -10197,7 +10208,7 @@
       <c r="Y133" s="28"/>
       <c r="Z133" s="28"/>
     </row>
-    <row r="134" ht="15.75" customHeight="1">
+    <row r="134" spans="1:26" ht="15.75" customHeight="1">
       <c r="A134" s="28"/>
       <c r="B134" s="28"/>
       <c r="C134" s="28"/>
@@ -10225,7 +10236,7 @@
       <c r="Y134" s="28"/>
       <c r="Z134" s="28"/>
     </row>
-    <row r="135" ht="15.75" customHeight="1">
+    <row r="135" spans="1:26" ht="15.75" customHeight="1">
       <c r="A135" s="28"/>
       <c r="B135" s="28"/>
       <c r="C135" s="28"/>
@@ -10253,7 +10264,7 @@
       <c r="Y135" s="28"/>
       <c r="Z135" s="28"/>
     </row>
-    <row r="136" ht="15.75" customHeight="1">
+    <row r="136" spans="1:26" ht="15.75" customHeight="1">
       <c r="A136" s="28"/>
       <c r="B136" s="28"/>
       <c r="C136" s="28"/>
@@ -10281,7 +10292,7 @@
       <c r="Y136" s="28"/>
       <c r="Z136" s="28"/>
     </row>
-    <row r="137" ht="15.75" customHeight="1">
+    <row r="137" spans="1:26" ht="15.75" customHeight="1">
       <c r="A137" s="28"/>
       <c r="B137" s="28"/>
       <c r="C137" s="28"/>
@@ -10309,7 +10320,7 @@
       <c r="Y137" s="28"/>
       <c r="Z137" s="28"/>
     </row>
-    <row r="138" ht="15.75" customHeight="1">
+    <row r="138" spans="1:26" ht="15.75" customHeight="1">
       <c r="A138" s="28"/>
       <c r="B138" s="28"/>
       <c r="C138" s="28"/>
@@ -10337,7 +10348,7 @@
       <c r="Y138" s="28"/>
       <c r="Z138" s="28"/>
     </row>
-    <row r="139" ht="15.75" customHeight="1">
+    <row r="139" spans="1:26" ht="15.75" customHeight="1">
       <c r="A139" s="28"/>
       <c r="B139" s="28"/>
       <c r="C139" s="28"/>
@@ -10365,7 +10376,7 @@
       <c r="Y139" s="28"/>
       <c r="Z139" s="28"/>
     </row>
-    <row r="140" ht="15.75" customHeight="1">
+    <row r="140" spans="1:26" ht="15.75" customHeight="1">
       <c r="A140" s="28"/>
       <c r="B140" s="28"/>
       <c r="C140" s="28"/>
@@ -10393,7 +10404,7 @@
       <c r="Y140" s="28"/>
       <c r="Z140" s="28"/>
     </row>
-    <row r="141" ht="15.75" customHeight="1">
+    <row r="141" spans="1:26" ht="15.75" customHeight="1">
       <c r="A141" s="28"/>
       <c r="B141" s="28"/>
       <c r="C141" s="28"/>
@@ -10421,7 +10432,7 @@
       <c r="Y141" s="28"/>
       <c r="Z141" s="28"/>
     </row>
-    <row r="142" ht="15.75" customHeight="1">
+    <row r="142" spans="1:26" ht="15.75" customHeight="1">
       <c r="A142" s="28"/>
       <c r="B142" s="28"/>
       <c r="C142" s="28"/>
@@ -10449,7 +10460,7 @@
       <c r="Y142" s="28"/>
       <c r="Z142" s="28"/>
     </row>
-    <row r="143" ht="15.75" customHeight="1">
+    <row r="143" spans="1:26" ht="15.75" customHeight="1">
       <c r="A143" s="28"/>
       <c r="B143" s="28"/>
       <c r="C143" s="28"/>
@@ -10477,7 +10488,7 @@
       <c r="Y143" s="28"/>
       <c r="Z143" s="28"/>
     </row>
-    <row r="144" ht="15.75" customHeight="1">
+    <row r="144" spans="1:26" ht="15.75" customHeight="1">
       <c r="A144" s="28"/>
       <c r="B144" s="28"/>
       <c r="C144" s="28"/>
@@ -10505,7 +10516,7 @@
       <c r="Y144" s="28"/>
       <c r="Z144" s="28"/>
     </row>
-    <row r="145" ht="15.75" customHeight="1">
+    <row r="145" spans="1:26" ht="15.75" customHeight="1">
       <c r="A145" s="28"/>
       <c r="B145" s="28"/>
       <c r="C145" s="28"/>
@@ -10533,7 +10544,7 @@
       <c r="Y145" s="28"/>
       <c r="Z145" s="28"/>
     </row>
-    <row r="146" ht="15.75" customHeight="1">
+    <row r="146" spans="1:26" ht="15.75" customHeight="1">
       <c r="A146" s="28"/>
       <c r="B146" s="28"/>
       <c r="C146" s="28"/>
@@ -10561,7 +10572,7 @@
       <c r="Y146" s="28"/>
       <c r="Z146" s="28"/>
     </row>
-    <row r="147" ht="15.75" customHeight="1">
+    <row r="147" spans="1:26" ht="15.75" customHeight="1">
       <c r="A147" s="28"/>
       <c r="B147" s="28"/>
       <c r="C147" s="28"/>
@@ -10589,7 +10600,7 @@
       <c r="Y147" s="28"/>
       <c r="Z147" s="28"/>
     </row>
-    <row r="148" ht="15.75" customHeight="1">
+    <row r="148" spans="1:26" ht="15.75" customHeight="1">
       <c r="A148" s="28"/>
       <c r="B148" s="28"/>
       <c r="C148" s="28"/>
@@ -10617,7 +10628,7 @@
       <c r="Y148" s="28"/>
       <c r="Z148" s="28"/>
     </row>
-    <row r="149" ht="15.75" customHeight="1">
+    <row r="149" spans="1:26" ht="15.75" customHeight="1">
       <c r="A149" s="28"/>
       <c r="B149" s="28"/>
       <c r="C149" s="28"/>
@@ -10645,7 +10656,7 @@
       <c r="Y149" s="28"/>
       <c r="Z149" s="28"/>
     </row>
-    <row r="150" ht="15.75" customHeight="1">
+    <row r="150" spans="1:26" ht="15.75" customHeight="1">
       <c r="A150" s="28"/>
       <c r="B150" s="28"/>
       <c r="C150" s="28"/>
@@ -10673,7 +10684,7 @@
       <c r="Y150" s="28"/>
       <c r="Z150" s="28"/>
     </row>
-    <row r="151" ht="15.75" customHeight="1">
+    <row r="151" spans="1:26" ht="15.75" customHeight="1">
       <c r="A151" s="28"/>
       <c r="B151" s="28"/>
       <c r="C151" s="28"/>
@@ -10701,7 +10712,7 @@
       <c r="Y151" s="28"/>
       <c r="Z151" s="28"/>
     </row>
-    <row r="152" ht="15.75" customHeight="1">
+    <row r="152" spans="1:26" ht="15.75" customHeight="1">
       <c r="A152" s="28"/>
       <c r="B152" s="28"/>
       <c r="C152" s="28"/>
@@ -10729,7 +10740,7 @@
       <c r="Y152" s="28"/>
       <c r="Z152" s="28"/>
     </row>
-    <row r="153" ht="15.75" customHeight="1">
+    <row r="153" spans="1:26" ht="15.75" customHeight="1">
       <c r="A153" s="28"/>
       <c r="B153" s="28"/>
       <c r="C153" s="28"/>
@@ -10757,7 +10768,7 @@
       <c r="Y153" s="28"/>
       <c r="Z153" s="28"/>
     </row>
-    <row r="154" ht="15.75" customHeight="1">
+    <row r="154" spans="1:26" ht="15.75" customHeight="1">
       <c r="A154" s="28"/>
       <c r="B154" s="28"/>
       <c r="C154" s="28"/>
@@ -10785,7 +10796,7 @@
       <c r="Y154" s="28"/>
       <c r="Z154" s="28"/>
     </row>
-    <row r="155" ht="15.75" customHeight="1">
+    <row r="155" spans="1:26" ht="15.75" customHeight="1">
       <c r="A155" s="28"/>
       <c r="B155" s="28"/>
       <c r="C155" s="28"/>
@@ -10813,7 +10824,7 @@
       <c r="Y155" s="28"/>
       <c r="Z155" s="28"/>
     </row>
-    <row r="156" ht="15.75" customHeight="1">
+    <row r="156" spans="1:26" ht="15.75" customHeight="1">
       <c r="A156" s="28"/>
       <c r="B156" s="28"/>
       <c r="C156" s="28"/>
@@ -10841,7 +10852,7 @@
       <c r="Y156" s="28"/>
       <c r="Z156" s="28"/>
     </row>
-    <row r="157" ht="15.75" customHeight="1">
+    <row r="157" spans="1:26" ht="15.75" customHeight="1">
       <c r="A157" s="28"/>
       <c r="B157" s="28"/>
       <c r="C157" s="28"/>
@@ -10869,7 +10880,7 @@
       <c r="Y157" s="28"/>
       <c r="Z157" s="28"/>
     </row>
-    <row r="158" ht="15.75" customHeight="1">
+    <row r="158" spans="1:26" ht="15.75" customHeight="1">
       <c r="A158" s="28"/>
       <c r="B158" s="28"/>
       <c r="C158" s="28"/>
@@ -10897,7 +10908,7 @@
       <c r="Y158" s="28"/>
       <c r="Z158" s="28"/>
     </row>
-    <row r="159" ht="15.75" customHeight="1">
+    <row r="159" spans="1:26" ht="15.75" customHeight="1">
       <c r="A159" s="28"/>
       <c r="B159" s="28"/>
       <c r="C159" s="28"/>
@@ -10925,7 +10936,7 @@
       <c r="Y159" s="28"/>
       <c r="Z159" s="28"/>
     </row>
-    <row r="160" ht="15.75" customHeight="1">
+    <row r="160" spans="1:26" ht="15.75" customHeight="1">
       <c r="A160" s="28"/>
       <c r="B160" s="28"/>
       <c r="C160" s="28"/>
@@ -10953,7 +10964,7 @@
       <c r="Y160" s="28"/>
       <c r="Z160" s="28"/>
     </row>
-    <row r="161" ht="15.75" customHeight="1">
+    <row r="161" spans="1:26" ht="15.75" customHeight="1">
       <c r="A161" s="28"/>
       <c r="B161" s="28"/>
       <c r="C161" s="28"/>
@@ -10981,7 +10992,7 @@
       <c r="Y161" s="28"/>
       <c r="Z161" s="28"/>
     </row>
-    <row r="162" ht="15.75" customHeight="1">
+    <row r="162" spans="1:26" ht="15.75" customHeight="1">
       <c r="A162" s="28"/>
       <c r="B162" s="28"/>
       <c r="C162" s="28"/>
@@ -11009,7 +11020,7 @@
       <c r="Y162" s="28"/>
       <c r="Z162" s="28"/>
     </row>
-    <row r="163" ht="15.75" customHeight="1">
+    <row r="163" spans="1:26" ht="15.75" customHeight="1">
       <c r="A163" s="28"/>
       <c r="B163" s="28"/>
       <c r="C163" s="28"/>
@@ -11037,7 +11048,7 @@
       <c r="Y163" s="28"/>
       <c r="Z163" s="28"/>
     </row>
-    <row r="164" ht="15.75" customHeight="1">
+    <row r="164" spans="1:26" ht="15.75" customHeight="1">
       <c r="A164" s="28"/>
       <c r="B164" s="28"/>
       <c r="C164" s="28"/>
@@ -11065,7 +11076,7 @@
       <c r="Y164" s="28"/>
       <c r="Z164" s="28"/>
     </row>
-    <row r="165" ht="15.75" customHeight="1">
+    <row r="165" spans="1:26" ht="15.75" customHeight="1">
       <c r="A165" s="28"/>
       <c r="B165" s="28"/>
       <c r="C165" s="28"/>
@@ -11093,7 +11104,7 @@
       <c r="Y165" s="28"/>
       <c r="Z165" s="28"/>
     </row>
-    <row r="166" ht="15.75" customHeight="1">
+    <row r="166" spans="1:26" ht="15.75" customHeight="1">
       <c r="A166" s="28"/>
       <c r="B166" s="28"/>
       <c r="C166" s="28"/>
@@ -11121,7 +11132,7 @@
       <c r="Y166" s="28"/>
       <c r="Z166" s="28"/>
     </row>
-    <row r="167" ht="15.75" customHeight="1">
+    <row r="167" spans="1:26" ht="15.75" customHeight="1">
       <c r="A167" s="28"/>
       <c r="B167" s="28"/>
       <c r="C167" s="28"/>
@@ -11149,7 +11160,7 @@
       <c r="Y167" s="28"/>
       <c r="Z167" s="28"/>
     </row>
-    <row r="168" ht="15.75" customHeight="1">
+    <row r="168" spans="1:26" ht="15.75" customHeight="1">
       <c r="A168" s="28"/>
       <c r="B168" s="28"/>
       <c r="C168" s="28"/>
@@ -11177,7 +11188,7 @@
       <c r="Y168" s="28"/>
       <c r="Z168" s="28"/>
     </row>
-    <row r="169" ht="15.75" customHeight="1">
+    <row r="169" spans="1:26" ht="15.75" customHeight="1">
       <c r="A169" s="28"/>
       <c r="B169" s="28"/>
       <c r="C169" s="28"/>
@@ -11205,7 +11216,7 @@
       <c r="Y169" s="28"/>
       <c r="Z169" s="28"/>
     </row>
-    <row r="170" ht="15.75" customHeight="1">
+    <row r="170" spans="1:26" ht="15.75" customHeight="1">
       <c r="A170" s="28"/>
       <c r="B170" s="28"/>
       <c r="C170" s="28"/>
@@ -11233,7 +11244,7 @@
       <c r="Y170" s="28"/>
       <c r="Z170" s="28"/>
     </row>
-    <row r="171" ht="15.75" customHeight="1">
+    <row r="171" spans="1:26" ht="15.75" customHeight="1">
       <c r="A171" s="28"/>
       <c r="B171" s="28"/>
       <c r="C171" s="28"/>
@@ -11261,7 +11272,7 @@
       <c r="Y171" s="28"/>
       <c r="Z171" s="28"/>
     </row>
-    <row r="172" ht="15.75" customHeight="1">
+    <row r="172" spans="1:26" ht="15.75" customHeight="1">
       <c r="A172" s="28"/>
       <c r="B172" s="28"/>
       <c r="C172" s="28"/>
@@ -11289,7 +11300,7 @@
       <c r="Y172" s="28"/>
       <c r="Z172" s="28"/>
     </row>
-    <row r="173" ht="15.75" customHeight="1">
+    <row r="173" spans="1:26" ht="15.75" customHeight="1">
       <c r="A173" s="28"/>
       <c r="B173" s="28"/>
       <c r="C173" s="28"/>
@@ -11317,7 +11328,7 @@
       <c r="Y173" s="28"/>
       <c r="Z173" s="28"/>
     </row>
-    <row r="174" ht="15.75" customHeight="1">
+    <row r="174" spans="1:26" ht="15.75" customHeight="1">
       <c r="A174" s="28"/>
       <c r="B174" s="28"/>
       <c r="C174" s="28"/>
@@ -11345,7 +11356,7 @@
       <c r="Y174" s="28"/>
       <c r="Z174" s="28"/>
     </row>
-    <row r="175" ht="15.75" customHeight="1">
+    <row r="175" spans="1:26" ht="15.75" customHeight="1">
       <c r="A175" s="28"/>
       <c r="B175" s="28"/>
       <c r="C175" s="28"/>
@@ -11373,7 +11384,7 @@
       <c r="Y175" s="28"/>
       <c r="Z175" s="28"/>
     </row>
-    <row r="176" ht="15.75" customHeight="1">
+    <row r="176" spans="1:26" ht="15.75" customHeight="1">
       <c r="A176" s="28"/>
       <c r="B176" s="28"/>
       <c r="C176" s="28"/>
@@ -11401,7 +11412,7 @@
       <c r="Y176" s="28"/>
       <c r="Z176" s="28"/>
     </row>
-    <row r="177" ht="15.75" customHeight="1">
+    <row r="177" spans="1:26" ht="15.75" customHeight="1">
       <c r="A177" s="28"/>
       <c r="B177" s="28"/>
       <c r="C177" s="28"/>
@@ -11429,7 +11440,7 @@
       <c r="Y177" s="28"/>
       <c r="Z177" s="28"/>
     </row>
-    <row r="178" ht="15.75" customHeight="1">
+    <row r="178" spans="1:26" ht="15.75" customHeight="1">
       <c r="A178" s="28"/>
       <c r="B178" s="28"/>
       <c r="C178" s="28"/>
@@ -11457,7 +11468,7 @@
       <c r="Y178" s="28"/>
       <c r="Z178" s="28"/>
     </row>
-    <row r="179" ht="15.75" customHeight="1">
+    <row r="179" spans="1:26" ht="15.75" customHeight="1">
       <c r="A179" s="28"/>
       <c r="B179" s="28"/>
       <c r="C179" s="28"/>
@@ -11485,7 +11496,7 @@
       <c r="Y179" s="28"/>
       <c r="Z179" s="28"/>
     </row>
-    <row r="180" ht="15.75" customHeight="1">
+    <row r="180" spans="1:26" ht="15.75" customHeight="1">
       <c r="A180" s="28"/>
       <c r="B180" s="28"/>
       <c r="C180" s="28"/>
@@ -11513,7 +11524,7 @@
       <c r="Y180" s="28"/>
       <c r="Z180" s="28"/>
     </row>
-    <row r="181" ht="15.75" customHeight="1">
+    <row r="181" spans="1:26" ht="15.75" customHeight="1">
       <c r="A181" s="28"/>
       <c r="B181" s="28"/>
       <c r="C181" s="28"/>
@@ -11541,7 +11552,7 @@
       <c r="Y181" s="28"/>
       <c r="Z181" s="28"/>
     </row>
-    <row r="182" ht="15.75" customHeight="1">
+    <row r="182" spans="1:26" ht="15.75" customHeight="1">
       <c r="A182" s="28"/>
       <c r="B182" s="28"/>
       <c r="C182" s="28"/>
@@ -11569,7 +11580,7 @@
       <c r="Y182" s="28"/>
       <c r="Z182" s="28"/>
     </row>
-    <row r="183" ht="15.75" customHeight="1">
+    <row r="183" spans="1:26" ht="15.75" customHeight="1">
       <c r="A183" s="28"/>
       <c r="B183" s="28"/>
       <c r="C183" s="28"/>
@@ -11597,7 +11608,7 @@
       <c r="Y183" s="28"/>
       <c r="Z183" s="28"/>
     </row>
-    <row r="184" ht="15.75" customHeight="1">
+    <row r="184" spans="1:26" ht="15.75" customHeight="1">
       <c r="A184" s="28"/>
       <c r="B184" s="28"/>
       <c r="C184" s="28"/>
@@ -11625,7 +11636,7 @@
       <c r="Y184" s="28"/>
       <c r="Z184" s="28"/>
     </row>
-    <row r="185" ht="15.75" customHeight="1">
+    <row r="185" spans="1:26" ht="15.75" customHeight="1">
       <c r="A185" s="28"/>
       <c r="B185" s="28"/>
       <c r="C185" s="28"/>
@@ -11653,7 +11664,7 @@
       <c r="Y185" s="28"/>
       <c r="Z185" s="28"/>
     </row>
-    <row r="186" ht="15.75" customHeight="1">
+    <row r="186" spans="1:26" ht="15.75" customHeight="1">
       <c r="A186" s="28"/>
       <c r="B186" s="28"/>
       <c r="C186" s="28"/>
@@ -11681,7 +11692,7 @@
       <c r="Y186" s="28"/>
       <c r="Z186" s="28"/>
     </row>
-    <row r="187" ht="15.75" customHeight="1">
+    <row r="187" spans="1:26" ht="15.75" customHeight="1">
       <c r="A187" s="28"/>
       <c r="B187" s="28"/>
       <c r="C187" s="28"/>
@@ -11709,7 +11720,7 @@
       <c r="Y187" s="28"/>
       <c r="Z187" s="28"/>
     </row>
-    <row r="188" ht="15.75" customHeight="1">
+    <row r="188" spans="1:26" ht="15.75" customHeight="1">
       <c r="A188" s="28"/>
       <c r="B188" s="28"/>
       <c r="C188" s="28"/>
@@ -11737,7 +11748,7 @@
       <c r="Y188" s="28"/>
       <c r="Z188" s="28"/>
     </row>
-    <row r="189" ht="15.75" customHeight="1">
+    <row r="189" spans="1:26" ht="15.75" customHeight="1">
       <c r="A189" s="28"/>
       <c r="B189" s="28"/>
       <c r="C189" s="28"/>
@@ -11765,7 +11776,7 @@
       <c r="Y189" s="28"/>
       <c r="Z189" s="28"/>
     </row>
-    <row r="190" ht="15.75" customHeight="1">
+    <row r="190" spans="1:26" ht="15.75" customHeight="1">
       <c r="A190" s="28"/>
       <c r="B190" s="28"/>
       <c r="C190" s="28"/>
@@ -11793,7 +11804,7 @@
       <c r="Y190" s="28"/>
       <c r="Z190" s="28"/>
     </row>
-    <row r="191" ht="15.75" customHeight="1">
+    <row r="191" spans="1:26" ht="15.75" customHeight="1">
       <c r="A191" s="28"/>
       <c r="B191" s="28"/>
       <c r="C191" s="28"/>
@@ -11821,7 +11832,7 @@
       <c r="Y191" s="28"/>
       <c r="Z191" s="28"/>
     </row>
-    <row r="192" ht="15.75" customHeight="1">
+    <row r="192" spans="1:26" ht="15.75" customHeight="1">
       <c r="A192" s="28"/>
       <c r="B192" s="28"/>
       <c r="C192" s="28"/>
@@ -11849,7 +11860,7 @@
       <c r="Y192" s="28"/>
       <c r="Z192" s="28"/>
     </row>
-    <row r="193" ht="15.75" customHeight="1">
+    <row r="193" spans="1:26" ht="15.75" customHeight="1">
       <c r="A193" s="28"/>
       <c r="B193" s="28"/>
       <c r="C193" s="28"/>
@@ -11877,7 +11888,7 @@
       <c r="Y193" s="28"/>
       <c r="Z193" s="28"/>
     </row>
-    <row r="194" ht="15.75" customHeight="1">
+    <row r="194" spans="1:26" ht="15.75" customHeight="1">
       <c r="A194" s="28"/>
       <c r="B194" s="28"/>
       <c r="C194" s="28"/>
@@ -11905,7 +11916,7 @@
       <c r="Y194" s="28"/>
       <c r="Z194" s="28"/>
     </row>
-    <row r="195" ht="15.75" customHeight="1">
+    <row r="195" spans="1:26" ht="15.75" customHeight="1">
       <c r="A195" s="28"/>
       <c r="B195" s="28"/>
       <c r="C195" s="28"/>
@@ -11933,7 +11944,7 @@
       <c r="Y195" s="28"/>
       <c r="Z195" s="28"/>
     </row>
-    <row r="196" ht="15.75" customHeight="1">
+    <row r="196" spans="1:26" ht="15.75" customHeight="1">
       <c r="A196" s="28"/>
       <c r="B196" s="28"/>
       <c r="C196" s="28"/>
@@ -11961,7 +11972,7 @@
       <c r="Y196" s="28"/>
       <c r="Z196" s="28"/>
     </row>
-    <row r="197" ht="15.75" customHeight="1">
+    <row r="197" spans="1:26" ht="15.75" customHeight="1">
       <c r="A197" s="28"/>
       <c r="B197" s="28"/>
       <c r="C197" s="28"/>
@@ -11989,7 +12000,7 @@
       <c r="Y197" s="28"/>
       <c r="Z197" s="28"/>
     </row>
-    <row r="198" ht="15.75" customHeight="1">
+    <row r="198" spans="1:26" ht="15.75" customHeight="1">
       <c r="A198" s="28"/>
       <c r="B198" s="28"/>
       <c r="C198" s="28"/>
@@ -12017,7 +12028,7 @@
       <c r="Y198" s="28"/>
       <c r="Z198" s="28"/>
     </row>
-    <row r="199" ht="15.75" customHeight="1">
+    <row r="199" spans="1:26" ht="15.75" customHeight="1">
       <c r="A199" s="28"/>
       <c r="B199" s="28"/>
       <c r="C199" s="28"/>
@@ -12045,7 +12056,7 @@
       <c r="Y199" s="28"/>
       <c r="Z199" s="28"/>
     </row>
-    <row r="200" ht="15.75" customHeight="1">
+    <row r="200" spans="1:26" ht="15.75" customHeight="1">
       <c r="A200" s="28"/>
       <c r="B200" s="28"/>
       <c r="C200" s="28"/>
@@ -12073,7 +12084,7 @@
       <c r="Y200" s="28"/>
       <c r="Z200" s="28"/>
     </row>
-    <row r="201" ht="15.75" customHeight="1">
+    <row r="201" spans="1:26" ht="15.75" customHeight="1">
       <c r="A201" s="28"/>
       <c r="B201" s="28"/>
       <c r="C201" s="28"/>
@@ -12101,7 +12112,7 @@
       <c r="Y201" s="28"/>
       <c r="Z201" s="28"/>
     </row>
-    <row r="202" ht="15.75" customHeight="1">
+    <row r="202" spans="1:26" ht="15.75" customHeight="1">
       <c r="A202" s="28"/>
       <c r="B202" s="28"/>
       <c r="C202" s="28"/>
@@ -12129,7 +12140,7 @@
       <c r="Y202" s="28"/>
       <c r="Z202" s="28"/>
     </row>
-    <row r="203" ht="15.75" customHeight="1">
+    <row r="203" spans="1:26" ht="15.75" customHeight="1">
       <c r="A203" s="28"/>
       <c r="B203" s="28"/>
       <c r="C203" s="28"/>
@@ -12157,7 +12168,7 @@
       <c r="Y203" s="28"/>
       <c r="Z203" s="28"/>
     </row>
-    <row r="204" ht="15.75" customHeight="1">
+    <row r="204" spans="1:26" ht="15.75" customHeight="1">
       <c r="A204" s="28"/>
       <c r="B204" s="28"/>
       <c r="C204" s="28"/>
@@ -12185,7 +12196,7 @@
       <c r="Y204" s="28"/>
       <c r="Z204" s="28"/>
     </row>
-    <row r="205" ht="15.75" customHeight="1">
+    <row r="205" spans="1:26" ht="15.75" customHeight="1">
       <c r="A205" s="28"/>
       <c r="B205" s="28"/>
       <c r="C205" s="28"/>
@@ -12213,7 +12224,7 @@
       <c r="Y205" s="28"/>
       <c r="Z205" s="28"/>
     </row>
-    <row r="206" ht="15.75" customHeight="1">
+    <row r="206" spans="1:26" ht="15.75" customHeight="1">
       <c r="A206" s="28"/>
       <c r="B206" s="28"/>
       <c r="C206" s="28"/>
@@ -12241,7 +12252,7 @@
       <c r="Y206" s="28"/>
       <c r="Z206" s="28"/>
     </row>
-    <row r="207" ht="15.75" customHeight="1">
+    <row r="207" spans="1:26" ht="15.75" customHeight="1">
       <c r="A207" s="28"/>
       <c r="B207" s="28"/>
       <c r="C207" s="28"/>
@@ -12269,7 +12280,7 @@
       <c r="Y207" s="28"/>
       <c r="Z207" s="28"/>
     </row>
-    <row r="208" ht="15.75" customHeight="1">
+    <row r="208" spans="1:26" ht="15.75" customHeight="1">
       <c r="A208" s="28"/>
       <c r="B208" s="28"/>
       <c r="C208" s="28"/>
@@ -12297,7 +12308,7 @@
       <c r="Y208" s="28"/>
       <c r="Z208" s="28"/>
     </row>
-    <row r="209" ht="15.75" customHeight="1">
+    <row r="209" spans="1:26" ht="15.75" customHeight="1">
       <c r="A209" s="28"/>
       <c r="B209" s="28"/>
       <c r="C209" s="28"/>
@@ -12325,7 +12336,7 @@
       <c r="Y209" s="28"/>
       <c r="Z209" s="28"/>
     </row>
-    <row r="210" ht="15.75" customHeight="1">
+    <row r="210" spans="1:26" ht="15.75" customHeight="1">
       <c r="A210" s="28"/>
       <c r="B210" s="28"/>
       <c r="C210" s="28"/>
@@ -12353,7 +12364,7 @@
       <c r="Y210" s="28"/>
       <c r="Z210" s="28"/>
     </row>
-    <row r="211" ht="15.75" customHeight="1">
+    <row r="211" spans="1:26" ht="15.75" customHeight="1">
       <c r="A211" s="28"/>
       <c r="B211" s="28"/>
       <c r="C211" s="28"/>
@@ -12381,7 +12392,7 @@
       <c r="Y211" s="28"/>
       <c r="Z211" s="28"/>
     </row>
-    <row r="212" ht="15.75" customHeight="1">
+    <row r="212" spans="1:26" ht="15.75" customHeight="1">
       <c r="A212" s="28"/>
       <c r="B212" s="28"/>
       <c r="C212" s="28"/>
@@ -12409,7 +12420,7 @@
       <c r="Y212" s="28"/>
       <c r="Z212" s="28"/>
     </row>
-    <row r="213" ht="15.75" customHeight="1">
+    <row r="213" spans="1:26" ht="15.75" customHeight="1">
       <c r="A213" s="28"/>
       <c r="B213" s="28"/>
       <c r="C213" s="28"/>
@@ -12437,7 +12448,7 @@
       <c r="Y213" s="28"/>
       <c r="Z213" s="28"/>
     </row>
-    <row r="214" ht="15.75" customHeight="1">
+    <row r="214" spans="1:26" ht="15.75" customHeight="1">
       <c r="A214" s="28"/>
       <c r="B214" s="28"/>
       <c r="C214" s="28"/>
@@ -12465,7 +12476,7 @@
       <c r="Y214" s="28"/>
       <c r="Z214" s="28"/>
     </row>
-    <row r="215" ht="15.75" customHeight="1">
+    <row r="215" spans="1:26" ht="15.75" customHeight="1">
       <c r="A215" s="28"/>
       <c r="B215" s="28"/>
       <c r="C215" s="28"/>
@@ -12493,7 +12504,7 @@
       <c r="Y215" s="28"/>
       <c r="Z215" s="28"/>
     </row>
-    <row r="216" ht="15.75" customHeight="1">
+    <row r="216" spans="1:26" ht="15.75" customHeight="1">
       <c r="A216" s="28"/>
       <c r="B216" s="28"/>
       <c r="C216" s="28"/>
@@ -12521,7 +12532,7 @@
       <c r="Y216" s="28"/>
       <c r="Z216" s="28"/>
     </row>
-    <row r="217" ht="15.75" customHeight="1">
+    <row r="217" spans="1:26" ht="15.75" customHeight="1">
       <c r="A217" s="28"/>
       <c r="B217" s="28"/>
       <c r="C217" s="28"/>
@@ -12549,7 +12560,7 @@
       <c r="Y217" s="28"/>
       <c r="Z217" s="28"/>
     </row>
-    <row r="218" ht="15.75" customHeight="1">
+    <row r="218" spans="1:26" ht="15.75" customHeight="1">
       <c r="A218" s="28"/>
       <c r="B218" s="28"/>
       <c r="C218" s="28"/>
@@ -12577,7 +12588,7 @@
       <c r="Y218" s="28"/>
       <c r="Z218" s="28"/>
     </row>
-    <row r="219" ht="15.75" customHeight="1">
+    <row r="219" spans="1:26" ht="15.75" customHeight="1">
       <c r="A219" s="28"/>
       <c r="B219" s="28"/>
       <c r="C219" s="28"/>
@@ -12605,7 +12616,7 @@
       <c r="Y219" s="28"/>
       <c r="Z219" s="28"/>
     </row>
-    <row r="220" ht="15.75" customHeight="1">
+    <row r="220" spans="1:26" ht="15.75" customHeight="1">
       <c r="A220" s="28"/>
       <c r="B220" s="28"/>
       <c r="C220" s="28"/>
@@ -12633,10 +12644,10 @@
       <c r="Y220" s="28"/>
       <c r="Z220" s="28"/>
     </row>
-    <row r="221" ht="15.75" customHeight="1"/>
-    <row r="222" ht="15.75" customHeight="1"/>
-    <row r="223" ht="15.75" customHeight="1"/>
-    <row r="224" ht="15.75" customHeight="1"/>
+    <row r="221" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="222" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="223" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="224" spans="1:26" ht="15.75" customHeight="1"/>
     <row r="225" ht="15.75" customHeight="1"/>
     <row r="226" ht="15.75" customHeight="1"/>
     <row r="227" ht="15.75" customHeight="1"/>
@@ -13414,9 +13425,7 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
chore(#9915): replace deprecated appearance fields in forms (#9924)
</commit_message>
<xml_diff>
--- a/config/covid-19/forms/contact/PLACE_TYPE-edit.xlsx
+++ b/config/covid-19/forms/contact/PLACE_TYPE-edit.xlsx
@@ -1,15 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\apoorva\cht-core\config\covid-19\forms\contact\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70D695B6-AB35-47B1-96E1-624F89DB045D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="survey" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="choices" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="settings" sheetId="3" r:id="rId6"/>
+    <sheet name="survey" sheetId="1" r:id="rId1"/>
+    <sheet name="choices" sheetId="2" r:id="rId2"/>
+    <sheet name="settings" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mgrHtCLCFoW/Qhae0+WX+vEV6cAMQ=="/>
     </ext>
@@ -18,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="255">
   <si>
     <t>type</t>
   </si>
@@ -164,9 +182,6 @@
     <t>Seems redundant, but needed to access name from choice label</t>
   </si>
   <si>
-    <t>db:person</t>
-  </si>
-  <si>
     <t>_id</t>
   </si>
   <si>
@@ -188,9 +203,6 @@
     <t>Contact primaire</t>
   </si>
   <si>
-    <t>db-object</t>
-  </si>
-  <si>
     <t>Select the Primary Contact</t>
   </si>
   <si>
@@ -236,9 +248,6 @@
     <t>not(${_id}) or selected( . , 'true') or boolean(${_id})</t>
   </si>
   <si>
-    <t>horizontal-compact</t>
-  </si>
-  <si>
     <t>boolean(${_id})</t>
   </si>
   <si>
@@ -786,41 +795,47 @@
   </si>
   <si>
     <t>en</t>
+  </si>
+  <si>
+    <t>select-contact type-person</t>
+  </si>
+  <si>
+    <t>columns-pack</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
@@ -830,7 +845,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -888,109 +903,107 @@
     </fill>
   </fills>
   <borders count="2">
-    <border/>
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="43">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="8" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="9" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="7" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="10" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="10" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="5" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="6" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="7" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="6" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="7" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="4" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1180,53 +1193,55 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:AR1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2.0" ySplit="1.0" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="C1" sqref="C1" pane="topRight"/>
-      <selection activeCell="A2" sqref="A2" pane="bottomLeft"/>
-      <selection activeCell="C2" sqref="C2" pane="bottomRight"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="19.71"/>
-    <col customWidth="1" min="2" max="2" width="22.71"/>
-    <col customWidth="1" min="3" max="3" width="24.29"/>
-    <col customWidth="1" hidden="1" min="4" max="4" width="38.71"/>
-    <col customWidth="1" hidden="1" min="5" max="5" width="54.57"/>
-    <col customWidth="1" hidden="1" min="6" max="6" width="23.57"/>
-    <col customWidth="1" hidden="1" min="7" max="7" width="55.14"/>
-    <col customWidth="1" hidden="1" min="8" max="8" width="8.14"/>
-    <col customWidth="1" hidden="1" min="9" max="9" width="16.43"/>
-    <col customWidth="1" min="10" max="10" width="8.14"/>
-    <col customWidth="1" min="11" max="11" width="11.43"/>
-    <col customWidth="1" min="12" max="12" width="10.71"/>
-    <col customWidth="1" min="13" max="13" width="15.14"/>
-    <col customWidth="1" min="14" max="14" width="32.0"/>
-    <col customWidth="1" min="15" max="15" width="50.14"/>
-    <col customWidth="1" min="16" max="16" width="48.71"/>
-    <col customWidth="1" min="17" max="17" width="31.14"/>
-    <col customWidth="1" min="18" max="18" width="33.43"/>
-    <col customWidth="1" min="19" max="19" width="36.29"/>
-    <col customWidth="1" min="20" max="21" width="8.14"/>
-    <col customWidth="1" min="22" max="22" width="33.86"/>
-    <col customWidth="1" min="23" max="24" width="8.14"/>
-    <col customWidth="1" min="25" max="25" width="8.71"/>
-    <col customWidth="1" min="26" max="36" width="7.71"/>
-    <col customWidth="1" min="37" max="44" width="15.14"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" customWidth="1"/>
+    <col min="4" max="4" width="38.6640625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="54.5546875" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5546875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="55.109375" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="8.109375" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="8.109375" customWidth="1"/>
+    <col min="11" max="11" width="11.44140625" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" customWidth="1"/>
+    <col min="13" max="13" width="15.109375" customWidth="1"/>
+    <col min="14" max="14" width="32" customWidth="1"/>
+    <col min="15" max="15" width="50.109375" customWidth="1"/>
+    <col min="16" max="16" width="48.6640625" customWidth="1"/>
+    <col min="17" max="17" width="31.109375" customWidth="1"/>
+    <col min="18" max="18" width="33.44140625" customWidth="1"/>
+    <col min="19" max="19" width="36.33203125" customWidth="1"/>
+    <col min="20" max="21" width="8.109375" customWidth="1"/>
+    <col min="22" max="22" width="33.88671875" customWidth="1"/>
+    <col min="23" max="24" width="8.109375" customWidth="1"/>
+    <col min="25" max="25" width="8.6640625" customWidth="1"/>
+    <col min="26" max="36" width="7.6640625" customWidth="1"/>
+    <col min="37" max="44" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
+    <row r="1" spans="1:44" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1324,7 +1339,7 @@
       <c r="AQ1" s="8"/>
       <c r="AR1" s="8"/>
     </row>
-    <row r="2" ht="14.25" customHeight="1">
+    <row r="2" spans="1:44" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
         <v>26</v>
       </c>
@@ -1388,7 +1403,7 @@
       <c r="AQ2" s="10"/>
       <c r="AR2" s="10"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:44" ht="14.4">
       <c r="A3" s="9" t="s">
         <v>26</v>
       </c>
@@ -1450,7 +1465,7 @@
       <c r="AQ3" s="10"/>
       <c r="AR3" s="10"/>
     </row>
-    <row r="4" ht="14.25" customHeight="1">
+    <row r="4" spans="1:44" ht="14.25" customHeight="1">
       <c r="A4" s="9" t="s">
         <v>30</v>
       </c>
@@ -1514,7 +1529,7 @@
       <c r="AQ4" s="10"/>
       <c r="AR4" s="10"/>
     </row>
-    <row r="5" ht="14.25" customHeight="1">
+    <row r="5" spans="1:44" ht="14.25" customHeight="1">
       <c r="A5" s="9" t="s">
         <v>30</v>
       </c>
@@ -1578,7 +1593,7 @@
       <c r="AQ5" s="10"/>
       <c r="AR5" s="10"/>
     </row>
-    <row r="6" ht="14.25" customHeight="1">
+    <row r="6" spans="1:44" ht="14.25" customHeight="1">
       <c r="A6" s="9" t="s">
         <v>30</v>
       </c>
@@ -1642,7 +1657,7 @@
       <c r="AQ6" s="10"/>
       <c r="AR6" s="10"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:44" ht="14.4">
       <c r="A7" s="9" t="s">
         <v>36</v>
       </c>
@@ -1690,7 +1705,7 @@
       <c r="AQ7" s="10"/>
       <c r="AR7" s="10"/>
     </row>
-    <row r="8" ht="14.25" customHeight="1">
+    <row r="8" spans="1:44" ht="14.25" customHeight="1">
       <c r="A8" s="9" t="s">
         <v>36</v>
       </c>
@@ -1738,7 +1753,7 @@
       <c r="AQ8" s="10"/>
       <c r="AR8" s="10"/>
     </row>
-    <row r="9" ht="14.25" customHeight="1">
+    <row r="9" spans="1:44" ht="14.25" customHeight="1">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -1784,7 +1799,7 @@
       <c r="AQ9" s="8"/>
       <c r="AR9" s="8"/>
     </row>
-    <row r="10" ht="14.25" customHeight="1">
+    <row r="10" spans="1:44" ht="14.25" customHeight="1">
       <c r="A10" s="17" t="s">
         <v>26</v>
       </c>
@@ -1848,7 +1863,7 @@
       <c r="AQ10" s="16"/>
       <c r="AR10" s="16"/>
     </row>
-    <row r="11" ht="14.25" customHeight="1">
+    <row r="11" spans="1:44" ht="14.25" customHeight="1">
       <c r="A11" s="17" t="s">
         <v>39</v>
       </c>
@@ -1912,7 +1927,7 @@
       <c r="AQ11" s="16"/>
       <c r="AR11" s="16"/>
     </row>
-    <row r="12" ht="14.25" customHeight="1">
+    <row r="12" spans="1:44" ht="14.25" customHeight="1">
       <c r="A12" s="17" t="s">
         <v>39</v>
       </c>
@@ -1976,7 +1991,7 @@
       <c r="AQ12" s="16"/>
       <c r="AR12" s="16"/>
     </row>
-    <row r="13" ht="14.25" customHeight="1">
+    <row r="13" spans="1:44" ht="14.25" customHeight="1">
       <c r="A13" s="17" t="s">
         <v>26</v>
       </c>
@@ -2040,7 +2055,7 @@
       <c r="AQ13" s="16"/>
       <c r="AR13" s="16"/>
     </row>
-    <row r="14" ht="14.25" customHeight="1">
+    <row r="14" spans="1:44" ht="14.25" customHeight="1">
       <c r="A14" s="17" t="s">
         <v>30</v>
       </c>
@@ -2104,7 +2119,7 @@
       <c r="AQ14" s="16"/>
       <c r="AR14" s="16"/>
     </row>
-    <row r="15" ht="14.25" customHeight="1">
+    <row r="15" spans="1:44" ht="14.25" customHeight="1">
       <c r="A15" s="17" t="s">
         <v>44</v>
       </c>
@@ -2158,36 +2173,36 @@
       <c r="AQ15" s="16"/>
       <c r="AR15" s="16"/>
     </row>
-    <row r="16" ht="14.25" customHeight="1">
+    <row r="16" spans="1:44" ht="14.25" customHeight="1">
       <c r="A16" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="C16" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="D16" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="E16" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="F16" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="16" t="s">
+      <c r="G16" s="16" t="s">
         <v>53</v>
-      </c>
-      <c r="G16" s="16" t="s">
-        <v>54</v>
       </c>
       <c r="H16" s="16"/>
       <c r="I16" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J16" s="16"/>
       <c r="K16" s="16"/>
       <c r="L16" s="16" t="s">
-        <v>56</v>
+        <v>253</v>
       </c>
       <c r="M16" s="16"/>
       <c r="N16" s="16"/>
@@ -2195,23 +2210,23 @@
       <c r="P16" s="16"/>
       <c r="Q16" s="16"/>
       <c r="R16" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="S16" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="T16" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="S16" s="16" t="s">
+      <c r="U16" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="T16" s="16" t="s">
+      <c r="V16" s="16" t="s">
         <v>59</v>
-      </c>
-      <c r="U16" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="V16" s="16" t="s">
-        <v>61</v>
       </c>
       <c r="W16" s="16"/>
       <c r="X16" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="Y16" s="16"/>
       <c r="Z16" s="16"/>
@@ -2234,7 +2249,7 @@
       <c r="AQ16" s="16"/>
       <c r="AR16" s="16"/>
     </row>
-    <row r="17" ht="14.25" customHeight="1">
+    <row r="17" spans="1:44" ht="14.25" customHeight="1">
       <c r="A17" s="17" t="s">
         <v>36</v>
       </c>
@@ -2282,48 +2297,48 @@
       <c r="AQ17" s="16"/>
       <c r="AR17" s="16"/>
     </row>
-    <row r="18" ht="14.25" customHeight="1">
+    <row r="18" spans="1:44" ht="14.25" customHeight="1">
       <c r="A18" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="D18" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="E18" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="F18" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="G18" s="16" t="s">
         <v>67</v>
-      </c>
-      <c r="F18" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="G18" s="16" t="s">
-        <v>69</v>
       </c>
       <c r="H18" s="16"/>
       <c r="I18" s="16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J18" s="16" t="s">
         <v>41</v>
       </c>
       <c r="K18" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L18" s="16" t="s">
-        <v>72</v>
+        <v>254</v>
       </c>
       <c r="M18" s="18" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="N18" s="16"/>
       <c r="O18" s="16"/>
       <c r="P18" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="Q18" s="16"/>
       <c r="R18" s="16"/>
@@ -2335,7 +2350,7 @@
       <c r="X18" s="16"/>
       <c r="Y18" s="16"/>
       <c r="Z18" s="18" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="AA18" s="16"/>
       <c r="AB18" s="16"/>
@@ -2356,12 +2371,12 @@
       <c r="AQ18" s="16"/>
       <c r="AR18" s="16"/>
     </row>
-    <row r="19" ht="14.25" customHeight="1">
+    <row r="19" spans="1:44" ht="14.25" customHeight="1">
       <c r="A19" s="17" t="s">
         <v>44</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
@@ -2377,7 +2392,7 @@
       <c r="N19" s="16"/>
       <c r="O19" s="16"/>
       <c r="P19" s="16" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="Q19" s="16"/>
       <c r="R19" s="16"/>
@@ -2408,7 +2423,7 @@
       <c r="AQ19" s="16"/>
       <c r="AR19" s="16"/>
     </row>
-    <row r="20" ht="14.25" customHeight="1">
+    <row r="20" spans="1:44" ht="14.25" customHeight="1">
       <c r="A20" s="17" t="s">
         <v>30</v>
       </c>
@@ -2416,36 +2431,36 @@
         <v>1</v>
       </c>
       <c r="C20" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="F20" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="G20" s="16" t="s">
         <v>79</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="F20" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="G20" s="16" t="s">
-        <v>82</v>
       </c>
       <c r="H20" s="16"/>
       <c r="I20" s="16" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="J20" s="16" t="s">
         <v>41</v>
       </c>
       <c r="K20" s="16" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="L20" s="16"/>
       <c r="M20" s="16"/>
       <c r="N20" s="16"/>
       <c r="O20" s="16"/>
       <c r="P20" s="18" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="Q20" s="16"/>
       <c r="R20" s="16"/>
@@ -2476,31 +2491,31 @@
       <c r="AQ20" s="16"/>
       <c r="AR20" s="16"/>
     </row>
-    <row r="21" ht="14.25" customHeight="1">
+    <row r="21" spans="1:44" ht="14.25" customHeight="1">
       <c r="A21" s="17" t="s">
         <v>30</v>
       </c>
       <c r="B21" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="E21" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="F21" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="G21" s="16" t="s">
         <v>88</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="F21" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="G21" s="16" t="s">
-        <v>91</v>
       </c>
       <c r="H21" s="16"/>
       <c r="I21" s="16" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="J21" s="16"/>
       <c r="K21" s="16"/>
@@ -2538,15 +2553,15 @@
       <c r="AQ21" s="16"/>
       <c r="AR21" s="16"/>
     </row>
-    <row r="22" ht="14.25" customHeight="1">
+    <row r="22" spans="1:44" ht="14.25" customHeight="1">
       <c r="A22" s="19" t="s">
         <v>30</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D22" s="20"/>
       <c r="E22" s="20"/>
@@ -2590,7 +2605,7 @@
       <c r="AQ22" s="20"/>
       <c r="AR22" s="20"/>
     </row>
-    <row r="23" ht="14.25" customHeight="1">
+    <row r="23" spans="1:44" ht="14.25" customHeight="1">
       <c r="A23" s="17" t="s">
         <v>30</v>
       </c>
@@ -2598,28 +2613,28 @@
         <v>25</v>
       </c>
       <c r="C23" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="F23" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="D23" s="16" t="s">
+      <c r="G23" s="16" t="s">
         <v>96</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="F23" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="G23" s="16" t="s">
-        <v>99</v>
       </c>
       <c r="H23" s="16"/>
       <c r="I23" s="16" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="J23" s="16"/>
       <c r="K23" s="16"/>
       <c r="L23" s="16" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="M23" s="16"/>
       <c r="N23" s="16"/>
@@ -2654,12 +2669,12 @@
       <c r="AQ23" s="16"/>
       <c r="AR23" s="16"/>
     </row>
-    <row r="24" ht="14.25" customHeight="1">
+    <row r="24" spans="1:44" ht="14.25" customHeight="1">
       <c r="A24" s="17" t="s">
         <v>44</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
@@ -2675,7 +2690,7 @@
       <c r="N24" s="16"/>
       <c r="O24" s="16"/>
       <c r="P24" s="16" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="Q24" s="16"/>
       <c r="R24" s="16"/>
@@ -2706,12 +2721,12 @@
       <c r="AQ24" s="16"/>
       <c r="AR24" s="16"/>
     </row>
-    <row r="25" ht="14.25" customHeight="1">
+    <row r="25" spans="1:44" ht="14.25" customHeight="1">
       <c r="A25" s="17" t="s">
         <v>26</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C25" s="16" t="s">
         <v>28</v>
@@ -2770,12 +2785,12 @@
       <c r="AQ25" s="16"/>
       <c r="AR25" s="16"/>
     </row>
-    <row r="26" ht="14.25" customHeight="1">
+    <row r="26" spans="1:44" ht="14.25" customHeight="1">
       <c r="A26" s="17" t="s">
         <v>39</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C26" s="16" t="s">
         <v>28</v>
@@ -2815,7 +2830,7 @@
       <c r="X26" s="16"/>
       <c r="Y26" s="16"/>
       <c r="Z26" s="16" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="AA26" s="16"/>
       <c r="AB26" s="16"/>
@@ -2836,12 +2851,12 @@
       <c r="AQ26" s="16"/>
       <c r="AR26" s="16"/>
     </row>
-    <row r="27" ht="14.25" customHeight="1">
+    <row r="27" spans="1:44" ht="14.25" customHeight="1">
       <c r="A27" s="17" t="s">
         <v>39</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C27" s="16" t="s">
         <v>28</v>
@@ -2900,12 +2915,12 @@
       <c r="AQ27" s="16"/>
       <c r="AR27" s="16"/>
     </row>
-    <row r="28" ht="14.25" customHeight="1">
+    <row r="28" spans="1:44" ht="14.25" customHeight="1">
       <c r="A28" s="17" t="s">
         <v>39</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C28" s="16" t="s">
         <v>28</v>
@@ -2962,12 +2977,12 @@
       <c r="AQ28" s="16"/>
       <c r="AR28" s="16"/>
     </row>
-    <row r="29" ht="14.25" customHeight="1">
+    <row r="29" spans="1:44" ht="14.25" customHeight="1">
       <c r="A29" s="17" t="s">
         <v>44</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C29" s="16"/>
       <c r="D29" s="16"/>
@@ -2983,7 +2998,7 @@
       <c r="N29" s="16"/>
       <c r="O29" s="16"/>
       <c r="P29" s="16" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="Q29" s="16"/>
       <c r="R29" s="16"/>
@@ -2995,7 +3010,7 @@
       <c r="X29" s="16"/>
       <c r="Y29" s="16"/>
       <c r="Z29" s="16" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="AA29" s="16"/>
       <c r="AB29" s="16"/>
@@ -3016,12 +3031,12 @@
       <c r="AQ29" s="16"/>
       <c r="AR29" s="16"/>
     </row>
-    <row r="30" ht="14.25" customHeight="1">
+    <row r="30" spans="1:44" ht="14.25" customHeight="1">
       <c r="A30" s="17" t="s">
         <v>44</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C30" s="16"/>
       <c r="D30" s="16"/>
@@ -3037,7 +3052,7 @@
       <c r="N30" s="16"/>
       <c r="O30" s="16"/>
       <c r="P30" s="16" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="Q30" s="16"/>
       <c r="R30" s="16"/>
@@ -3068,12 +3083,12 @@
       <c r="AQ30" s="16"/>
       <c r="AR30" s="16"/>
     </row>
-    <row r="31" ht="14.25" customHeight="1">
+    <row r="31" spans="1:44" ht="14.25" customHeight="1">
       <c r="A31" s="17" t="s">
         <v>44</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C31" s="16"/>
       <c r="D31" s="16"/>
@@ -3089,7 +3104,7 @@
       <c r="N31" s="16"/>
       <c r="O31" s="16"/>
       <c r="P31" s="16" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="Q31" s="16"/>
       <c r="R31" s="16"/>
@@ -3120,7 +3135,7 @@
       <c r="AQ31" s="16"/>
       <c r="AR31" s="16"/>
     </row>
-    <row r="32" ht="14.25" customHeight="1">
+    <row r="32" spans="1:44" ht="14.25" customHeight="1">
       <c r="A32" s="17" t="s">
         <v>36</v>
       </c>
@@ -3168,7 +3183,7 @@
       <c r="AQ32" s="16"/>
       <c r="AR32" s="16"/>
     </row>
-    <row r="33" ht="14.25" customHeight="1">
+    <row r="33" spans="1:44" ht="14.25" customHeight="1">
       <c r="A33" s="17" t="s">
         <v>36</v>
       </c>
@@ -3216,7 +3231,7 @@
       <c r="AQ33" s="16"/>
       <c r="AR33" s="16"/>
     </row>
-    <row r="34" ht="14.25" customHeight="1">
+    <row r="34" spans="1:44" ht="14.25" customHeight="1">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
@@ -3262,12 +3277,12 @@
       <c r="AQ34" s="8"/>
       <c r="AR34" s="8"/>
     </row>
-    <row r="35" ht="14.25" customHeight="1">
+    <row r="35" spans="1:44" ht="14.25" customHeight="1">
       <c r="A35" s="17" t="s">
         <v>26</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C35" s="16" t="s">
         <v>28</v>
@@ -3291,7 +3306,7 @@
       <c r="J35" s="16"/>
       <c r="K35" s="16"/>
       <c r="L35" s="16" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="M35" s="16"/>
       <c r="N35" s="16"/>
@@ -3326,12 +3341,12 @@
       <c r="AQ35" s="16"/>
       <c r="AR35" s="16"/>
     </row>
-    <row r="36" ht="14.25" customHeight="1">
+    <row r="36" spans="1:44" ht="14.25" customHeight="1">
       <c r="A36" s="17" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C36" s="16" t="s">
         <v>28</v>
@@ -3361,7 +3376,7 @@
       <c r="N36" s="16"/>
       <c r="O36" s="16"/>
       <c r="P36" s="18" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="Q36" s="16"/>
       <c r="R36" s="16"/>
@@ -3392,12 +3407,12 @@
       <c r="AQ36" s="16"/>
       <c r="AR36" s="16"/>
     </row>
-    <row r="37" ht="13.5" customHeight="1">
+    <row r="37" spans="1:44" ht="13.5" customHeight="1">
       <c r="A37" s="17" t="s">
         <v>44</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C37" s="16"/>
       <c r="D37" s="16"/>
@@ -3413,7 +3428,7 @@
       <c r="N37" s="16"/>
       <c r="O37" s="16"/>
       <c r="P37" s="18" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="Q37" s="16"/>
       <c r="R37" s="16"/>
@@ -3444,12 +3459,12 @@
       <c r="AQ37" s="16"/>
       <c r="AR37" s="16"/>
     </row>
-    <row r="38" ht="14.25" customHeight="1">
+    <row r="38" spans="1:44" ht="14.25" customHeight="1">
       <c r="A38" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C38" s="16" t="s">
         <v>28</v>
@@ -3479,7 +3494,7 @@
       <c r="N38" s="16"/>
       <c r="O38" s="16"/>
       <c r="P38" s="18" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="Q38" s="16"/>
       <c r="R38" s="16"/>
@@ -3510,12 +3525,12 @@
       <c r="AQ38" s="16"/>
       <c r="AR38" s="16"/>
     </row>
-    <row r="39" ht="14.25" customHeight="1">
+    <row r="39" spans="1:44" ht="14.25" customHeight="1">
       <c r="A39" s="17" t="s">
         <v>44</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C39" s="16"/>
       <c r="D39" s="16"/>
@@ -3531,7 +3546,7 @@
       <c r="N39" s="16"/>
       <c r="O39" s="16"/>
       <c r="P39" s="18" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="Q39" s="16"/>
       <c r="R39" s="16"/>
@@ -3562,7 +3577,7 @@
       <c r="AQ39" s="16"/>
       <c r="AR39" s="16"/>
     </row>
-    <row r="40" ht="14.25" customHeight="1">
+    <row r="40" spans="1:44" ht="14.25" customHeight="1">
       <c r="A40" s="17" t="s">
         <v>36</v>
       </c>
@@ -3610,14 +3625,14 @@
       <c r="AQ40" s="16"/>
       <c r="AR40" s="16"/>
     </row>
-    <row r="41" ht="15.75" customHeight="1"/>
-    <row r="42" ht="15.75" customHeight="1"/>
-    <row r="43" ht="15.75" customHeight="1"/>
-    <row r="44" ht="15.75" customHeight="1"/>
-    <row r="45" ht="15.75" customHeight="1"/>
-    <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
-    <row r="48" ht="15.75" customHeight="1"/>
+    <row r="41" spans="1:44" ht="15.75" customHeight="1"/>
+    <row r="42" spans="1:44" ht="15.75" customHeight="1"/>
+    <row r="43" spans="1:44" ht="15.75" customHeight="1"/>
+    <row r="44" spans="1:44" ht="15.75" customHeight="1"/>
+    <row r="45" spans="1:44" ht="15.75" customHeight="1"/>
+    <row r="46" spans="1:44" ht="15.75" customHeight="1"/>
+    <row r="47" spans="1:44" ht="15.75" customHeight="1"/>
+    <row r="48" spans="1:44" ht="15.75" customHeight="1"/>
     <row r="49" ht="15.75" customHeight="1"/>
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1"/>
@@ -4572,46 +4587,44 @@
     <row r="1000" ht="15.75" customHeight="1"/>
     <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="21.14"/>
-    <col customWidth="1" min="2" max="2" width="9.71"/>
-    <col customWidth="1" min="3" max="3" width="26.71"/>
-    <col customWidth="1" min="4" max="4" width="46.0"/>
-    <col customWidth="1" min="5" max="5" width="51.57"/>
-    <col customWidth="1" min="6" max="6" width="49.14"/>
-    <col customWidth="1" min="7" max="7" width="35.0"/>
-    <col customWidth="1" min="8" max="8" width="7.71"/>
-    <col customWidth="1" min="9" max="9" width="17.57"/>
-    <col customWidth="1" min="10" max="13" width="7.71"/>
-    <col customWidth="1" min="14" max="26" width="15.14"/>
+    <col min="1" max="1" width="21.109375" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="46" customWidth="1"/>
+    <col min="5" max="5" width="51.5546875" customWidth="1"/>
+    <col min="6" max="6" width="49.109375" customWidth="1"/>
+    <col min="7" max="7" width="35" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" customWidth="1"/>
+    <col min="9" max="9" width="17.5546875" customWidth="1"/>
+    <col min="10" max="13" width="7.6640625" customWidth="1"/>
+    <col min="14" max="26" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
+    <row r="1" spans="1:26" ht="14.25" customHeight="1">
       <c r="A1" s="21" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D1" s="22" t="s">
         <v>3</v>
@@ -4649,31 +4662,31 @@
       <c r="Y1" s="28"/>
       <c r="Z1" s="28"/>
     </row>
-    <row r="2" ht="14.25" customHeight="1">
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" s="30" t="s">
         <v>128</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="E2" s="31" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="F2" s="32" t="s">
         <v>130</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="G2" s="33" t="s">
         <v>131</v>
-      </c>
-      <c r="E2" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="F2" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="G2" s="33" t="s">
-        <v>134</v>
       </c>
       <c r="H2" s="34"/>
       <c r="I2" s="35" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J2" s="28"/>
       <c r="K2" s="28"/>
@@ -4693,31 +4706,31 @@
       <c r="Y2" s="28"/>
       <c r="Z2" s="28"/>
     </row>
-    <row r="3" ht="14.25" customHeight="1">
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="29" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B3" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="E3" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="F3" s="32" t="s">
         <v>137</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="G3" s="33" t="s">
         <v>138</v>
-      </c>
-      <c r="E3" s="31" t="s">
-        <v>139</v>
-      </c>
-      <c r="F3" s="32" t="s">
-        <v>140</v>
-      </c>
-      <c r="G3" s="33" t="s">
-        <v>141</v>
       </c>
       <c r="H3" s="34"/>
       <c r="I3" s="35" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="J3" s="28"/>
       <c r="K3" s="28"/>
@@ -4737,31 +4750,31 @@
       <c r="Y3" s="28"/>
       <c r="Z3" s="28"/>
     </row>
-    <row r="4" ht="14.25" customHeight="1">
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="29" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" s="37" t="s">
+        <v>141</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>142</v>
+      </c>
+      <c r="E4" s="39" t="s">
         <v>143</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="F4" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="G4" s="33" t="s">
         <v>145</v>
-      </c>
-      <c r="E4" s="39" t="s">
-        <v>146</v>
-      </c>
-      <c r="F4" s="32" t="s">
-        <v>147</v>
-      </c>
-      <c r="G4" s="33" t="s">
-        <v>148</v>
       </c>
       <c r="H4" s="34"/>
       <c r="I4" s="35" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J4" s="28"/>
       <c r="K4" s="28"/>
@@ -4781,31 +4794,31 @@
       <c r="Y4" s="28"/>
       <c r="Z4" s="28"/>
     </row>
-    <row r="5" ht="14.25" customHeight="1">
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" s="29" t="s">
         <v>42</v>
       </c>
       <c r="B5" s="36" t="s">
+        <v>147</v>
+      </c>
+      <c r="C5" s="37" t="s">
+        <v>148</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="E5" s="39" t="s">
         <v>150</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="F5" s="32" t="s">
         <v>151</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="G5" s="33" t="s">
         <v>152</v>
-      </c>
-      <c r="E5" s="39" t="s">
-        <v>153</v>
-      </c>
-      <c r="F5" s="32" t="s">
-        <v>154</v>
-      </c>
-      <c r="G5" s="33" t="s">
-        <v>155</v>
       </c>
       <c r="H5" s="34"/>
       <c r="I5" s="35" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="J5" s="28"/>
       <c r="K5" s="28"/>
@@ -4825,31 +4838,31 @@
       <c r="Y5" s="28"/>
       <c r="Z5" s="28"/>
     </row>
-    <row r="6" ht="14.25" customHeight="1">
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="B6" s="36" t="s">
+        <v>155</v>
+      </c>
+      <c r="C6" s="37" t="s">
+        <v>156</v>
+      </c>
+      <c r="D6" s="30" t="s">
         <v>157</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="E6" s="39" t="s">
         <v>158</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="F6" s="32" t="s">
         <v>159</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="G6" s="33" t="s">
         <v>160</v>
-      </c>
-      <c r="E6" s="39" t="s">
-        <v>161</v>
-      </c>
-      <c r="F6" s="32" t="s">
-        <v>162</v>
-      </c>
-      <c r="G6" s="33" t="s">
-        <v>163</v>
       </c>
       <c r="H6" s="34"/>
       <c r="I6" s="35" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J6" s="28"/>
       <c r="K6" s="28"/>
@@ -4869,31 +4882,31 @@
       <c r="Y6" s="28"/>
       <c r="Z6" s="28"/>
     </row>
-    <row r="7" ht="14.25" customHeight="1">
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="28" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B7" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>163</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>164</v>
+      </c>
+      <c r="E7" s="39" t="s">
         <v>165</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="F7" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="G7" s="33" t="s">
         <v>167</v>
-      </c>
-      <c r="E7" s="39" t="s">
-        <v>168</v>
-      </c>
-      <c r="F7" s="32" t="s">
-        <v>169</v>
-      </c>
-      <c r="G7" s="33" t="s">
-        <v>170</v>
       </c>
       <c r="H7" s="34"/>
       <c r="I7" s="35" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="J7" s="28"/>
       <c r="K7" s="28"/>
@@ -4913,31 +4926,31 @@
       <c r="Y7" s="28"/>
       <c r="Z7" s="28"/>
     </row>
-    <row r="8" ht="14.25" customHeight="1">
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="28" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B8" s="28" t="s">
+        <v>169</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>170</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="E8" s="39" t="s">
         <v>172</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="F8" s="32" t="s">
         <v>173</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="G8" s="33" t="s">
         <v>174</v>
-      </c>
-      <c r="E8" s="39" t="s">
-        <v>175</v>
-      </c>
-      <c r="F8" s="32" t="s">
-        <v>176</v>
-      </c>
-      <c r="G8" s="33" t="s">
-        <v>177</v>
       </c>
       <c r="H8" s="34"/>
       <c r="I8" s="35" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J8" s="28"/>
       <c r="K8" s="28"/>
@@ -4957,31 +4970,31 @@
       <c r="Y8" s="28"/>
       <c r="Z8" s="28"/>
     </row>
-    <row r="9" ht="14.25" customHeight="1">
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="28" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B9" s="36" t="s">
+        <v>175</v>
+      </c>
+      <c r="C9" s="37" t="s">
+        <v>176</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>177</v>
+      </c>
+      <c r="E9" s="39" t="s">
         <v>178</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="F9" s="32" t="s">
         <v>179</v>
       </c>
-      <c r="D9" s="30" t="s">
-        <v>180</v>
-      </c>
-      <c r="E9" s="39" t="s">
-        <v>181</v>
-      </c>
-      <c r="F9" s="32" t="s">
-        <v>182</v>
-      </c>
       <c r="G9" s="33" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H9" s="34"/>
       <c r="I9" s="35" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="J9" s="28"/>
       <c r="K9" s="28"/>
@@ -5001,31 +5014,31 @@
       <c r="Y9" s="28"/>
       <c r="Z9" s="28"/>
     </row>
-    <row r="10" ht="14.25" customHeight="1">
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>182</v>
+      </c>
+      <c r="C10" s="37" t="s">
+        <v>183</v>
+      </c>
+      <c r="D10" s="30" t="s">
         <v>184</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="E10" s="39" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="F10" s="40" t="s">
         <v>186</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="G10" s="33" t="s">
         <v>187</v>
-      </c>
-      <c r="E10" s="39" t="s">
-        <v>188</v>
-      </c>
-      <c r="F10" s="40" t="s">
-        <v>189</v>
-      </c>
-      <c r="G10" s="33" t="s">
-        <v>190</v>
       </c>
       <c r="H10" s="34"/>
       <c r="I10" s="35" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="J10" s="28"/>
       <c r="K10" s="28"/>
@@ -5045,31 +5058,31 @@
       <c r="Y10" s="28"/>
       <c r="Z10" s="28"/>
     </row>
-    <row r="11" ht="14.25" customHeight="1">
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="28" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B11" s="36" t="s">
+        <v>189</v>
+      </c>
+      <c r="C11" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="E11" s="39" t="s">
         <v>192</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="F11" s="40" t="s">
         <v>193</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="G11" s="33" t="s">
         <v>194</v>
-      </c>
-      <c r="E11" s="39" t="s">
-        <v>195</v>
-      </c>
-      <c r="F11" s="40" t="s">
-        <v>196</v>
-      </c>
-      <c r="G11" s="33" t="s">
-        <v>197</v>
       </c>
       <c r="H11" s="34"/>
       <c r="I11" s="35" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="J11" s="28"/>
       <c r="K11" s="28"/>
@@ -5089,31 +5102,31 @@
       <c r="Y11" s="28"/>
       <c r="Z11" s="28"/>
     </row>
-    <row r="12" ht="14.25" customHeight="1">
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="29" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B12" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="E12" s="39" t="s">
         <v>129</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="F12" s="32" t="s">
         <v>130</v>
       </c>
-      <c r="D12" s="30" t="s">
-        <v>131</v>
-      </c>
-      <c r="E12" s="39" t="s">
-        <v>132</v>
-      </c>
-      <c r="F12" s="32" t="s">
-        <v>133</v>
-      </c>
       <c r="G12" s="33" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="H12" s="34"/>
       <c r="I12" s="35" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J12" s="28"/>
       <c r="K12" s="28"/>
@@ -5133,31 +5146,31 @@
       <c r="Y12" s="28"/>
       <c r="Z12" s="28"/>
     </row>
-    <row r="13" ht="14.25" customHeight="1">
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="29" t="s">
+        <v>196</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="D13" s="30" t="s">
         <v>199</v>
       </c>
-      <c r="B13" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="C13" s="29" t="s">
+      <c r="E13" s="39" t="s">
+        <v>200</v>
+      </c>
+      <c r="F13" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="D13" s="30" t="s">
+      <c r="G13" s="33" t="s">
         <v>202</v>
-      </c>
-      <c r="E13" s="39" t="s">
-        <v>203</v>
-      </c>
-      <c r="F13" s="32" t="s">
-        <v>204</v>
-      </c>
-      <c r="G13" s="33" t="s">
-        <v>205</v>
       </c>
       <c r="H13" s="34"/>
       <c r="I13" s="35" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="K13" s="28"/>
       <c r="L13" s="28"/>
@@ -5176,31 +5189,31 @@
       <c r="Y13" s="28"/>
       <c r="Z13" s="28"/>
     </row>
-    <row r="14" ht="14.25" customHeight="1">
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="28" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B14" s="36" t="s">
+        <v>204</v>
+      </c>
+      <c r="C14" s="37" t="s">
+        <v>205</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>206</v>
+      </c>
+      <c r="E14" s="39" t="s">
         <v>207</v>
       </c>
-      <c r="C14" s="37" t="s">
+      <c r="F14" s="32" t="s">
         <v>208</v>
       </c>
-      <c r="D14" s="30" t="s">
+      <c r="G14" s="33" t="s">
         <v>209</v>
-      </c>
-      <c r="E14" s="39" t="s">
-        <v>210</v>
-      </c>
-      <c r="F14" s="32" t="s">
-        <v>211</v>
-      </c>
-      <c r="G14" s="33" t="s">
-        <v>212</v>
       </c>
       <c r="H14" s="34"/>
       <c r="I14" s="35" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="J14" s="28"/>
       <c r="K14" s="28"/>
@@ -5220,31 +5233,31 @@
       <c r="Y14" s="28"/>
       <c r="Z14" s="28"/>
     </row>
-    <row r="15" ht="14.25" customHeight="1">
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="28" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B15" s="36" t="s">
+        <v>211</v>
+      </c>
+      <c r="C15" s="37" t="s">
+        <v>212</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>213</v>
+      </c>
+      <c r="E15" s="39" t="s">
         <v>214</v>
       </c>
-      <c r="C15" s="37" t="s">
+      <c r="F15" s="32" t="s">
         <v>215</v>
       </c>
-      <c r="D15" s="30" t="s">
+      <c r="G15" s="33" t="s">
         <v>216</v>
-      </c>
-      <c r="E15" s="39" t="s">
-        <v>217</v>
-      </c>
-      <c r="F15" s="32" t="s">
-        <v>218</v>
-      </c>
-      <c r="G15" s="33" t="s">
-        <v>219</v>
       </c>
       <c r="H15" s="34"/>
       <c r="I15" s="35" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="J15" s="28"/>
       <c r="K15" s="28"/>
@@ -5264,31 +5277,31 @@
       <c r="Y15" s="28"/>
       <c r="Z15" s="28"/>
     </row>
-    <row r="16" ht="14.25" customHeight="1">
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="28" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B16" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="C16" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>220</v>
+      </c>
+      <c r="E16" s="39" t="s">
         <v>221</v>
       </c>
-      <c r="C16" s="37" t="s">
+      <c r="F16" s="32" t="s">
         <v>222</v>
       </c>
-      <c r="D16" s="30" t="s">
-        <v>223</v>
-      </c>
-      <c r="E16" s="39" t="s">
-        <v>224</v>
-      </c>
-      <c r="F16" s="32" t="s">
-        <v>225</v>
-      </c>
       <c r="G16" s="33" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="H16" s="34"/>
       <c r="I16" s="35" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="J16" s="28"/>
       <c r="K16" s="28"/>
@@ -5308,31 +5321,31 @@
       <c r="Y16" s="28"/>
       <c r="Z16" s="28"/>
     </row>
-    <row r="17" ht="14.25" customHeight="1">
+    <row r="17" spans="1:26" ht="14.25" customHeight="1">
       <c r="A17" s="28" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B17" s="36" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C17" s="37" t="s">
+        <v>224</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>225</v>
+      </c>
+      <c r="E17" s="39" t="s">
+        <v>226</v>
+      </c>
+      <c r="F17" s="32" t="s">
         <v>227</v>
       </c>
-      <c r="D17" s="30" t="s">
+      <c r="G17" s="33" t="s">
         <v>228</v>
-      </c>
-      <c r="E17" s="39" t="s">
-        <v>229</v>
-      </c>
-      <c r="F17" s="32" t="s">
-        <v>230</v>
-      </c>
-      <c r="G17" s="33" t="s">
-        <v>231</v>
       </c>
       <c r="H17" s="34"/>
       <c r="I17" s="35" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
@@ -5352,31 +5365,31 @@
       <c r="Y17" s="8"/>
       <c r="Z17" s="8"/>
     </row>
-    <row r="18" ht="14.25" customHeight="1">
+    <row r="18" spans="1:26" ht="14.25" customHeight="1">
       <c r="A18" s="28" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B18" s="36" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C18" s="37" t="s">
+        <v>230</v>
+      </c>
+      <c r="D18" s="30" t="s">
+        <v>231</v>
+      </c>
+      <c r="E18" s="39" t="s">
+        <v>232</v>
+      </c>
+      <c r="F18" s="32" t="s">
         <v>233</v>
       </c>
-      <c r="D18" s="30" t="s">
+      <c r="G18" s="33" t="s">
         <v>234</v>
-      </c>
-      <c r="E18" s="39" t="s">
-        <v>235</v>
-      </c>
-      <c r="F18" s="32" t="s">
-        <v>236</v>
-      </c>
-      <c r="G18" s="33" t="s">
-        <v>237</v>
       </c>
       <c r="H18" s="34"/>
       <c r="I18" s="35" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
@@ -5396,31 +5409,31 @@
       <c r="Y18" s="8"/>
       <c r="Z18" s="8"/>
     </row>
-    <row r="19" ht="14.25" customHeight="1">
+    <row r="19" spans="1:26" ht="14.25" customHeight="1">
       <c r="A19" s="28" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B19" s="36" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C19" s="37" t="s">
+        <v>236</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>237</v>
+      </c>
+      <c r="E19" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="F19" s="32" t="s">
         <v>239</v>
       </c>
-      <c r="D19" s="30" t="s">
+      <c r="G19" s="33" t="s">
         <v>240</v>
-      </c>
-      <c r="E19" s="39" t="s">
-        <v>241</v>
-      </c>
-      <c r="F19" s="32" t="s">
-        <v>242</v>
-      </c>
-      <c r="G19" s="33" t="s">
-        <v>243</v>
       </c>
       <c r="H19" s="34"/>
       <c r="I19" s="35" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
@@ -5440,19 +5453,19 @@
       <c r="Y19" s="8"/>
       <c r="Z19" s="8"/>
     </row>
-    <row r="20" ht="15.75" customHeight="1"/>
-    <row r="21" ht="15.75" customHeight="1"/>
-    <row r="22" ht="15.75" customHeight="1"/>
-    <row r="23" ht="15.75" customHeight="1"/>
-    <row r="24" ht="15.75" customHeight="1"/>
-    <row r="25" ht="15.75" customHeight="1"/>
-    <row r="26" ht="15.75" customHeight="1"/>
-    <row r="27" ht="15.75" customHeight="1"/>
-    <row r="28" ht="15.75" customHeight="1"/>
-    <row r="29" ht="15.75" customHeight="1"/>
-    <row r="30" ht="15.75" customHeight="1"/>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
+    <row r="20" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="21" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="22" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="23" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="24" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="25" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="26" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="27" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="28" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="29" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="30" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="31" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="32" spans="1:26" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -6420,55 +6433,53 @@
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="28.14"/>
-    <col customWidth="1" min="2" max="2" width="12.71"/>
-    <col customWidth="1" min="3" max="3" width="20.14"/>
-    <col customWidth="1" min="4" max="4" width="5.71"/>
-    <col customWidth="1" min="5" max="5" width="14.29"/>
-    <col customWidth="1" min="6" max="6" width="34.0"/>
-    <col customWidth="1" min="7" max="16" width="7.71"/>
-    <col customWidth="1" min="17" max="26" width="15.14"/>
+    <col min="1" max="1" width="28.109375" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" customWidth="1"/>
+    <col min="4" max="4" width="5.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="34" customWidth="1"/>
+    <col min="7" max="16" width="7.6640625" customWidth="1"/>
+    <col min="17" max="26" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
+    <row r="1" spans="1:26" ht="14.25" customHeight="1">
       <c r="A1" s="41" t="s">
+        <v>242</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>243</v>
+      </c>
+      <c r="C1" s="41" t="s">
+        <v>244</v>
+      </c>
+      <c r="D1" s="41" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="E1" s="41" t="s">
         <v>246</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="F1" s="41" t="s">
         <v>247</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="G1" s="41" t="s">
         <v>248</v>
-      </c>
-      <c r="E1" s="41" t="s">
-        <v>249</v>
-      </c>
-      <c r="F1" s="41" t="s">
-        <v>250</v>
-      </c>
-      <c r="G1" s="41" t="s">
-        <v>251</v>
       </c>
       <c r="H1" s="28"/>
       <c r="I1" s="28"/>
@@ -6490,24 +6501,24 @@
       <c r="Y1" s="28"/>
       <c r="Z1" s="28"/>
     </row>
-    <row r="2" ht="14.25" customHeight="1">
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="28" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C2" s="42" t="str">
-        <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2021-08-18_00-07</v>
+        <f ca="1">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
+        <v>2025-05-01 23-04</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F2" s="28"/>
       <c r="G2" s="28" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="H2" s="28"/>
       <c r="I2" s="28"/>
@@ -6529,7 +6540,7 @@
       <c r="Y2" s="28"/>
       <c r="Z2" s="28"/>
     </row>
-    <row r="3" ht="14.25" customHeight="1">
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="28"/>
       <c r="B3" s="28"/>
       <c r="C3" s="28"/>
@@ -6557,7 +6568,7 @@
       <c r="Y3" s="28"/>
       <c r="Z3" s="28"/>
     </row>
-    <row r="4" ht="14.25" customHeight="1">
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="28"/>
       <c r="B4" s="28"/>
       <c r="C4" s="28"/>
@@ -6585,7 +6596,7 @@
       <c r="Y4" s="28"/>
       <c r="Z4" s="28"/>
     </row>
-    <row r="5" ht="14.25" customHeight="1">
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" s="28"/>
       <c r="B5" s="28"/>
       <c r="C5" s="28"/>
@@ -6613,7 +6624,7 @@
       <c r="Y5" s="28"/>
       <c r="Z5" s="28"/>
     </row>
-    <row r="6" ht="14.25" customHeight="1">
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="28"/>
       <c r="B6" s="28"/>
       <c r="C6" s="28"/>
@@ -6641,7 +6652,7 @@
       <c r="Y6" s="28"/>
       <c r="Z6" s="28"/>
     </row>
-    <row r="7" ht="14.25" customHeight="1">
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="28"/>
       <c r="B7" s="28"/>
       <c r="C7" s="28"/>
@@ -6669,7 +6680,7 @@
       <c r="Y7" s="28"/>
       <c r="Z7" s="28"/>
     </row>
-    <row r="8" ht="14.25" customHeight="1">
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="28"/>
       <c r="B8" s="28"/>
       <c r="C8" s="28"/>
@@ -6697,7 +6708,7 @@
       <c r="Y8" s="28"/>
       <c r="Z8" s="28"/>
     </row>
-    <row r="9" ht="14.25" customHeight="1">
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="28"/>
       <c r="B9" s="28"/>
       <c r="C9" s="28"/>
@@ -6725,7 +6736,7 @@
       <c r="Y9" s="28"/>
       <c r="Z9" s="28"/>
     </row>
-    <row r="10" ht="14.25" customHeight="1">
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="28"/>
       <c r="B10" s="28"/>
       <c r="C10" s="28"/>
@@ -6753,7 +6764,7 @@
       <c r="Y10" s="28"/>
       <c r="Z10" s="28"/>
     </row>
-    <row r="11" ht="14.25" customHeight="1">
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="28"/>
       <c r="B11" s="28"/>
       <c r="C11" s="28"/>
@@ -6781,7 +6792,7 @@
       <c r="Y11" s="28"/>
       <c r="Z11" s="28"/>
     </row>
-    <row r="12" ht="14.25" customHeight="1">
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="28"/>
       <c r="B12" s="28"/>
       <c r="C12" s="28"/>
@@ -6809,7 +6820,7 @@
       <c r="Y12" s="28"/>
       <c r="Z12" s="28"/>
     </row>
-    <row r="13" ht="14.25" customHeight="1">
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="28"/>
       <c r="B13" s="28"/>
       <c r="C13" s="28"/>
@@ -6837,7 +6848,7 @@
       <c r="Y13" s="28"/>
       <c r="Z13" s="28"/>
     </row>
-    <row r="14" ht="14.25" customHeight="1">
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="28"/>
       <c r="B14" s="28"/>
       <c r="C14" s="28"/>
@@ -6865,7 +6876,7 @@
       <c r="Y14" s="28"/>
       <c r="Z14" s="28"/>
     </row>
-    <row r="15" ht="14.25" customHeight="1">
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="28"/>
       <c r="B15" s="28"/>
       <c r="C15" s="28"/>
@@ -6893,7 +6904,7 @@
       <c r="Y15" s="28"/>
       <c r="Z15" s="28"/>
     </row>
-    <row r="16" ht="14.25" customHeight="1">
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="28"/>
       <c r="B16" s="28"/>
       <c r="C16" s="28"/>
@@ -6921,7 +6932,7 @@
       <c r="Y16" s="28"/>
       <c r="Z16" s="28"/>
     </row>
-    <row r="17" ht="14.25" customHeight="1">
+    <row r="17" spans="1:26" ht="14.25" customHeight="1">
       <c r="A17" s="28"/>
       <c r="B17" s="28"/>
       <c r="C17" s="28"/>
@@ -6949,7 +6960,7 @@
       <c r="Y17" s="28"/>
       <c r="Z17" s="28"/>
     </row>
-    <row r="18" ht="14.25" customHeight="1">
+    <row r="18" spans="1:26" ht="14.25" customHeight="1">
       <c r="A18" s="28"/>
       <c r="B18" s="28"/>
       <c r="C18" s="28"/>
@@ -6977,7 +6988,7 @@
       <c r="Y18" s="28"/>
       <c r="Z18" s="28"/>
     </row>
-    <row r="19" ht="14.25" customHeight="1">
+    <row r="19" spans="1:26" ht="14.25" customHeight="1">
       <c r="A19" s="28"/>
       <c r="B19" s="28"/>
       <c r="C19" s="28"/>
@@ -7005,7 +7016,7 @@
       <c r="Y19" s="28"/>
       <c r="Z19" s="28"/>
     </row>
-    <row r="20" ht="14.25" customHeight="1">
+    <row r="20" spans="1:26" ht="14.25" customHeight="1">
       <c r="A20" s="28"/>
       <c r="B20" s="28"/>
       <c r="C20" s="28"/>
@@ -7033,7 +7044,7 @@
       <c r="Y20" s="28"/>
       <c r="Z20" s="28"/>
     </row>
-    <row r="21" ht="14.25" customHeight="1">
+    <row r="21" spans="1:26" ht="14.25" customHeight="1">
       <c r="A21" s="28"/>
       <c r="B21" s="28"/>
       <c r="C21" s="28"/>
@@ -7061,7 +7072,7 @@
       <c r="Y21" s="28"/>
       <c r="Z21" s="28"/>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
+    <row r="22" spans="1:26" ht="15.75" customHeight="1">
       <c r="A22" s="28"/>
       <c r="B22" s="28"/>
       <c r="C22" s="28"/>
@@ -7089,7 +7100,7 @@
       <c r="Y22" s="28"/>
       <c r="Z22" s="28"/>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
+    <row r="23" spans="1:26" ht="15.75" customHeight="1">
       <c r="A23" s="28"/>
       <c r="B23" s="28"/>
       <c r="C23" s="28"/>
@@ -7117,7 +7128,7 @@
       <c r="Y23" s="28"/>
       <c r="Z23" s="28"/>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
+    <row r="24" spans="1:26" ht="15.75" customHeight="1">
       <c r="A24" s="28"/>
       <c r="B24" s="28"/>
       <c r="C24" s="28"/>
@@ -7145,7 +7156,7 @@
       <c r="Y24" s="28"/>
       <c r="Z24" s="28"/>
     </row>
-    <row r="25" ht="15.75" customHeight="1">
+    <row r="25" spans="1:26" ht="15.75" customHeight="1">
       <c r="A25" s="28"/>
       <c r="B25" s="28"/>
       <c r="C25" s="28"/>
@@ -7173,7 +7184,7 @@
       <c r="Y25" s="28"/>
       <c r="Z25" s="28"/>
     </row>
-    <row r="26" ht="15.75" customHeight="1">
+    <row r="26" spans="1:26" ht="15.75" customHeight="1">
       <c r="A26" s="28"/>
       <c r="B26" s="28"/>
       <c r="C26" s="28"/>
@@ -7201,7 +7212,7 @@
       <c r="Y26" s="28"/>
       <c r="Z26" s="28"/>
     </row>
-    <row r="27" ht="15.75" customHeight="1">
+    <row r="27" spans="1:26" ht="15.75" customHeight="1">
       <c r="A27" s="28"/>
       <c r="B27" s="28"/>
       <c r="C27" s="28"/>
@@ -7229,7 +7240,7 @@
       <c r="Y27" s="28"/>
       <c r="Z27" s="28"/>
     </row>
-    <row r="28" ht="15.75" customHeight="1">
+    <row r="28" spans="1:26" ht="15.75" customHeight="1">
       <c r="A28" s="28"/>
       <c r="B28" s="28"/>
       <c r="C28" s="28"/>
@@ -7257,7 +7268,7 @@
       <c r="Y28" s="28"/>
       <c r="Z28" s="28"/>
     </row>
-    <row r="29" ht="15.75" customHeight="1">
+    <row r="29" spans="1:26" ht="15.75" customHeight="1">
       <c r="A29" s="28"/>
       <c r="B29" s="28"/>
       <c r="C29" s="28"/>
@@ -7285,7 +7296,7 @@
       <c r="Y29" s="28"/>
       <c r="Z29" s="28"/>
     </row>
-    <row r="30" ht="15.75" customHeight="1">
+    <row r="30" spans="1:26" ht="15.75" customHeight="1">
       <c r="A30" s="28"/>
       <c r="B30" s="28"/>
       <c r="C30" s="28"/>
@@ -7313,7 +7324,7 @@
       <c r="Y30" s="28"/>
       <c r="Z30" s="28"/>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
+    <row r="31" spans="1:26" ht="15.75" customHeight="1">
       <c r="A31" s="28"/>
       <c r="B31" s="28"/>
       <c r="C31" s="28"/>
@@ -7341,7 +7352,7 @@
       <c r="Y31" s="28"/>
       <c r="Z31" s="28"/>
     </row>
-    <row r="32" ht="15.75" customHeight="1">
+    <row r="32" spans="1:26" ht="15.75" customHeight="1">
       <c r="A32" s="28"/>
       <c r="B32" s="28"/>
       <c r="C32" s="28"/>
@@ -7369,7 +7380,7 @@
       <c r="Y32" s="28"/>
       <c r="Z32" s="28"/>
     </row>
-    <row r="33" ht="15.75" customHeight="1">
+    <row r="33" spans="1:26" ht="15.75" customHeight="1">
       <c r="A33" s="28"/>
       <c r="B33" s="28"/>
       <c r="C33" s="28"/>
@@ -7397,7 +7408,7 @@
       <c r="Y33" s="28"/>
       <c r="Z33" s="28"/>
     </row>
-    <row r="34" ht="15.75" customHeight="1">
+    <row r="34" spans="1:26" ht="15.75" customHeight="1">
       <c r="A34" s="28"/>
       <c r="B34" s="28"/>
       <c r="C34" s="28"/>
@@ -7425,7 +7436,7 @@
       <c r="Y34" s="28"/>
       <c r="Z34" s="28"/>
     </row>
-    <row r="35" ht="15.75" customHeight="1">
+    <row r="35" spans="1:26" ht="15.75" customHeight="1">
       <c r="A35" s="28"/>
       <c r="B35" s="28"/>
       <c r="C35" s="28"/>
@@ -7453,7 +7464,7 @@
       <c r="Y35" s="28"/>
       <c r="Z35" s="28"/>
     </row>
-    <row r="36" ht="15.75" customHeight="1">
+    <row r="36" spans="1:26" ht="15.75" customHeight="1">
       <c r="A36" s="28"/>
       <c r="B36" s="28"/>
       <c r="C36" s="28"/>
@@ -7481,7 +7492,7 @@
       <c r="Y36" s="28"/>
       <c r="Z36" s="28"/>
     </row>
-    <row r="37" ht="15.75" customHeight="1">
+    <row r="37" spans="1:26" ht="15.75" customHeight="1">
       <c r="A37" s="28"/>
       <c r="B37" s="28"/>
       <c r="C37" s="28"/>
@@ -7509,7 +7520,7 @@
       <c r="Y37" s="28"/>
       <c r="Z37" s="28"/>
     </row>
-    <row r="38" ht="15.75" customHeight="1">
+    <row r="38" spans="1:26" ht="15.75" customHeight="1">
       <c r="A38" s="28"/>
       <c r="B38" s="28"/>
       <c r="C38" s="28"/>
@@ -7537,7 +7548,7 @@
       <c r="Y38" s="28"/>
       <c r="Z38" s="28"/>
     </row>
-    <row r="39" ht="15.75" customHeight="1">
+    <row r="39" spans="1:26" ht="15.75" customHeight="1">
       <c r="A39" s="28"/>
       <c r="B39" s="28"/>
       <c r="C39" s="28"/>
@@ -7565,7 +7576,7 @@
       <c r="Y39" s="28"/>
       <c r="Z39" s="28"/>
     </row>
-    <row r="40" ht="15.75" customHeight="1">
+    <row r="40" spans="1:26" ht="15.75" customHeight="1">
       <c r="A40" s="28"/>
       <c r="B40" s="28"/>
       <c r="C40" s="28"/>
@@ -7593,7 +7604,7 @@
       <c r="Y40" s="28"/>
       <c r="Z40" s="28"/>
     </row>
-    <row r="41" ht="15.75" customHeight="1">
+    <row r="41" spans="1:26" ht="15.75" customHeight="1">
       <c r="A41" s="28"/>
       <c r="B41" s="28"/>
       <c r="C41" s="28"/>
@@ -7621,7 +7632,7 @@
       <c r="Y41" s="28"/>
       <c r="Z41" s="28"/>
     </row>
-    <row r="42" ht="15.75" customHeight="1">
+    <row r="42" spans="1:26" ht="15.75" customHeight="1">
       <c r="A42" s="28"/>
       <c r="B42" s="28"/>
       <c r="C42" s="28"/>
@@ -7649,7 +7660,7 @@
       <c r="Y42" s="28"/>
       <c r="Z42" s="28"/>
     </row>
-    <row r="43" ht="15.75" customHeight="1">
+    <row r="43" spans="1:26" ht="15.75" customHeight="1">
       <c r="A43" s="28"/>
       <c r="B43" s="28"/>
       <c r="C43" s="28"/>
@@ -7677,7 +7688,7 @@
       <c r="Y43" s="28"/>
       <c r="Z43" s="28"/>
     </row>
-    <row r="44" ht="15.75" customHeight="1">
+    <row r="44" spans="1:26" ht="15.75" customHeight="1">
       <c r="A44" s="28"/>
       <c r="B44" s="28"/>
       <c r="C44" s="28"/>
@@ -7705,7 +7716,7 @@
       <c r="Y44" s="28"/>
       <c r="Z44" s="28"/>
     </row>
-    <row r="45" ht="15.75" customHeight="1">
+    <row r="45" spans="1:26" ht="15.75" customHeight="1">
       <c r="A45" s="28"/>
       <c r="B45" s="28"/>
       <c r="C45" s="28"/>
@@ -7733,7 +7744,7 @@
       <c r="Y45" s="28"/>
       <c r="Z45" s="28"/>
     </row>
-    <row r="46" ht="15.75" customHeight="1">
+    <row r="46" spans="1:26" ht="15.75" customHeight="1">
       <c r="A46" s="28"/>
       <c r="B46" s="28"/>
       <c r="C46" s="28"/>
@@ -7761,7 +7772,7 @@
       <c r="Y46" s="28"/>
       <c r="Z46" s="28"/>
     </row>
-    <row r="47" ht="15.75" customHeight="1">
+    <row r="47" spans="1:26" ht="15.75" customHeight="1">
       <c r="A47" s="28"/>
       <c r="B47" s="28"/>
       <c r="C47" s="28"/>
@@ -7789,7 +7800,7 @@
       <c r="Y47" s="28"/>
       <c r="Z47" s="28"/>
     </row>
-    <row r="48" ht="15.75" customHeight="1">
+    <row r="48" spans="1:26" ht="15.75" customHeight="1">
       <c r="A48" s="28"/>
       <c r="B48" s="28"/>
       <c r="C48" s="28"/>
@@ -7817,7 +7828,7 @@
       <c r="Y48" s="28"/>
       <c r="Z48" s="28"/>
     </row>
-    <row r="49" ht="15.75" customHeight="1">
+    <row r="49" spans="1:26" ht="15.75" customHeight="1">
       <c r="A49" s="28"/>
       <c r="B49" s="28"/>
       <c r="C49" s="28"/>
@@ -7845,7 +7856,7 @@
       <c r="Y49" s="28"/>
       <c r="Z49" s="28"/>
     </row>
-    <row r="50" ht="15.75" customHeight="1">
+    <row r="50" spans="1:26" ht="15.75" customHeight="1">
       <c r="A50" s="28"/>
       <c r="B50" s="28"/>
       <c r="C50" s="28"/>
@@ -7873,7 +7884,7 @@
       <c r="Y50" s="28"/>
       <c r="Z50" s="28"/>
     </row>
-    <row r="51" ht="15.75" customHeight="1">
+    <row r="51" spans="1:26" ht="15.75" customHeight="1">
       <c r="A51" s="28"/>
       <c r="B51" s="28"/>
       <c r="C51" s="28"/>
@@ -7901,7 +7912,7 @@
       <c r="Y51" s="28"/>
       <c r="Z51" s="28"/>
     </row>
-    <row r="52" ht="15.75" customHeight="1">
+    <row r="52" spans="1:26" ht="15.75" customHeight="1">
       <c r="A52" s="28"/>
       <c r="B52" s="28"/>
       <c r="C52" s="28"/>
@@ -7929,7 +7940,7 @@
       <c r="Y52" s="28"/>
       <c r="Z52" s="28"/>
     </row>
-    <row r="53" ht="15.75" customHeight="1">
+    <row r="53" spans="1:26" ht="15.75" customHeight="1">
       <c r="A53" s="28"/>
       <c r="B53" s="28"/>
       <c r="C53" s="28"/>
@@ -7957,7 +7968,7 @@
       <c r="Y53" s="28"/>
       <c r="Z53" s="28"/>
     </row>
-    <row r="54" ht="15.75" customHeight="1">
+    <row r="54" spans="1:26" ht="15.75" customHeight="1">
       <c r="A54" s="28"/>
       <c r="B54" s="28"/>
       <c r="C54" s="28"/>
@@ -7985,7 +7996,7 @@
       <c r="Y54" s="28"/>
       <c r="Z54" s="28"/>
     </row>
-    <row r="55" ht="15.75" customHeight="1">
+    <row r="55" spans="1:26" ht="15.75" customHeight="1">
       <c r="A55" s="28"/>
       <c r="B55" s="28"/>
       <c r="C55" s="28"/>
@@ -8013,7 +8024,7 @@
       <c r="Y55" s="28"/>
       <c r="Z55" s="28"/>
     </row>
-    <row r="56" ht="15.75" customHeight="1">
+    <row r="56" spans="1:26" ht="15.75" customHeight="1">
       <c r="A56" s="28"/>
       <c r="B56" s="28"/>
       <c r="C56" s="28"/>
@@ -8041,7 +8052,7 @@
       <c r="Y56" s="28"/>
       <c r="Z56" s="28"/>
     </row>
-    <row r="57" ht="15.75" customHeight="1">
+    <row r="57" spans="1:26" ht="15.75" customHeight="1">
       <c r="A57" s="28"/>
       <c r="B57" s="28"/>
       <c r="C57" s="28"/>
@@ -8069,7 +8080,7 @@
       <c r="Y57" s="28"/>
       <c r="Z57" s="28"/>
     </row>
-    <row r="58" ht="15.75" customHeight="1">
+    <row r="58" spans="1:26" ht="15.75" customHeight="1">
       <c r="A58" s="28"/>
       <c r="B58" s="28"/>
       <c r="C58" s="28"/>
@@ -8097,7 +8108,7 @@
       <c r="Y58" s="28"/>
       <c r="Z58" s="28"/>
     </row>
-    <row r="59" ht="15.75" customHeight="1">
+    <row r="59" spans="1:26" ht="15.75" customHeight="1">
       <c r="A59" s="28"/>
       <c r="B59" s="28"/>
       <c r="C59" s="28"/>
@@ -8125,7 +8136,7 @@
       <c r="Y59" s="28"/>
       <c r="Z59" s="28"/>
     </row>
-    <row r="60" ht="15.75" customHeight="1">
+    <row r="60" spans="1:26" ht="15.75" customHeight="1">
       <c r="A60" s="28"/>
       <c r="B60" s="28"/>
       <c r="C60" s="28"/>
@@ -8153,7 +8164,7 @@
       <c r="Y60" s="28"/>
       <c r="Z60" s="28"/>
     </row>
-    <row r="61" ht="15.75" customHeight="1">
+    <row r="61" spans="1:26" ht="15.75" customHeight="1">
       <c r="A61" s="28"/>
       <c r="B61" s="28"/>
       <c r="C61" s="28"/>
@@ -8181,7 +8192,7 @@
       <c r="Y61" s="28"/>
       <c r="Z61" s="28"/>
     </row>
-    <row r="62" ht="15.75" customHeight="1">
+    <row r="62" spans="1:26" ht="15.75" customHeight="1">
       <c r="A62" s="28"/>
       <c r="B62" s="28"/>
       <c r="C62" s="28"/>
@@ -8209,7 +8220,7 @@
       <c r="Y62" s="28"/>
       <c r="Z62" s="28"/>
     </row>
-    <row r="63" ht="15.75" customHeight="1">
+    <row r="63" spans="1:26" ht="15.75" customHeight="1">
       <c r="A63" s="28"/>
       <c r="B63" s="28"/>
       <c r="C63" s="28"/>
@@ -8237,7 +8248,7 @@
       <c r="Y63" s="28"/>
       <c r="Z63" s="28"/>
     </row>
-    <row r="64" ht="15.75" customHeight="1">
+    <row r="64" spans="1:26" ht="15.75" customHeight="1">
       <c r="A64" s="28"/>
       <c r="B64" s="28"/>
       <c r="C64" s="28"/>
@@ -8265,7 +8276,7 @@
       <c r="Y64" s="28"/>
       <c r="Z64" s="28"/>
     </row>
-    <row r="65" ht="15.75" customHeight="1">
+    <row r="65" spans="1:26" ht="15.75" customHeight="1">
       <c r="A65" s="28"/>
       <c r="B65" s="28"/>
       <c r="C65" s="28"/>
@@ -8293,7 +8304,7 @@
       <c r="Y65" s="28"/>
       <c r="Z65" s="28"/>
     </row>
-    <row r="66" ht="15.75" customHeight="1">
+    <row r="66" spans="1:26" ht="15.75" customHeight="1">
       <c r="A66" s="28"/>
       <c r="B66" s="28"/>
       <c r="C66" s="28"/>
@@ -8321,7 +8332,7 @@
       <c r="Y66" s="28"/>
       <c r="Z66" s="28"/>
     </row>
-    <row r="67" ht="15.75" customHeight="1">
+    <row r="67" spans="1:26" ht="15.75" customHeight="1">
       <c r="A67" s="28"/>
       <c r="B67" s="28"/>
       <c r="C67" s="28"/>
@@ -8349,7 +8360,7 @@
       <c r="Y67" s="28"/>
       <c r="Z67" s="28"/>
     </row>
-    <row r="68" ht="15.75" customHeight="1">
+    <row r="68" spans="1:26" ht="15.75" customHeight="1">
       <c r="A68" s="28"/>
       <c r="B68" s="28"/>
       <c r="C68" s="28"/>
@@ -8377,7 +8388,7 @@
       <c r="Y68" s="28"/>
       <c r="Z68" s="28"/>
     </row>
-    <row r="69" ht="15.75" customHeight="1">
+    <row r="69" spans="1:26" ht="15.75" customHeight="1">
       <c r="A69" s="28"/>
       <c r="B69" s="28"/>
       <c r="C69" s="28"/>
@@ -8405,7 +8416,7 @@
       <c r="Y69" s="28"/>
       <c r="Z69" s="28"/>
     </row>
-    <row r="70" ht="15.75" customHeight="1">
+    <row r="70" spans="1:26" ht="15.75" customHeight="1">
       <c r="A70" s="28"/>
       <c r="B70" s="28"/>
       <c r="C70" s="28"/>
@@ -8433,7 +8444,7 @@
       <c r="Y70" s="28"/>
       <c r="Z70" s="28"/>
     </row>
-    <row r="71" ht="15.75" customHeight="1">
+    <row r="71" spans="1:26" ht="15.75" customHeight="1">
       <c r="A71" s="28"/>
       <c r="B71" s="28"/>
       <c r="C71" s="28"/>
@@ -8461,7 +8472,7 @@
       <c r="Y71" s="28"/>
       <c r="Z71" s="28"/>
     </row>
-    <row r="72" ht="15.75" customHeight="1">
+    <row r="72" spans="1:26" ht="15.75" customHeight="1">
       <c r="A72" s="28"/>
       <c r="B72" s="28"/>
       <c r="C72" s="28"/>
@@ -8489,7 +8500,7 @@
       <c r="Y72" s="28"/>
       <c r="Z72" s="28"/>
     </row>
-    <row r="73" ht="15.75" customHeight="1">
+    <row r="73" spans="1:26" ht="15.75" customHeight="1">
       <c r="A73" s="28"/>
       <c r="B73" s="28"/>
       <c r="C73" s="28"/>
@@ -8517,7 +8528,7 @@
       <c r="Y73" s="28"/>
       <c r="Z73" s="28"/>
     </row>
-    <row r="74" ht="15.75" customHeight="1">
+    <row r="74" spans="1:26" ht="15.75" customHeight="1">
       <c r="A74" s="28"/>
       <c r="B74" s="28"/>
       <c r="C74" s="28"/>
@@ -8545,7 +8556,7 @@
       <c r="Y74" s="28"/>
       <c r="Z74" s="28"/>
     </row>
-    <row r="75" ht="15.75" customHeight="1">
+    <row r="75" spans="1:26" ht="15.75" customHeight="1">
       <c r="A75" s="28"/>
       <c r="B75" s="28"/>
       <c r="C75" s="28"/>
@@ -8573,7 +8584,7 @@
       <c r="Y75" s="28"/>
       <c r="Z75" s="28"/>
     </row>
-    <row r="76" ht="15.75" customHeight="1">
+    <row r="76" spans="1:26" ht="15.75" customHeight="1">
       <c r="A76" s="28"/>
       <c r="B76" s="28"/>
       <c r="C76" s="28"/>
@@ -8601,7 +8612,7 @@
       <c r="Y76" s="28"/>
       <c r="Z76" s="28"/>
     </row>
-    <row r="77" ht="15.75" customHeight="1">
+    <row r="77" spans="1:26" ht="15.75" customHeight="1">
       <c r="A77" s="28"/>
       <c r="B77" s="28"/>
       <c r="C77" s="28"/>
@@ -8629,7 +8640,7 @@
       <c r="Y77" s="28"/>
       <c r="Z77" s="28"/>
     </row>
-    <row r="78" ht="15.75" customHeight="1">
+    <row r="78" spans="1:26" ht="15.75" customHeight="1">
       <c r="A78" s="28"/>
       <c r="B78" s="28"/>
       <c r="C78" s="28"/>
@@ -8657,7 +8668,7 @@
       <c r="Y78" s="28"/>
       <c r="Z78" s="28"/>
     </row>
-    <row r="79" ht="15.75" customHeight="1">
+    <row r="79" spans="1:26" ht="15.75" customHeight="1">
       <c r="A79" s="28"/>
       <c r="B79" s="28"/>
       <c r="C79" s="28"/>
@@ -8685,7 +8696,7 @@
       <c r="Y79" s="28"/>
       <c r="Z79" s="28"/>
     </row>
-    <row r="80" ht="15.75" customHeight="1">
+    <row r="80" spans="1:26" ht="15.75" customHeight="1">
       <c r="A80" s="28"/>
       <c r="B80" s="28"/>
       <c r="C80" s="28"/>
@@ -8713,7 +8724,7 @@
       <c r="Y80" s="28"/>
       <c r="Z80" s="28"/>
     </row>
-    <row r="81" ht="15.75" customHeight="1">
+    <row r="81" spans="1:26" ht="15.75" customHeight="1">
       <c r="A81" s="28"/>
       <c r="B81" s="28"/>
       <c r="C81" s="28"/>
@@ -8741,7 +8752,7 @@
       <c r="Y81" s="28"/>
       <c r="Z81" s="28"/>
     </row>
-    <row r="82" ht="15.75" customHeight="1">
+    <row r="82" spans="1:26" ht="15.75" customHeight="1">
       <c r="A82" s="28"/>
       <c r="B82" s="28"/>
       <c r="C82" s="28"/>
@@ -8769,7 +8780,7 @@
       <c r="Y82" s="28"/>
       <c r="Z82" s="28"/>
     </row>
-    <row r="83" ht="15.75" customHeight="1">
+    <row r="83" spans="1:26" ht="15.75" customHeight="1">
       <c r="A83" s="28"/>
       <c r="B83" s="28"/>
       <c r="C83" s="28"/>
@@ -8797,7 +8808,7 @@
       <c r="Y83" s="28"/>
       <c r="Z83" s="28"/>
     </row>
-    <row r="84" ht="15.75" customHeight="1">
+    <row r="84" spans="1:26" ht="15.75" customHeight="1">
       <c r="A84" s="28"/>
       <c r="B84" s="28"/>
       <c r="C84" s="28"/>
@@ -8825,7 +8836,7 @@
       <c r="Y84" s="28"/>
       <c r="Z84" s="28"/>
     </row>
-    <row r="85" ht="15.75" customHeight="1">
+    <row r="85" spans="1:26" ht="15.75" customHeight="1">
       <c r="A85" s="28"/>
       <c r="B85" s="28"/>
       <c r="C85" s="28"/>
@@ -8853,7 +8864,7 @@
       <c r="Y85" s="28"/>
       <c r="Z85" s="28"/>
     </row>
-    <row r="86" ht="15.75" customHeight="1">
+    <row r="86" spans="1:26" ht="15.75" customHeight="1">
       <c r="A86" s="28"/>
       <c r="B86" s="28"/>
       <c r="C86" s="28"/>
@@ -8881,7 +8892,7 @@
       <c r="Y86" s="28"/>
       <c r="Z86" s="28"/>
     </row>
-    <row r="87" ht="15.75" customHeight="1">
+    <row r="87" spans="1:26" ht="15.75" customHeight="1">
       <c r="A87" s="28"/>
       <c r="B87" s="28"/>
       <c r="C87" s="28"/>
@@ -8909,7 +8920,7 @@
       <c r="Y87" s="28"/>
       <c r="Z87" s="28"/>
     </row>
-    <row r="88" ht="15.75" customHeight="1">
+    <row r="88" spans="1:26" ht="15.75" customHeight="1">
       <c r="A88" s="28"/>
       <c r="B88" s="28"/>
       <c r="C88" s="28"/>
@@ -8937,7 +8948,7 @@
       <c r="Y88" s="28"/>
       <c r="Z88" s="28"/>
     </row>
-    <row r="89" ht="15.75" customHeight="1">
+    <row r="89" spans="1:26" ht="15.75" customHeight="1">
       <c r="A89" s="28"/>
       <c r="B89" s="28"/>
       <c r="C89" s="28"/>
@@ -8965,7 +8976,7 @@
       <c r="Y89" s="28"/>
       <c r="Z89" s="28"/>
     </row>
-    <row r="90" ht="15.75" customHeight="1">
+    <row r="90" spans="1:26" ht="15.75" customHeight="1">
       <c r="A90" s="28"/>
       <c r="B90" s="28"/>
       <c r="C90" s="28"/>
@@ -8993,7 +9004,7 @@
       <c r="Y90" s="28"/>
       <c r="Z90" s="28"/>
     </row>
-    <row r="91" ht="15.75" customHeight="1">
+    <row r="91" spans="1:26" ht="15.75" customHeight="1">
       <c r="A91" s="28"/>
       <c r="B91" s="28"/>
       <c r="C91" s="28"/>
@@ -9021,7 +9032,7 @@
       <c r="Y91" s="28"/>
       <c r="Z91" s="28"/>
     </row>
-    <row r="92" ht="15.75" customHeight="1">
+    <row r="92" spans="1:26" ht="15.75" customHeight="1">
       <c r="A92" s="28"/>
       <c r="B92" s="28"/>
       <c r="C92" s="28"/>
@@ -9049,7 +9060,7 @@
       <c r="Y92" s="28"/>
       <c r="Z92" s="28"/>
     </row>
-    <row r="93" ht="15.75" customHeight="1">
+    <row r="93" spans="1:26" ht="15.75" customHeight="1">
       <c r="A93" s="28"/>
       <c r="B93" s="28"/>
       <c r="C93" s="28"/>
@@ -9077,7 +9088,7 @@
       <c r="Y93" s="28"/>
       <c r="Z93" s="28"/>
     </row>
-    <row r="94" ht="15.75" customHeight="1">
+    <row r="94" spans="1:26" ht="15.75" customHeight="1">
       <c r="A94" s="28"/>
       <c r="B94" s="28"/>
       <c r="C94" s="28"/>
@@ -9105,7 +9116,7 @@
       <c r="Y94" s="28"/>
       <c r="Z94" s="28"/>
     </row>
-    <row r="95" ht="15.75" customHeight="1">
+    <row r="95" spans="1:26" ht="15.75" customHeight="1">
       <c r="A95" s="28"/>
       <c r="B95" s="28"/>
       <c r="C95" s="28"/>
@@ -9133,7 +9144,7 @@
       <c r="Y95" s="28"/>
       <c r="Z95" s="28"/>
     </row>
-    <row r="96" ht="15.75" customHeight="1">
+    <row r="96" spans="1:26" ht="15.75" customHeight="1">
       <c r="A96" s="28"/>
       <c r="B96" s="28"/>
       <c r="C96" s="28"/>
@@ -9161,7 +9172,7 @@
       <c r="Y96" s="28"/>
       <c r="Z96" s="28"/>
     </row>
-    <row r="97" ht="15.75" customHeight="1">
+    <row r="97" spans="1:26" ht="15.75" customHeight="1">
       <c r="A97" s="28"/>
       <c r="B97" s="28"/>
       <c r="C97" s="28"/>
@@ -9189,7 +9200,7 @@
       <c r="Y97" s="28"/>
       <c r="Z97" s="28"/>
     </row>
-    <row r="98" ht="15.75" customHeight="1">
+    <row r="98" spans="1:26" ht="15.75" customHeight="1">
       <c r="A98" s="28"/>
       <c r="B98" s="28"/>
       <c r="C98" s="28"/>
@@ -9217,7 +9228,7 @@
       <c r="Y98" s="28"/>
       <c r="Z98" s="28"/>
     </row>
-    <row r="99" ht="15.75" customHeight="1">
+    <row r="99" spans="1:26" ht="15.75" customHeight="1">
       <c r="A99" s="28"/>
       <c r="B99" s="28"/>
       <c r="C99" s="28"/>
@@ -9245,7 +9256,7 @@
       <c r="Y99" s="28"/>
       <c r="Z99" s="28"/>
     </row>
-    <row r="100" ht="15.75" customHeight="1">
+    <row r="100" spans="1:26" ht="15.75" customHeight="1">
       <c r="A100" s="28"/>
       <c r="B100" s="28"/>
       <c r="C100" s="28"/>
@@ -9273,7 +9284,7 @@
       <c r="Y100" s="28"/>
       <c r="Z100" s="28"/>
     </row>
-    <row r="101" ht="15.75" customHeight="1">
+    <row r="101" spans="1:26" ht="15.75" customHeight="1">
       <c r="A101" s="28"/>
       <c r="B101" s="28"/>
       <c r="C101" s="28"/>
@@ -9301,7 +9312,7 @@
       <c r="Y101" s="28"/>
       <c r="Z101" s="28"/>
     </row>
-    <row r="102" ht="15.75" customHeight="1">
+    <row r="102" spans="1:26" ht="15.75" customHeight="1">
       <c r="A102" s="28"/>
       <c r="B102" s="28"/>
       <c r="C102" s="28"/>
@@ -9329,7 +9340,7 @@
       <c r="Y102" s="28"/>
       <c r="Z102" s="28"/>
     </row>
-    <row r="103" ht="15.75" customHeight="1">
+    <row r="103" spans="1:26" ht="15.75" customHeight="1">
       <c r="A103" s="28"/>
       <c r="B103" s="28"/>
       <c r="C103" s="28"/>
@@ -9357,7 +9368,7 @@
       <c r="Y103" s="28"/>
       <c r="Z103" s="28"/>
     </row>
-    <row r="104" ht="15.75" customHeight="1">
+    <row r="104" spans="1:26" ht="15.75" customHeight="1">
       <c r="A104" s="28"/>
       <c r="B104" s="28"/>
       <c r="C104" s="28"/>
@@ -9385,7 +9396,7 @@
       <c r="Y104" s="28"/>
       <c r="Z104" s="28"/>
     </row>
-    <row r="105" ht="15.75" customHeight="1">
+    <row r="105" spans="1:26" ht="15.75" customHeight="1">
       <c r="A105" s="28"/>
       <c r="B105" s="28"/>
       <c r="C105" s="28"/>
@@ -9413,7 +9424,7 @@
       <c r="Y105" s="28"/>
       <c r="Z105" s="28"/>
     </row>
-    <row r="106" ht="15.75" customHeight="1">
+    <row r="106" spans="1:26" ht="15.75" customHeight="1">
       <c r="A106" s="28"/>
       <c r="B106" s="28"/>
       <c r="C106" s="28"/>
@@ -9441,7 +9452,7 @@
       <c r="Y106" s="28"/>
       <c r="Z106" s="28"/>
     </row>
-    <row r="107" ht="15.75" customHeight="1">
+    <row r="107" spans="1:26" ht="15.75" customHeight="1">
       <c r="A107" s="28"/>
       <c r="B107" s="28"/>
       <c r="C107" s="28"/>
@@ -9469,7 +9480,7 @@
       <c r="Y107" s="28"/>
       <c r="Z107" s="28"/>
     </row>
-    <row r="108" ht="15.75" customHeight="1">
+    <row r="108" spans="1:26" ht="15.75" customHeight="1">
       <c r="A108" s="28"/>
       <c r="B108" s="28"/>
       <c r="C108" s="28"/>
@@ -9497,7 +9508,7 @@
       <c r="Y108" s="28"/>
       <c r="Z108" s="28"/>
     </row>
-    <row r="109" ht="15.75" customHeight="1">
+    <row r="109" spans="1:26" ht="15.75" customHeight="1">
       <c r="A109" s="28"/>
       <c r="B109" s="28"/>
       <c r="C109" s="28"/>
@@ -9525,7 +9536,7 @@
       <c r="Y109" s="28"/>
       <c r="Z109" s="28"/>
     </row>
-    <row r="110" ht="15.75" customHeight="1">
+    <row r="110" spans="1:26" ht="15.75" customHeight="1">
       <c r="A110" s="28"/>
       <c r="B110" s="28"/>
       <c r="C110" s="28"/>
@@ -9553,7 +9564,7 @@
       <c r="Y110" s="28"/>
       <c r="Z110" s="28"/>
     </row>
-    <row r="111" ht="15.75" customHeight="1">
+    <row r="111" spans="1:26" ht="15.75" customHeight="1">
       <c r="A111" s="28"/>
       <c r="B111" s="28"/>
       <c r="C111" s="28"/>
@@ -9581,7 +9592,7 @@
       <c r="Y111" s="28"/>
       <c r="Z111" s="28"/>
     </row>
-    <row r="112" ht="15.75" customHeight="1">
+    <row r="112" spans="1:26" ht="15.75" customHeight="1">
       <c r="A112" s="28"/>
       <c r="B112" s="28"/>
       <c r="C112" s="28"/>
@@ -9609,7 +9620,7 @@
       <c r="Y112" s="28"/>
       <c r="Z112" s="28"/>
     </row>
-    <row r="113" ht="15.75" customHeight="1">
+    <row r="113" spans="1:26" ht="15.75" customHeight="1">
       <c r="A113" s="28"/>
       <c r="B113" s="28"/>
       <c r="C113" s="28"/>
@@ -9637,7 +9648,7 @@
       <c r="Y113" s="28"/>
       <c r="Z113" s="28"/>
     </row>
-    <row r="114" ht="15.75" customHeight="1">
+    <row r="114" spans="1:26" ht="15.75" customHeight="1">
       <c r="A114" s="28"/>
       <c r="B114" s="28"/>
       <c r="C114" s="28"/>
@@ -9665,7 +9676,7 @@
       <c r="Y114" s="28"/>
       <c r="Z114" s="28"/>
     </row>
-    <row r="115" ht="15.75" customHeight="1">
+    <row r="115" spans="1:26" ht="15.75" customHeight="1">
       <c r="A115" s="28"/>
       <c r="B115" s="28"/>
       <c r="C115" s="28"/>
@@ -9693,7 +9704,7 @@
       <c r="Y115" s="28"/>
       <c r="Z115" s="28"/>
     </row>
-    <row r="116" ht="15.75" customHeight="1">
+    <row r="116" spans="1:26" ht="15.75" customHeight="1">
       <c r="A116" s="28"/>
       <c r="B116" s="28"/>
       <c r="C116" s="28"/>
@@ -9721,7 +9732,7 @@
       <c r="Y116" s="28"/>
       <c r="Z116" s="28"/>
     </row>
-    <row r="117" ht="15.75" customHeight="1">
+    <row r="117" spans="1:26" ht="15.75" customHeight="1">
       <c r="A117" s="28"/>
       <c r="B117" s="28"/>
       <c r="C117" s="28"/>
@@ -9749,7 +9760,7 @@
       <c r="Y117" s="28"/>
       <c r="Z117" s="28"/>
     </row>
-    <row r="118" ht="15.75" customHeight="1">
+    <row r="118" spans="1:26" ht="15.75" customHeight="1">
       <c r="A118" s="28"/>
       <c r="B118" s="28"/>
       <c r="C118" s="28"/>
@@ -9777,7 +9788,7 @@
       <c r="Y118" s="28"/>
       <c r="Z118" s="28"/>
     </row>
-    <row r="119" ht="15.75" customHeight="1">
+    <row r="119" spans="1:26" ht="15.75" customHeight="1">
       <c r="A119" s="28"/>
       <c r="B119" s="28"/>
       <c r="C119" s="28"/>
@@ -9805,7 +9816,7 @@
       <c r="Y119" s="28"/>
       <c r="Z119" s="28"/>
     </row>
-    <row r="120" ht="15.75" customHeight="1">
+    <row r="120" spans="1:26" ht="15.75" customHeight="1">
       <c r="A120" s="28"/>
       <c r="B120" s="28"/>
       <c r="C120" s="28"/>
@@ -9833,7 +9844,7 @@
       <c r="Y120" s="28"/>
       <c r="Z120" s="28"/>
     </row>
-    <row r="121" ht="15.75" customHeight="1">
+    <row r="121" spans="1:26" ht="15.75" customHeight="1">
       <c r="A121" s="28"/>
       <c r="B121" s="28"/>
       <c r="C121" s="28"/>
@@ -9861,7 +9872,7 @@
       <c r="Y121" s="28"/>
       <c r="Z121" s="28"/>
     </row>
-    <row r="122" ht="15.75" customHeight="1">
+    <row r="122" spans="1:26" ht="15.75" customHeight="1">
       <c r="A122" s="28"/>
       <c r="B122" s="28"/>
       <c r="C122" s="28"/>
@@ -9889,7 +9900,7 @@
       <c r="Y122" s="28"/>
       <c r="Z122" s="28"/>
     </row>
-    <row r="123" ht="15.75" customHeight="1">
+    <row r="123" spans="1:26" ht="15.75" customHeight="1">
       <c r="A123" s="28"/>
       <c r="B123" s="28"/>
       <c r="C123" s="28"/>
@@ -9917,7 +9928,7 @@
       <c r="Y123" s="28"/>
       <c r="Z123" s="28"/>
     </row>
-    <row r="124" ht="15.75" customHeight="1">
+    <row r="124" spans="1:26" ht="15.75" customHeight="1">
       <c r="A124" s="28"/>
       <c r="B124" s="28"/>
       <c r="C124" s="28"/>
@@ -9945,7 +9956,7 @@
       <c r="Y124" s="28"/>
       <c r="Z124" s="28"/>
     </row>
-    <row r="125" ht="15.75" customHeight="1">
+    <row r="125" spans="1:26" ht="15.75" customHeight="1">
       <c r="A125" s="28"/>
       <c r="B125" s="28"/>
       <c r="C125" s="28"/>
@@ -9973,7 +9984,7 @@
       <c r="Y125" s="28"/>
       <c r="Z125" s="28"/>
     </row>
-    <row r="126" ht="15.75" customHeight="1">
+    <row r="126" spans="1:26" ht="15.75" customHeight="1">
       <c r="A126" s="28"/>
       <c r="B126" s="28"/>
       <c r="C126" s="28"/>
@@ -10001,7 +10012,7 @@
       <c r="Y126" s="28"/>
       <c r="Z126" s="28"/>
     </row>
-    <row r="127" ht="15.75" customHeight="1">
+    <row r="127" spans="1:26" ht="15.75" customHeight="1">
       <c r="A127" s="28"/>
       <c r="B127" s="28"/>
       <c r="C127" s="28"/>
@@ -10029,7 +10040,7 @@
       <c r="Y127" s="28"/>
       <c r="Z127" s="28"/>
     </row>
-    <row r="128" ht="15.75" customHeight="1">
+    <row r="128" spans="1:26" ht="15.75" customHeight="1">
       <c r="A128" s="28"/>
       <c r="B128" s="28"/>
       <c r="C128" s="28"/>
@@ -10057,7 +10068,7 @@
       <c r="Y128" s="28"/>
       <c r="Z128" s="28"/>
     </row>
-    <row r="129" ht="15.75" customHeight="1">
+    <row r="129" spans="1:26" ht="15.75" customHeight="1">
       <c r="A129" s="28"/>
       <c r="B129" s="28"/>
       <c r="C129" s="28"/>
@@ -10085,7 +10096,7 @@
       <c r="Y129" s="28"/>
       <c r="Z129" s="28"/>
     </row>
-    <row r="130" ht="15.75" customHeight="1">
+    <row r="130" spans="1:26" ht="15.75" customHeight="1">
       <c r="A130" s="28"/>
       <c r="B130" s="28"/>
       <c r="C130" s="28"/>
@@ -10113,7 +10124,7 @@
       <c r="Y130" s="28"/>
       <c r="Z130" s="28"/>
     </row>
-    <row r="131" ht="15.75" customHeight="1">
+    <row r="131" spans="1:26" ht="15.75" customHeight="1">
       <c r="A131" s="28"/>
       <c r="B131" s="28"/>
       <c r="C131" s="28"/>
@@ -10141,7 +10152,7 @@
       <c r="Y131" s="28"/>
       <c r="Z131" s="28"/>
     </row>
-    <row r="132" ht="15.75" customHeight="1">
+    <row r="132" spans="1:26" ht="15.75" customHeight="1">
       <c r="A132" s="28"/>
       <c r="B132" s="28"/>
       <c r="C132" s="28"/>
@@ -10169,7 +10180,7 @@
       <c r="Y132" s="28"/>
       <c r="Z132" s="28"/>
     </row>
-    <row r="133" ht="15.75" customHeight="1">
+    <row r="133" spans="1:26" ht="15.75" customHeight="1">
       <c r="A133" s="28"/>
       <c r="B133" s="28"/>
       <c r="C133" s="28"/>
@@ -10197,7 +10208,7 @@
       <c r="Y133" s="28"/>
       <c r="Z133" s="28"/>
     </row>
-    <row r="134" ht="15.75" customHeight="1">
+    <row r="134" spans="1:26" ht="15.75" customHeight="1">
       <c r="A134" s="28"/>
       <c r="B134" s="28"/>
       <c r="C134" s="28"/>
@@ -10225,7 +10236,7 @@
       <c r="Y134" s="28"/>
       <c r="Z134" s="28"/>
     </row>
-    <row r="135" ht="15.75" customHeight="1">
+    <row r="135" spans="1:26" ht="15.75" customHeight="1">
       <c r="A135" s="28"/>
       <c r="B135" s="28"/>
       <c r="C135" s="28"/>
@@ -10253,7 +10264,7 @@
       <c r="Y135" s="28"/>
       <c r="Z135" s="28"/>
     </row>
-    <row r="136" ht="15.75" customHeight="1">
+    <row r="136" spans="1:26" ht="15.75" customHeight="1">
       <c r="A136" s="28"/>
       <c r="B136" s="28"/>
       <c r="C136" s="28"/>
@@ -10281,7 +10292,7 @@
       <c r="Y136" s="28"/>
       <c r="Z136" s="28"/>
     </row>
-    <row r="137" ht="15.75" customHeight="1">
+    <row r="137" spans="1:26" ht="15.75" customHeight="1">
       <c r="A137" s="28"/>
       <c r="B137" s="28"/>
       <c r="C137" s="28"/>
@@ -10309,7 +10320,7 @@
       <c r="Y137" s="28"/>
       <c r="Z137" s="28"/>
     </row>
-    <row r="138" ht="15.75" customHeight="1">
+    <row r="138" spans="1:26" ht="15.75" customHeight="1">
       <c r="A138" s="28"/>
       <c r="B138" s="28"/>
       <c r="C138" s="28"/>
@@ -10337,7 +10348,7 @@
       <c r="Y138" s="28"/>
       <c r="Z138" s="28"/>
     </row>
-    <row r="139" ht="15.75" customHeight="1">
+    <row r="139" spans="1:26" ht="15.75" customHeight="1">
       <c r="A139" s="28"/>
       <c r="B139" s="28"/>
       <c r="C139" s="28"/>
@@ -10365,7 +10376,7 @@
       <c r="Y139" s="28"/>
       <c r="Z139" s="28"/>
     </row>
-    <row r="140" ht="15.75" customHeight="1">
+    <row r="140" spans="1:26" ht="15.75" customHeight="1">
       <c r="A140" s="28"/>
       <c r="B140" s="28"/>
       <c r="C140" s="28"/>
@@ -10393,7 +10404,7 @@
       <c r="Y140" s="28"/>
       <c r="Z140" s="28"/>
     </row>
-    <row r="141" ht="15.75" customHeight="1">
+    <row r="141" spans="1:26" ht="15.75" customHeight="1">
       <c r="A141" s="28"/>
       <c r="B141" s="28"/>
       <c r="C141" s="28"/>
@@ -10421,7 +10432,7 @@
       <c r="Y141" s="28"/>
       <c r="Z141" s="28"/>
     </row>
-    <row r="142" ht="15.75" customHeight="1">
+    <row r="142" spans="1:26" ht="15.75" customHeight="1">
       <c r="A142" s="28"/>
       <c r="B142" s="28"/>
       <c r="C142" s="28"/>
@@ -10449,7 +10460,7 @@
       <c r="Y142" s="28"/>
       <c r="Z142" s="28"/>
     </row>
-    <row r="143" ht="15.75" customHeight="1">
+    <row r="143" spans="1:26" ht="15.75" customHeight="1">
       <c r="A143" s="28"/>
       <c r="B143" s="28"/>
       <c r="C143" s="28"/>
@@ -10477,7 +10488,7 @@
       <c r="Y143" s="28"/>
       <c r="Z143" s="28"/>
     </row>
-    <row r="144" ht="15.75" customHeight="1">
+    <row r="144" spans="1:26" ht="15.75" customHeight="1">
       <c r="A144" s="28"/>
       <c r="B144" s="28"/>
       <c r="C144" s="28"/>
@@ -10505,7 +10516,7 @@
       <c r="Y144" s="28"/>
       <c r="Z144" s="28"/>
     </row>
-    <row r="145" ht="15.75" customHeight="1">
+    <row r="145" spans="1:26" ht="15.75" customHeight="1">
       <c r="A145" s="28"/>
       <c r="B145" s="28"/>
       <c r="C145" s="28"/>
@@ -10533,7 +10544,7 @@
       <c r="Y145" s="28"/>
       <c r="Z145" s="28"/>
     </row>
-    <row r="146" ht="15.75" customHeight="1">
+    <row r="146" spans="1:26" ht="15.75" customHeight="1">
       <c r="A146" s="28"/>
       <c r="B146" s="28"/>
       <c r="C146" s="28"/>
@@ -10561,7 +10572,7 @@
       <c r="Y146" s="28"/>
       <c r="Z146" s="28"/>
     </row>
-    <row r="147" ht="15.75" customHeight="1">
+    <row r="147" spans="1:26" ht="15.75" customHeight="1">
       <c r="A147" s="28"/>
       <c r="B147" s="28"/>
       <c r="C147" s="28"/>
@@ -10589,7 +10600,7 @@
       <c r="Y147" s="28"/>
       <c r="Z147" s="28"/>
     </row>
-    <row r="148" ht="15.75" customHeight="1">
+    <row r="148" spans="1:26" ht="15.75" customHeight="1">
       <c r="A148" s="28"/>
       <c r="B148" s="28"/>
       <c r="C148" s="28"/>
@@ -10617,7 +10628,7 @@
       <c r="Y148" s="28"/>
       <c r="Z148" s="28"/>
     </row>
-    <row r="149" ht="15.75" customHeight="1">
+    <row r="149" spans="1:26" ht="15.75" customHeight="1">
       <c r="A149" s="28"/>
       <c r="B149" s="28"/>
       <c r="C149" s="28"/>
@@ -10645,7 +10656,7 @@
       <c r="Y149" s="28"/>
       <c r="Z149" s="28"/>
     </row>
-    <row r="150" ht="15.75" customHeight="1">
+    <row r="150" spans="1:26" ht="15.75" customHeight="1">
       <c r="A150" s="28"/>
       <c r="B150" s="28"/>
       <c r="C150" s="28"/>
@@ -10673,7 +10684,7 @@
       <c r="Y150" s="28"/>
       <c r="Z150" s="28"/>
     </row>
-    <row r="151" ht="15.75" customHeight="1">
+    <row r="151" spans="1:26" ht="15.75" customHeight="1">
       <c r="A151" s="28"/>
       <c r="B151" s="28"/>
       <c r="C151" s="28"/>
@@ -10701,7 +10712,7 @@
       <c r="Y151" s="28"/>
       <c r="Z151" s="28"/>
     </row>
-    <row r="152" ht="15.75" customHeight="1">
+    <row r="152" spans="1:26" ht="15.75" customHeight="1">
       <c r="A152" s="28"/>
       <c r="B152" s="28"/>
       <c r="C152" s="28"/>
@@ -10729,7 +10740,7 @@
       <c r="Y152" s="28"/>
       <c r="Z152" s="28"/>
     </row>
-    <row r="153" ht="15.75" customHeight="1">
+    <row r="153" spans="1:26" ht="15.75" customHeight="1">
       <c r="A153" s="28"/>
       <c r="B153" s="28"/>
       <c r="C153" s="28"/>
@@ -10757,7 +10768,7 @@
       <c r="Y153" s="28"/>
       <c r="Z153" s="28"/>
     </row>
-    <row r="154" ht="15.75" customHeight="1">
+    <row r="154" spans="1:26" ht="15.75" customHeight="1">
       <c r="A154" s="28"/>
       <c r="B154" s="28"/>
       <c r="C154" s="28"/>
@@ -10785,7 +10796,7 @@
       <c r="Y154" s="28"/>
       <c r="Z154" s="28"/>
     </row>
-    <row r="155" ht="15.75" customHeight="1">
+    <row r="155" spans="1:26" ht="15.75" customHeight="1">
       <c r="A155" s="28"/>
       <c r="B155" s="28"/>
       <c r="C155" s="28"/>
@@ -10813,7 +10824,7 @@
       <c r="Y155" s="28"/>
       <c r="Z155" s="28"/>
     </row>
-    <row r="156" ht="15.75" customHeight="1">
+    <row r="156" spans="1:26" ht="15.75" customHeight="1">
       <c r="A156" s="28"/>
       <c r="B156" s="28"/>
       <c r="C156" s="28"/>
@@ -10841,7 +10852,7 @@
       <c r="Y156" s="28"/>
       <c r="Z156" s="28"/>
     </row>
-    <row r="157" ht="15.75" customHeight="1">
+    <row r="157" spans="1:26" ht="15.75" customHeight="1">
       <c r="A157" s="28"/>
       <c r="B157" s="28"/>
       <c r="C157" s="28"/>
@@ -10869,7 +10880,7 @@
       <c r="Y157" s="28"/>
       <c r="Z157" s="28"/>
     </row>
-    <row r="158" ht="15.75" customHeight="1">
+    <row r="158" spans="1:26" ht="15.75" customHeight="1">
       <c r="A158" s="28"/>
       <c r="B158" s="28"/>
       <c r="C158" s="28"/>
@@ -10897,7 +10908,7 @@
       <c r="Y158" s="28"/>
       <c r="Z158" s="28"/>
     </row>
-    <row r="159" ht="15.75" customHeight="1">
+    <row r="159" spans="1:26" ht="15.75" customHeight="1">
       <c r="A159" s="28"/>
       <c r="B159" s="28"/>
       <c r="C159" s="28"/>
@@ -10925,7 +10936,7 @@
       <c r="Y159" s="28"/>
       <c r="Z159" s="28"/>
     </row>
-    <row r="160" ht="15.75" customHeight="1">
+    <row r="160" spans="1:26" ht="15.75" customHeight="1">
       <c r="A160" s="28"/>
       <c r="B160" s="28"/>
       <c r="C160" s="28"/>
@@ -10953,7 +10964,7 @@
       <c r="Y160" s="28"/>
       <c r="Z160" s="28"/>
     </row>
-    <row r="161" ht="15.75" customHeight="1">
+    <row r="161" spans="1:26" ht="15.75" customHeight="1">
       <c r="A161" s="28"/>
       <c r="B161" s="28"/>
       <c r="C161" s="28"/>
@@ -10981,7 +10992,7 @@
       <c r="Y161" s="28"/>
       <c r="Z161" s="28"/>
     </row>
-    <row r="162" ht="15.75" customHeight="1">
+    <row r="162" spans="1:26" ht="15.75" customHeight="1">
       <c r="A162" s="28"/>
       <c r="B162" s="28"/>
       <c r="C162" s="28"/>
@@ -11009,7 +11020,7 @@
       <c r="Y162" s="28"/>
       <c r="Z162" s="28"/>
     </row>
-    <row r="163" ht="15.75" customHeight="1">
+    <row r="163" spans="1:26" ht="15.75" customHeight="1">
       <c r="A163" s="28"/>
       <c r="B163" s="28"/>
       <c r="C163" s="28"/>
@@ -11037,7 +11048,7 @@
       <c r="Y163" s="28"/>
       <c r="Z163" s="28"/>
     </row>
-    <row r="164" ht="15.75" customHeight="1">
+    <row r="164" spans="1:26" ht="15.75" customHeight="1">
       <c r="A164" s="28"/>
       <c r="B164" s="28"/>
       <c r="C164" s="28"/>
@@ -11065,7 +11076,7 @@
       <c r="Y164" s="28"/>
       <c r="Z164" s="28"/>
     </row>
-    <row r="165" ht="15.75" customHeight="1">
+    <row r="165" spans="1:26" ht="15.75" customHeight="1">
       <c r="A165" s="28"/>
       <c r="B165" s="28"/>
       <c r="C165" s="28"/>
@@ -11093,7 +11104,7 @@
       <c r="Y165" s="28"/>
       <c r="Z165" s="28"/>
     </row>
-    <row r="166" ht="15.75" customHeight="1">
+    <row r="166" spans="1:26" ht="15.75" customHeight="1">
       <c r="A166" s="28"/>
       <c r="B166" s="28"/>
       <c r="C166" s="28"/>
@@ -11121,7 +11132,7 @@
       <c r="Y166" s="28"/>
       <c r="Z166" s="28"/>
     </row>
-    <row r="167" ht="15.75" customHeight="1">
+    <row r="167" spans="1:26" ht="15.75" customHeight="1">
       <c r="A167" s="28"/>
       <c r="B167" s="28"/>
       <c r="C167" s="28"/>
@@ -11149,7 +11160,7 @@
       <c r="Y167" s="28"/>
       <c r="Z167" s="28"/>
     </row>
-    <row r="168" ht="15.75" customHeight="1">
+    <row r="168" spans="1:26" ht="15.75" customHeight="1">
       <c r="A168" s="28"/>
       <c r="B168" s="28"/>
       <c r="C168" s="28"/>
@@ -11177,7 +11188,7 @@
       <c r="Y168" s="28"/>
       <c r="Z168" s="28"/>
     </row>
-    <row r="169" ht="15.75" customHeight="1">
+    <row r="169" spans="1:26" ht="15.75" customHeight="1">
       <c r="A169" s="28"/>
       <c r="B169" s="28"/>
       <c r="C169" s="28"/>
@@ -11205,7 +11216,7 @@
       <c r="Y169" s="28"/>
       <c r="Z169" s="28"/>
     </row>
-    <row r="170" ht="15.75" customHeight="1">
+    <row r="170" spans="1:26" ht="15.75" customHeight="1">
       <c r="A170" s="28"/>
       <c r="B170" s="28"/>
       <c r="C170" s="28"/>
@@ -11233,7 +11244,7 @@
       <c r="Y170" s="28"/>
       <c r="Z170" s="28"/>
     </row>
-    <row r="171" ht="15.75" customHeight="1">
+    <row r="171" spans="1:26" ht="15.75" customHeight="1">
       <c r="A171" s="28"/>
       <c r="B171" s="28"/>
       <c r="C171" s="28"/>
@@ -11261,7 +11272,7 @@
       <c r="Y171" s="28"/>
       <c r="Z171" s="28"/>
     </row>
-    <row r="172" ht="15.75" customHeight="1">
+    <row r="172" spans="1:26" ht="15.75" customHeight="1">
       <c r="A172" s="28"/>
       <c r="B172" s="28"/>
       <c r="C172" s="28"/>
@@ -11289,7 +11300,7 @@
       <c r="Y172" s="28"/>
       <c r="Z172" s="28"/>
     </row>
-    <row r="173" ht="15.75" customHeight="1">
+    <row r="173" spans="1:26" ht="15.75" customHeight="1">
       <c r="A173" s="28"/>
       <c r="B173" s="28"/>
       <c r="C173" s="28"/>
@@ -11317,7 +11328,7 @@
       <c r="Y173" s="28"/>
       <c r="Z173" s="28"/>
     </row>
-    <row r="174" ht="15.75" customHeight="1">
+    <row r="174" spans="1:26" ht="15.75" customHeight="1">
       <c r="A174" s="28"/>
       <c r="B174" s="28"/>
       <c r="C174" s="28"/>
@@ -11345,7 +11356,7 @@
       <c r="Y174" s="28"/>
       <c r="Z174" s="28"/>
     </row>
-    <row r="175" ht="15.75" customHeight="1">
+    <row r="175" spans="1:26" ht="15.75" customHeight="1">
       <c r="A175" s="28"/>
       <c r="B175" s="28"/>
       <c r="C175" s="28"/>
@@ -11373,7 +11384,7 @@
       <c r="Y175" s="28"/>
       <c r="Z175" s="28"/>
     </row>
-    <row r="176" ht="15.75" customHeight="1">
+    <row r="176" spans="1:26" ht="15.75" customHeight="1">
       <c r="A176" s="28"/>
       <c r="B176" s="28"/>
       <c r="C176" s="28"/>
@@ -11401,7 +11412,7 @@
       <c r="Y176" s="28"/>
       <c r="Z176" s="28"/>
     </row>
-    <row r="177" ht="15.75" customHeight="1">
+    <row r="177" spans="1:26" ht="15.75" customHeight="1">
       <c r="A177" s="28"/>
       <c r="B177" s="28"/>
       <c r="C177" s="28"/>
@@ -11429,7 +11440,7 @@
       <c r="Y177" s="28"/>
       <c r="Z177" s="28"/>
     </row>
-    <row r="178" ht="15.75" customHeight="1">
+    <row r="178" spans="1:26" ht="15.75" customHeight="1">
       <c r="A178" s="28"/>
       <c r="B178" s="28"/>
       <c r="C178" s="28"/>
@@ -11457,7 +11468,7 @@
       <c r="Y178" s="28"/>
       <c r="Z178" s="28"/>
     </row>
-    <row r="179" ht="15.75" customHeight="1">
+    <row r="179" spans="1:26" ht="15.75" customHeight="1">
       <c r="A179" s="28"/>
       <c r="B179" s="28"/>
       <c r="C179" s="28"/>
@@ -11485,7 +11496,7 @@
       <c r="Y179" s="28"/>
       <c r="Z179" s="28"/>
     </row>
-    <row r="180" ht="15.75" customHeight="1">
+    <row r="180" spans="1:26" ht="15.75" customHeight="1">
       <c r="A180" s="28"/>
       <c r="B180" s="28"/>
       <c r="C180" s="28"/>
@@ -11513,7 +11524,7 @@
       <c r="Y180" s="28"/>
       <c r="Z180" s="28"/>
     </row>
-    <row r="181" ht="15.75" customHeight="1">
+    <row r="181" spans="1:26" ht="15.75" customHeight="1">
       <c r="A181" s="28"/>
       <c r="B181" s="28"/>
       <c r="C181" s="28"/>
@@ -11541,7 +11552,7 @@
       <c r="Y181" s="28"/>
       <c r="Z181" s="28"/>
     </row>
-    <row r="182" ht="15.75" customHeight="1">
+    <row r="182" spans="1:26" ht="15.75" customHeight="1">
       <c r="A182" s="28"/>
       <c r="B182" s="28"/>
       <c r="C182" s="28"/>
@@ -11569,7 +11580,7 @@
       <c r="Y182" s="28"/>
       <c r="Z182" s="28"/>
     </row>
-    <row r="183" ht="15.75" customHeight="1">
+    <row r="183" spans="1:26" ht="15.75" customHeight="1">
       <c r="A183" s="28"/>
       <c r="B183" s="28"/>
       <c r="C183" s="28"/>
@@ -11597,7 +11608,7 @@
       <c r="Y183" s="28"/>
       <c r="Z183" s="28"/>
     </row>
-    <row r="184" ht="15.75" customHeight="1">
+    <row r="184" spans="1:26" ht="15.75" customHeight="1">
       <c r="A184" s="28"/>
       <c r="B184" s="28"/>
       <c r="C184" s="28"/>
@@ -11625,7 +11636,7 @@
       <c r="Y184" s="28"/>
       <c r="Z184" s="28"/>
     </row>
-    <row r="185" ht="15.75" customHeight="1">
+    <row r="185" spans="1:26" ht="15.75" customHeight="1">
       <c r="A185" s="28"/>
       <c r="B185" s="28"/>
       <c r="C185" s="28"/>
@@ -11653,7 +11664,7 @@
       <c r="Y185" s="28"/>
       <c r="Z185" s="28"/>
     </row>
-    <row r="186" ht="15.75" customHeight="1">
+    <row r="186" spans="1:26" ht="15.75" customHeight="1">
       <c r="A186" s="28"/>
       <c r="B186" s="28"/>
       <c r="C186" s="28"/>
@@ -11681,7 +11692,7 @@
       <c r="Y186" s="28"/>
       <c r="Z186" s="28"/>
     </row>
-    <row r="187" ht="15.75" customHeight="1">
+    <row r="187" spans="1:26" ht="15.75" customHeight="1">
       <c r="A187" s="28"/>
       <c r="B187" s="28"/>
       <c r="C187" s="28"/>
@@ -11709,7 +11720,7 @@
       <c r="Y187" s="28"/>
       <c r="Z187" s="28"/>
     </row>
-    <row r="188" ht="15.75" customHeight="1">
+    <row r="188" spans="1:26" ht="15.75" customHeight="1">
       <c r="A188" s="28"/>
       <c r="B188" s="28"/>
       <c r="C188" s="28"/>
@@ -11737,7 +11748,7 @@
       <c r="Y188" s="28"/>
       <c r="Z188" s="28"/>
     </row>
-    <row r="189" ht="15.75" customHeight="1">
+    <row r="189" spans="1:26" ht="15.75" customHeight="1">
       <c r="A189" s="28"/>
       <c r="B189" s="28"/>
       <c r="C189" s="28"/>
@@ -11765,7 +11776,7 @@
       <c r="Y189" s="28"/>
       <c r="Z189" s="28"/>
     </row>
-    <row r="190" ht="15.75" customHeight="1">
+    <row r="190" spans="1:26" ht="15.75" customHeight="1">
       <c r="A190" s="28"/>
       <c r="B190" s="28"/>
       <c r="C190" s="28"/>
@@ -11793,7 +11804,7 @@
       <c r="Y190" s="28"/>
       <c r="Z190" s="28"/>
     </row>
-    <row r="191" ht="15.75" customHeight="1">
+    <row r="191" spans="1:26" ht="15.75" customHeight="1">
       <c r="A191" s="28"/>
       <c r="B191" s="28"/>
       <c r="C191" s="28"/>
@@ -11821,7 +11832,7 @@
       <c r="Y191" s="28"/>
       <c r="Z191" s="28"/>
     </row>
-    <row r="192" ht="15.75" customHeight="1">
+    <row r="192" spans="1:26" ht="15.75" customHeight="1">
       <c r="A192" s="28"/>
       <c r="B192" s="28"/>
       <c r="C192" s="28"/>
@@ -11849,7 +11860,7 @@
       <c r="Y192" s="28"/>
       <c r="Z192" s="28"/>
     </row>
-    <row r="193" ht="15.75" customHeight="1">
+    <row r="193" spans="1:26" ht="15.75" customHeight="1">
       <c r="A193" s="28"/>
       <c r="B193" s="28"/>
       <c r="C193" s="28"/>
@@ -11877,7 +11888,7 @@
       <c r="Y193" s="28"/>
       <c r="Z193" s="28"/>
     </row>
-    <row r="194" ht="15.75" customHeight="1">
+    <row r="194" spans="1:26" ht="15.75" customHeight="1">
       <c r="A194" s="28"/>
       <c r="B194" s="28"/>
       <c r="C194" s="28"/>
@@ -11905,7 +11916,7 @@
       <c r="Y194" s="28"/>
       <c r="Z194" s="28"/>
     </row>
-    <row r="195" ht="15.75" customHeight="1">
+    <row r="195" spans="1:26" ht="15.75" customHeight="1">
       <c r="A195" s="28"/>
       <c r="B195" s="28"/>
       <c r="C195" s="28"/>
@@ -11933,7 +11944,7 @@
       <c r="Y195" s="28"/>
       <c r="Z195" s="28"/>
     </row>
-    <row r="196" ht="15.75" customHeight="1">
+    <row r="196" spans="1:26" ht="15.75" customHeight="1">
       <c r="A196" s="28"/>
       <c r="B196" s="28"/>
       <c r="C196" s="28"/>
@@ -11961,7 +11972,7 @@
       <c r="Y196" s="28"/>
       <c r="Z196" s="28"/>
     </row>
-    <row r="197" ht="15.75" customHeight="1">
+    <row r="197" spans="1:26" ht="15.75" customHeight="1">
       <c r="A197" s="28"/>
       <c r="B197" s="28"/>
       <c r="C197" s="28"/>
@@ -11989,7 +12000,7 @@
       <c r="Y197" s="28"/>
       <c r="Z197" s="28"/>
     </row>
-    <row r="198" ht="15.75" customHeight="1">
+    <row r="198" spans="1:26" ht="15.75" customHeight="1">
       <c r="A198" s="28"/>
       <c r="B198" s="28"/>
       <c r="C198" s="28"/>
@@ -12017,7 +12028,7 @@
       <c r="Y198" s="28"/>
       <c r="Z198" s="28"/>
     </row>
-    <row r="199" ht="15.75" customHeight="1">
+    <row r="199" spans="1:26" ht="15.75" customHeight="1">
       <c r="A199" s="28"/>
       <c r="B199" s="28"/>
       <c r="C199" s="28"/>
@@ -12045,7 +12056,7 @@
       <c r="Y199" s="28"/>
       <c r="Z199" s="28"/>
     </row>
-    <row r="200" ht="15.75" customHeight="1">
+    <row r="200" spans="1:26" ht="15.75" customHeight="1">
       <c r="A200" s="28"/>
       <c r="B200" s="28"/>
       <c r="C200" s="28"/>
@@ -12073,7 +12084,7 @@
       <c r="Y200" s="28"/>
       <c r="Z200" s="28"/>
     </row>
-    <row r="201" ht="15.75" customHeight="1">
+    <row r="201" spans="1:26" ht="15.75" customHeight="1">
       <c r="A201" s="28"/>
       <c r="B201" s="28"/>
       <c r="C201" s="28"/>
@@ -12101,7 +12112,7 @@
       <c r="Y201" s="28"/>
       <c r="Z201" s="28"/>
     </row>
-    <row r="202" ht="15.75" customHeight="1">
+    <row r="202" spans="1:26" ht="15.75" customHeight="1">
       <c r="A202" s="28"/>
       <c r="B202" s="28"/>
       <c r="C202" s="28"/>
@@ -12129,7 +12140,7 @@
       <c r="Y202" s="28"/>
       <c r="Z202" s="28"/>
     </row>
-    <row r="203" ht="15.75" customHeight="1">
+    <row r="203" spans="1:26" ht="15.75" customHeight="1">
       <c r="A203" s="28"/>
       <c r="B203" s="28"/>
       <c r="C203" s="28"/>
@@ -12157,7 +12168,7 @@
       <c r="Y203" s="28"/>
       <c r="Z203" s="28"/>
     </row>
-    <row r="204" ht="15.75" customHeight="1">
+    <row r="204" spans="1:26" ht="15.75" customHeight="1">
       <c r="A204" s="28"/>
       <c r="B204" s="28"/>
       <c r="C204" s="28"/>
@@ -12185,7 +12196,7 @@
       <c r="Y204" s="28"/>
       <c r="Z204" s="28"/>
     </row>
-    <row r="205" ht="15.75" customHeight="1">
+    <row r="205" spans="1:26" ht="15.75" customHeight="1">
       <c r="A205" s="28"/>
       <c r="B205" s="28"/>
       <c r="C205" s="28"/>
@@ -12213,7 +12224,7 @@
       <c r="Y205" s="28"/>
       <c r="Z205" s="28"/>
     </row>
-    <row r="206" ht="15.75" customHeight="1">
+    <row r="206" spans="1:26" ht="15.75" customHeight="1">
       <c r="A206" s="28"/>
       <c r="B206" s="28"/>
       <c r="C206" s="28"/>
@@ -12241,7 +12252,7 @@
       <c r="Y206" s="28"/>
       <c r="Z206" s="28"/>
     </row>
-    <row r="207" ht="15.75" customHeight="1">
+    <row r="207" spans="1:26" ht="15.75" customHeight="1">
       <c r="A207" s="28"/>
       <c r="B207" s="28"/>
       <c r="C207" s="28"/>
@@ -12269,7 +12280,7 @@
       <c r="Y207" s="28"/>
       <c r="Z207" s="28"/>
     </row>
-    <row r="208" ht="15.75" customHeight="1">
+    <row r="208" spans="1:26" ht="15.75" customHeight="1">
       <c r="A208" s="28"/>
       <c r="B208" s="28"/>
       <c r="C208" s="28"/>
@@ -12297,7 +12308,7 @@
       <c r="Y208" s="28"/>
       <c r="Z208" s="28"/>
     </row>
-    <row r="209" ht="15.75" customHeight="1">
+    <row r="209" spans="1:26" ht="15.75" customHeight="1">
       <c r="A209" s="28"/>
       <c r="B209" s="28"/>
       <c r="C209" s="28"/>
@@ -12325,7 +12336,7 @@
       <c r="Y209" s="28"/>
       <c r="Z209" s="28"/>
     </row>
-    <row r="210" ht="15.75" customHeight="1">
+    <row r="210" spans="1:26" ht="15.75" customHeight="1">
       <c r="A210" s="28"/>
       <c r="B210" s="28"/>
       <c r="C210" s="28"/>
@@ -12353,7 +12364,7 @@
       <c r="Y210" s="28"/>
       <c r="Z210" s="28"/>
     </row>
-    <row r="211" ht="15.75" customHeight="1">
+    <row r="211" spans="1:26" ht="15.75" customHeight="1">
       <c r="A211" s="28"/>
       <c r="B211" s="28"/>
       <c r="C211" s="28"/>
@@ -12381,7 +12392,7 @@
       <c r="Y211" s="28"/>
       <c r="Z211" s="28"/>
     </row>
-    <row r="212" ht="15.75" customHeight="1">
+    <row r="212" spans="1:26" ht="15.75" customHeight="1">
       <c r="A212" s="28"/>
       <c r="B212" s="28"/>
       <c r="C212" s="28"/>
@@ -12409,7 +12420,7 @@
       <c r="Y212" s="28"/>
       <c r="Z212" s="28"/>
     </row>
-    <row r="213" ht="15.75" customHeight="1">
+    <row r="213" spans="1:26" ht="15.75" customHeight="1">
       <c r="A213" s="28"/>
       <c r="B213" s="28"/>
       <c r="C213" s="28"/>
@@ -12437,7 +12448,7 @@
       <c r="Y213" s="28"/>
       <c r="Z213" s="28"/>
     </row>
-    <row r="214" ht="15.75" customHeight="1">
+    <row r="214" spans="1:26" ht="15.75" customHeight="1">
       <c r="A214" s="28"/>
       <c r="B214" s="28"/>
       <c r="C214" s="28"/>
@@ -12465,7 +12476,7 @@
       <c r="Y214" s="28"/>
       <c r="Z214" s="28"/>
     </row>
-    <row r="215" ht="15.75" customHeight="1">
+    <row r="215" spans="1:26" ht="15.75" customHeight="1">
       <c r="A215" s="28"/>
       <c r="B215" s="28"/>
       <c r="C215" s="28"/>
@@ -12493,7 +12504,7 @@
       <c r="Y215" s="28"/>
       <c r="Z215" s="28"/>
     </row>
-    <row r="216" ht="15.75" customHeight="1">
+    <row r="216" spans="1:26" ht="15.75" customHeight="1">
       <c r="A216" s="28"/>
       <c r="B216" s="28"/>
       <c r="C216" s="28"/>
@@ -12521,7 +12532,7 @@
       <c r="Y216" s="28"/>
       <c r="Z216" s="28"/>
     </row>
-    <row r="217" ht="15.75" customHeight="1">
+    <row r="217" spans="1:26" ht="15.75" customHeight="1">
       <c r="A217" s="28"/>
       <c r="B217" s="28"/>
       <c r="C217" s="28"/>
@@ -12549,7 +12560,7 @@
       <c r="Y217" s="28"/>
       <c r="Z217" s="28"/>
     </row>
-    <row r="218" ht="15.75" customHeight="1">
+    <row r="218" spans="1:26" ht="15.75" customHeight="1">
       <c r="A218" s="28"/>
       <c r="B218" s="28"/>
       <c r="C218" s="28"/>
@@ -12577,7 +12588,7 @@
       <c r="Y218" s="28"/>
       <c r="Z218" s="28"/>
     </row>
-    <row r="219" ht="15.75" customHeight="1">
+    <row r="219" spans="1:26" ht="15.75" customHeight="1">
       <c r="A219" s="28"/>
       <c r="B219" s="28"/>
       <c r="C219" s="28"/>
@@ -12605,7 +12616,7 @@
       <c r="Y219" s="28"/>
       <c r="Z219" s="28"/>
     </row>
-    <row r="220" ht="15.75" customHeight="1">
+    <row r="220" spans="1:26" ht="15.75" customHeight="1">
       <c r="A220" s="28"/>
       <c r="B220" s="28"/>
       <c r="C220" s="28"/>
@@ -12633,10 +12644,10 @@
       <c r="Y220" s="28"/>
       <c r="Z220" s="28"/>
     </row>
-    <row r="221" ht="15.75" customHeight="1"/>
-    <row r="222" ht="15.75" customHeight="1"/>
-    <row r="223" ht="15.75" customHeight="1"/>
-    <row r="224" ht="15.75" customHeight="1"/>
+    <row r="221" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="222" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="223" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="224" spans="1:26" ht="15.75" customHeight="1"/>
     <row r="225" ht="15.75" customHeight="1"/>
     <row r="226" ht="15.75" customHeight="1"/>
     <row r="227" ht="15.75" customHeight="1"/>
@@ -13414,9 +13425,7 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>